<commit_message>
Added setup data for lab products
</commit_message>
<xml_diff>
--- a/bika/lims/setupdata/test/test.xlsx
+++ b/bika/lims/setupdata/test/test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="46" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="934" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="47" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="934" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" state="visible" r:id="rId2"/>
@@ -55,6 +55,7 @@
     <sheet name="Setup" sheetId="45" state="visible" r:id="rId46"/>
     <sheet name="Constants" sheetId="46" state="visible" r:id="rId47"/>
     <sheet name="Invoice Batches" sheetId="47" state="visible" r:id="rId48"/>
+    <sheet name="Lab Products" sheetId="48" state="visible" r:id="rId49"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
@@ -196,7 +197,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2954" uniqueCount="1284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2973" uniqueCount="1296">
   <si>
     <t>Instructions</t>
   </si>
@@ -4048,6 +4049,42 @@
   </si>
   <si>
     <t>September 2012</t>
+  </si>
+  <si>
+    <t>volume</t>
+  </si>
+  <si>
+    <t>vat</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>Lab Products</t>
+  </si>
+  <si>
+    <t>Appelsuur</t>
+  </si>
+  <si>
+    <t>Byvoegings by Wyn</t>
+  </si>
+  <si>
+    <t>kg</t>
+  </si>
+  <si>
+    <t>Asetaldehied</t>
+  </si>
+  <si>
+    <t>Balling standaard</t>
+  </si>
+  <si>
+    <t>18deg</t>
+  </si>
+  <si>
+    <t>Ballingmeter</t>
+  </si>
+  <si>
+    <t>-5 - +5deg</t>
   </si>
 </sst>
 </file>
@@ -4338,7 +4375,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="152">
+  <cellXfs count="153">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
@@ -4757,6 +4794,9 @@
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
     </xf>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="17" numFmtId="168" xfId="0"/>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="23" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
@@ -4841,9 +4881,9 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="93.2627450980392"/>
-    <col collapsed="false" hidden="false" max="1023" min="2" style="1" width="118.98431372549"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="8.54117647058824"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="93.6509803921569"/>
+    <col collapsed="false" hidden="false" max="1023" min="2" style="1" width="119.474509803922"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="8.57647058823529"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="32.05" outlineLevel="0" r="1" s="4">
@@ -4911,13 +4951,13 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="19.5960784313726"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="22.1647058823529"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="6.49019607843137"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="7" width="15.8627450980392"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="7" width="8.82745098039216"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="7" width="10.678431372549"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="7" width="5.78039215686275"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="19.678431372549"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="22.2588235294118"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="6.51764705882353"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="7" width="15.9254901960784"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="7" width="8.86274509803922"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="7" width="10.7294117647059"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="7" width="5.8078431372549"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="12.2" outlineLevel="0" r="1" s="6">
@@ -5101,9 +5141,9 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="11.8470588235294"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="18.9450980392157"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="7" width="5.78039215686275"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="11.8980392156863"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="19.0235294117647"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="7" width="5.8078431372549"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="12.2" outlineLevel="0" r="1" s="6">
@@ -5210,16 +5250,16 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="27" width="12.8941176470588"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="27" width="25.1254901960784"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="27" width="6.49019607843137"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="27" width="4.50196078431373"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="27" width="8.40392156862745"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="27" width="6.5843137254902"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="27" width="7.27058823529412"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="27" width="13.7764705882353"/>
-    <col collapsed="false" hidden="false" max="1023" min="9" style="27" width="6.5843137254902"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="7" width="5.62352941176471"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="27" width="12.9490196078431"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="27" width="25.2274509803922"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="27" width="6.51764705882353"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="27" width="4.51764705882353"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="27" width="8.43921568627451"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="27" width="6.61176470588235"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="27" width="7.29803921568627"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="27" width="13.8313725490196"/>
+    <col collapsed="false" hidden="false" max="1023" min="9" style="27" width="6.61176470588235"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="7" width="5.64313725490196"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="13.2" outlineLevel="0" r="1" s="16">
@@ -5646,14 +5686,14 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="7" width="12.5137254901961"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="24.1725490196078"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="7" width="16.1137254901961"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="7" width="17.0745098039216"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="7" width="7.3921568627451"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="7" width="9.83921568627451"/>
-    <col collapsed="false" hidden="false" max="1018" min="9" style="7" width="5.78039215686275"/>
-    <col collapsed="false" hidden="false" max="1025" min="1019" style="7" width="5.50588235294118"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="7" width="12.5647058823529"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="24.2745098039216"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="7" width="16.1764705882353"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="7" width="17.1450980392157"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="7" width="7.42352941176471"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="7" width="9.88235294117647"/>
+    <col collapsed="false" hidden="false" max="1018" min="9" style="7" width="5.8078431372549"/>
+    <col collapsed="false" hidden="false" max="1025" min="1019" style="7" width="5.52941176470588"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="13.2" outlineLevel="0" r="1" s="6">
@@ -5922,11 +5962,11 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="27" width="18.2627450980392"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="27" width="20.9529411764706"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="15.5019607843137"/>
-    <col collapsed="false" hidden="false" max="1018" min="4" style="27" width="5.78039215686275"/>
-    <col collapsed="false" hidden="false" max="1025" min="1019" style="7" width="4.94901960784314"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="27" width="18.3372549019608"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="27" width="21.0392156862745"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="15.5686274509804"/>
+    <col collapsed="false" hidden="false" max="1018" min="4" style="27" width="5.8078431372549"/>
+    <col collapsed="false" hidden="false" max="1025" min="1019" style="7" width="4.96862745098039"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="12.2" outlineLevel="0" r="1" s="16">
@@ -5994,10 +6034,10 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="27" width="15.0509803921569"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="27" width="54.5333333333333"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="27" width="24.1725490196078"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="27" width="5.78039215686275"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="27" width="15.1176470588235"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="27" width="54.7647058823529"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="27" width="24.2745098039216"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="27" width="5.8078431372549"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="13.2" outlineLevel="0" r="1" s="16">
@@ -6118,9 +6158,9 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="24.1372549019608"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="16.356862745098"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="7" width="5.78039215686275"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="24.2392156862745"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="16.4196078431373"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="7" width="5.8078431372549"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="12.2" outlineLevel="0" r="1" s="6">
@@ -6258,11 +6298,11 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="16.2549019607843"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="7" width="9.34901960784314"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="7" width="14.9529411764706"/>
-    <col collapsed="false" hidden="false" max="21" min="6" style="7" width="9.34901960784314"/>
-    <col collapsed="false" hidden="false" max="1025" min="22" style="7" width="16.2549019607843"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="16.321568627451"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="7" width="9.38823529411765"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="7" width="15.0156862745098"/>
+    <col collapsed="false" hidden="false" max="21" min="6" style="7" width="9.38823529411765"/>
+    <col collapsed="false" hidden="false" max="1025" min="22" style="7" width="16.321568627451"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="13.2" outlineLevel="0" r="1" s="6">
@@ -6488,9 +6528,9 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="22.2509803921569"/>
-    <col collapsed="false" hidden="false" max="21" min="2" style="7" width="7.84313725490196"/>
-    <col collapsed="false" hidden="false" max="1025" min="22" style="7" width="5.78039215686275"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="22.3450980392157"/>
+    <col collapsed="false" hidden="false" max="21" min="2" style="7" width="7.87450980392157"/>
+    <col collapsed="false" hidden="false" max="1025" min="22" style="7" width="5.8078431372549"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="13.2" outlineLevel="0" r="1" s="6">
@@ -6766,10 +6806,10 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.0823529411765"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.7098039215686"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="7.45882352941177"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="7.42352941176471"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.1686274509804"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.8235294117647"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="7.48627450980392"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="7.45882352941177"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="13.4" outlineLevel="0" r="1">
@@ -6887,10 +6927,10 @@
   </sheetViews>
   <cols>
     <col collapsed="false" hidden="true" max="1" min="1" style="6" width="0"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="6" width="15.2666666666667"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="6.14509803921569"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="7" width="4.59607843137255"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="7" width="6.55294117647059"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="6" width="15.3294117647059"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="6.17254901960784"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="7" width="4.61176470588235"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="7" width="6.5843137254902"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="12.2" outlineLevel="0" r="1" s="6">
@@ -7084,18 +7124,18 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="83" width="19.5960784313726"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="83" width="23.1254901960784"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="83" width="16.8313725490196"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="83" width="16.6941176470588"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="83" width="12.3607843137255"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="84" width="22.4078431372549"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="84" width="10.8274509803922"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="84" width="11.1137254901961"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="85" width="12.0980392156863"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="83" width="7.45882352941177"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="83" width="11.043137254902"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="83" width="5.78039215686275"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="83" width="19.678431372549"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="83" width="23.2196078431373"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="83" width="16.9019607843137"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="83" width="16.756862745098"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="83" width="12.4117647058824"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="84" width="22.5019607843137"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="84" width="10.8705882352941"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="84" width="11.156862745098"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="85" width="12.1490196078431"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="83" width="7.48627450980392"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="83" width="11.0941176470588"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="83" width="5.8078431372549"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="15.05" outlineLevel="0" r="1" s="86">
@@ -8322,15 +8362,15 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.9137254901961"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.121568627451"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.4352941176471"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.25098039215686"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.1137254901961"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.878431372549"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.356862745098"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="28.0666666666667"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="7.45882352941177"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.9843137254902"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.1921568627451"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.4823529411765"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.28627450980392"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.1647058823529"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.9529411764706"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.4196078431373"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="28.1803921568627"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="7.48627450980392"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="15.1" outlineLevel="0" r="1" s="86">
@@ -8468,15 +8508,15 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.9137254901961"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.356862745098"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.4352941176471"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.25098039215686"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.1137254901961"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.878431372549"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.356862745098"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="28.0666666666667"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="7.45882352941177"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.9843137254902"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.4"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.4823529411765"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.28627450980392"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.1647058823529"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.9529411764706"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.4196078431373"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="28.1803921568627"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="7.48627450980392"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="15.1" outlineLevel="0" r="1" s="86">
@@ -8607,14 +8647,14 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.6196078431373"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.3607843137255"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.45882352941177"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.68235294117647"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="7.45882352941177"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.1372549019608"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.1254901960784"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="7.45882352941177"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.678431372549"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.4392156862745"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.48627450980392"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.72156862745098"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="7.48627450980392"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.2039215686275"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.2274509803922"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="7.48627450980392"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="14.9" outlineLevel="0" r="1">
@@ -9597,18 +9637,18 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.7686274509804"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.4352941176471"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.7490196078431"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.89019607843137"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.9803921568627"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="7.45882352941177"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.8666666666667"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.9333333333333"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="14.9725490196078"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="5.15686274509804"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="100" width="7.45882352941177"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="7.45882352941177"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.8235294117647"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.5333333333333"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.8196078431373"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.93333333333333"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.0274509803922"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="7.48627450980392"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.9254901960784"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.9921568627451"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.0392156862745"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="5.17647058823529"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="100" width="7.48627450980392"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="7.48627450980392"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="14.9" outlineLevel="0" r="1" s="86">
@@ -9824,17 +9864,17 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.9960784313726"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.1529411764706"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.2470588235294"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.89019607843137"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.9803921568627"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.5137254901961"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.9333333333333"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.1882352941176"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="26.9921568627451"/>
-    <col collapsed="false" hidden="false" max="1023" min="10" style="0" width="7.45882352941177"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="7.42352941176471"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0666666666667"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.2392156862745"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.3254901960784"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.93333333333333"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.0274509803922"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.5725490196078"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.9921568627451"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.2313725490196"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="27.1058823529412"/>
+    <col collapsed="false" hidden="false" max="1023" min="10" style="0" width="7.48627450980392"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="7.45882352941177"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="14.9" outlineLevel="0" r="1" s="86">
@@ -9926,10 +9966,10 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="28.1450980392157"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="31.6862745098039"/>
-    <col collapsed="false" hidden="false" max="5" min="3" style="7" width="20.4509803921569"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="7" width="5.78039215686275"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="28.2588235294118"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="31.8156862745098"/>
+    <col collapsed="false" hidden="false" max="5" min="3" style="7" width="20.5372549019608"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="7" width="5.8078431372549"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="12.2" outlineLevel="0" r="1" s="6">
@@ -10028,10 +10068,10 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="106" width="16.7803921568627"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="106" width="45.443137254902"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="106" width="46"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="106" width="6.15294117647059"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="106" width="16.8509803921569"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="106" width="45.6274509803922"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="106" width="46.1882352941177"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="106" width="6.18039215686275"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="14.15" outlineLevel="0" r="1" s="107">
@@ -10165,10 +10205,10 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="7" width="24.2235294117647"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="7" width="6.97647058823529"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="7" width="3.22745098039216"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="7" width="5.78039215686275"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="7" width="24.3254901960784"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="7" width="7.0078431372549"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="7" width="3.24313725490196"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="7" width="5.8078431372549"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="12.2" outlineLevel="0" r="1" s="6">
@@ -10742,28 +10782,28 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="27" width="20.2705882352941"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="27" width="28.3254901960784"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="27" width="8.06666666666667"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="27" width="5.09803921568627"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="27" width="17.0745098039216"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="27" width="9.98039215686275"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="114" width="9.8078431372549"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="27" width="7.15686274509804"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="16" width="5.90980392156863"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="27" width="7.4156862745098"/>
-    <col collapsed="false" hidden="false" max="13" min="11" style="27" width="3.54901960784314"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="27" width="3.82352941176471"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="27" width="6.21176470588235"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="27" width="3.22745098039216"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="27" width="13.0862745098039"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="27" width="9.38039215686275"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="27" width="12.9921568627451"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="114" width="11.1019607843137"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="27" width="8.92156862745098"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="27" width="8.09411764705882"/>
-    <col collapsed="false" hidden="false" max="24" min="23" style="27" width="10.3764705882353"/>
-    <col collapsed="false" hidden="false" max="1025" min="25" style="27" width="7.42352941176471"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="27" width="20.356862745098"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="27" width="28.4392156862745"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="27" width="8.09411764705882"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="27" width="5.12156862745098"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="27" width="17.1450980392157"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="27" width="10.0196078431373"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="114" width="9.85098039215686"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="27" width="7.1843137254902"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="16" width="5.93725490196078"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="27" width="7.45098039215686"/>
+    <col collapsed="false" hidden="false" max="13" min="11" style="27" width="3.56470588235294"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="27" width="3.83529411764706"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="27" width="6.23921568627451"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="27" width="3.24313725490196"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="27" width="13.1372549019608"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="27" width="9.42352941176471"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="27" width="13.043137254902"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="114" width="11.1490196078431"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="27" width="8.96470588235294"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="27" width="8.12549019607843"/>
+    <col collapsed="false" hidden="false" max="24" min="23" style="27" width="10.4196078431373"/>
+    <col collapsed="false" hidden="false" max="1025" min="25" style="27" width="7.45882352941177"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="34.9" outlineLevel="0" r="1" s="16">
@@ -12522,9 +12562,9 @@
   </sheetViews>
   <cols>
     <col collapsed="false" hidden="true" max="1" min="1" style="6" width="0"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="6" width="32.0549019607843"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="17.0313725490196"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="7" width="6.5843137254902"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="6" width="32.1882352941176"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="17.1019607843137"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="7" width="6.61176470588235"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="12.2" outlineLevel="0" r="1" s="6">
@@ -12923,12 +12963,12 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="27.2980392156863"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="8.57647058823529"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="8.36862745098039"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="7" width="13.8627450980392"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="7" width="3.22745098039216"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="7" width="5.78039215686275"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="27.4156862745098"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="8.61176470588235"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="8.40392156862745"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="7" width="13.9176470588235"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="7" width="3.24313725490196"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="7" width="5.8078431372549"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="12.2" outlineLevel="0" r="1" s="6">
@@ -12994,12 +13034,12 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="27" width="10.2274509803922"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="27" width="11.2745098039216"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="125" width="8.25490196078431"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="27" width="13.8666666666667"/>
-    <col collapsed="false" hidden="false" max="973" min="5" style="27" width="5.78039215686275"/>
-    <col collapsed="false" hidden="false" max="1025" min="974" style="7" width="4.94901960784314"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="27" width="10.2705882352941"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="27" width="11.321568627451"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="125" width="8.29019607843137"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="27" width="13.9254901960784"/>
+    <col collapsed="false" hidden="false" max="973" min="5" style="27" width="5.8078431372549"/>
+    <col collapsed="false" hidden="false" max="1025" min="974" style="7" width="4.96862745098039"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="24.5" outlineLevel="0" r="1" s="16">
@@ -13202,12 +13242,12 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="27" width="35"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="27" width="9.13725490196078"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="27" width="9.45098039215686"/>
-    <col collapsed="false" hidden="false" max="997" min="5" style="27" width="5.78039215686275"/>
-    <col collapsed="false" hidden="false" max="1023" min="998" style="7" width="4.94901960784314"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="4.94901960784314"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="27" width="35.1450980392157"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="27" width="9.18039215686274"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="27" width="9.48627450980392"/>
+    <col collapsed="false" hidden="false" max="997" min="5" style="27" width="5.8078431372549"/>
+    <col collapsed="false" hidden="false" max="1023" min="998" style="7" width="4.96862745098039"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="4.96862745098039"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="24.5" outlineLevel="0" r="1" s="16">
@@ -14679,13 +14719,13 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="40" width="16.4588235294118"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="40" width="14.1921568627451"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="40" width="26.3450980392157"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="40" width="11.6078431372549"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="40" width="10.3176470588235"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="40" width="5.32156862745098"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="40" width="5.78039215686275"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="40" width="16.5294117647059"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="40" width="14.2470588235294"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="40" width="26.4549019607843"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="40" width="11.6509803921569"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="40" width="10.3607843137255"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="40" width="5.34117647058824"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="40" width="5.8078431372549"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="14.15" outlineLevel="0" r="1" s="43">
@@ -14814,10 +14854,10 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="40" width="21.6549019607843"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="40" width="26.8627450980392"/>
-    <col collapsed="false" hidden="false" max="6" min="3" style="40" width="28.4196078431373"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="40" width="5.78039215686275"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="40" width="21.7490196078431"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="40" width="26.9764705882353"/>
+    <col collapsed="false" hidden="false" max="6" min="3" style="40" width="28.5411764705882"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="40" width="5.8078431372549"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.2" outlineLevel="0" r="1" s="43">
@@ -15006,11 +15046,11 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="5.37254901960784"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="10.9725490196078"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="19.4627450980392"/>
-    <col collapsed="false" hidden="false" max="6" min="4" style="7" width="9.78823529411765"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="7" width="5.78039215686275"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="5.3921568627451"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="11.0156862745098"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="19.5411764705882"/>
+    <col collapsed="false" hidden="false" max="6" min="4" style="7" width="9.83137254901961"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="7" width="5.8078431372549"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="23.55" outlineLevel="0" r="1" s="6">
@@ -18650,7 +18690,7 @@
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="greaterThan" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E4:E203" type="decimal">
-      <formula1>#REF!</formula1>
+      <formula1>#ref!</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" error="Value must be between 0 and 100" errorTitle="Invalid entry" operator="between" prompt="Value must be between 0 and 100" promptTitle="Enter a percentage" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="F4:F203" type="decimal">
@@ -18683,14 +18723,14 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="24.5176470588235"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="10.5254901960784"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="12.0666666666667"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="7" width="9.90980392156863"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="7" width="15.2666666666667"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="7" width="14.0392156862745"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="7" width="12.8862745098039"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="7" width="5.78039215686275"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="24.6156862745098"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="10.5686274509804"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="12.1098039215686"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="7" width="9.95294117647059"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="7" width="15.3294117647059"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="7" width="14.0980392156863"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="7" width="12.9450980392157"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="7" width="5.8078431372549"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="1" s="6">
@@ -18845,10 +18885,10 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="15.4392156862745"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="13.2078431372549"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="15.3607843137255"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="7" width="5.78039215686275"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="15.5019607843137"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="13.2588235294118"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="15.4235294117647"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="7" width="5.8078431372549"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="13.2" outlineLevel="0" r="1" s="6">
@@ -19022,12 +19062,12 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="14.4352941176471"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="12.0392156862745"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="11.9411764705882"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="7" width="13.5019607843137"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="7" width="17.9647058823529"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="7" width="5.78039215686275"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="14.4980392156863"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="12.0901960784314"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="11.9882352941176"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="7" width="13.5607843137255"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="7" width="18.0352941176471"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="7" width="5.8078431372549"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="13.2" outlineLevel="0" r="1" s="6">
@@ -19090,11 +19130,11 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="18.1725490196078"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="22.8549019607843"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="7" width="10.0313725490196"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="7" width="11.043137254902"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="7" width="5.78039215686275"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="18.2509803921569"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="22.9450980392157"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="7" width="10.0745098039216"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="7" width="11.0941176470588"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="7" width="5.8078431372549"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="13.2" outlineLevel="0" r="1" s="6">
@@ -19223,21 +19263,21 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="27" width="4.36078431372549"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="27" width="6.93333333333333"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="27" width="9.83921568627451"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="27" width="16.721568627451"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="27" width="14.8078431372549"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="27" width="9.49411764705882"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="27" width="12.4039215686275"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="27" width="10.5254901960784"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="27" width="10.1843137254902"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="27" width="8.89019607843137"/>
-    <col collapsed="false" hidden="false" max="12" min="11" style="27" width="14.8078431372549"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="27" width="11.6392156862745"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="27" width="10.0980392156863"/>
-    <col collapsed="false" hidden="false" max="16" min="15" style="27" width="29.1921568627451"/>
-    <col collapsed="false" hidden="false" max="1025" min="17" style="27" width="14.8078431372549"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="27" width="4.38039215686275"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="27" width="6.96470588235294"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="27" width="9.88235294117647"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="27" width="16.7882352941176"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="27" width="14.8705882352941"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="27" width="9.52941176470588"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="27" width="12.4549019607843"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="27" width="10.5686274509804"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="27" width="10.2274509803922"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="27" width="8.92941176470588"/>
+    <col collapsed="false" hidden="false" max="12" min="11" style="27" width="14.8705882352941"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="27" width="11.6901960784314"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="27" width="10.1411764705882"/>
+    <col collapsed="false" hidden="false" max="16" min="15" style="27" width="29.3137254901961"/>
+    <col collapsed="false" hidden="false" max="1025" min="17" style="27" width="14.8705882352941"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="1" s="16">
@@ -20297,13 +20337,13 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="16.8588235294118"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="30.1333333333333"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="5.78039215686275"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="7" width="5.83529411764706"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="7" width="5.78039215686275"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="7" width="18.2274509803922"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="7" width="5.78039215686275"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="16.9294117647059"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="30.2627450980392"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="5.8078431372549"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="7" width="5.85882352941176"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="7" width="5.8078431372549"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="7" width="18.3019607843137"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="7" width="5.8078431372549"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="13.2" outlineLevel="0" r="1" s="6">
@@ -20627,9 +20667,9 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="20.1137254901961"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="38.1764705882353"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="7" width="5.78039215686275"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="20.2"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="38.3372549019608"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="7" width="5.8078431372549"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="12.2" outlineLevel="0" r="1" s="6">
@@ -20701,10 +20741,10 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="16.0901960784314"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="20.2235294117647"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="14.5843137254902"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="7" width="5.78039215686275"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="16.156862745098"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="20.3098039215686"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="14.643137254902"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="7" width="5.8078431372549"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="12.2" outlineLevel="0" r="1" s="6">
@@ -20778,9 +20818,9 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="17.5764705882353"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="16.878431372549"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="7" width="5.78039215686275"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="17.6470588235294"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="16.9529411764706"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="7" width="5.8078431372549"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="13.2" outlineLevel="0" r="1" s="6">
@@ -20857,12 +20897,12 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="22.1647058823529"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="15.2901960784314"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="10.6039215686275"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="7" width="10.4196078431373"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="7" width="9.90980392156863"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="7" width="5.78039215686275"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="22.2588235294118"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="15.3529411764706"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="10.6470588235294"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="7" width="10.4627450980392"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="7" width="9.95294117647059"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="7" width="5.8078431372549"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="1" s="6">
@@ -21254,12 +21294,12 @@
   </sheetViews>
   <cols>
     <col collapsed="false" hidden="true" max="1" min="1" style="6" width="0"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="26.3529411764706"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="112" width="6.59607843137255"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="7" width="23.5843137254902"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="7" width="20.1843137254902"/>
-    <col collapsed="false" hidden="false" max="1023" min="6" style="7" width="5.78039215686275"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="7" width="4.94901960784314"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="26.4588235294118"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="112" width="6.62745098039216"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="7" width="23.678431372549"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="7" width="20.2705882352941"/>
+    <col collapsed="false" hidden="false" max="1023" min="6" style="7" width="5.8078431372549"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="7" width="4.96862745098039"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="12.2" outlineLevel="0" r="1" s="6">
@@ -21710,15 +21750,15 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="111" width="9.90980392156863"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="111" width="8.66274509803922"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="111" width="9.90980392156863"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="140" width="6.9921568627451"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="111" width="8.39607843137255"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="111" width="7.82352941176471"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="111" width="6.59607843137255"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="111" width="9.90980392156863"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="111" width="8.10196078431373"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="111" width="9.95294117647059"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="111" width="8.69803921568627"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="111" width="9.95294117647059"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="140" width="7.01960784313726"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="111" width="8.43137254901961"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="111" width="7.85098039215686"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="111" width="6.62745098039216"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="111" width="9.95294117647059"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="111" width="8.13333333333333"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="44.75" outlineLevel="0" r="1" s="68">
@@ -22975,75 +23015,207 @@
   </sheetPr>
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="C2" activeCellId="0" pane="topLeft" sqref="C2"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A3" activeCellId="0" pane="topLeft" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="147" width="27.2509803921569"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="40" width="18.3372549019608"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="40" width="18.2352941176471"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="40" width="9.18039215686274"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="147" width="27.3647058823529"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="40" width="18.4156862745098"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="40" width="18.3058823529412"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="40" width="9.22352941176471"/>
+  </cols>
+  <sheetData>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="1">
+      <c r="A1" s="147" t="s">
+        <v>202</v>
+      </c>
+      <c r="B1" s="40" t="s">
+        <v>1276</v>
+      </c>
+      <c r="C1" s="40" t="s">
+        <v>1277</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="26.1" outlineLevel="0" r="2" s="149">
+      <c r="A2" s="148" t="s">
+        <v>1278</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="25.35" outlineLevel="0" r="3" s="53">
+      <c r="A3" s="150" t="s">
+        <v>206</v>
+      </c>
+      <c r="B3" s="53" t="s">
+        <v>1279</v>
+      </c>
+      <c r="C3" s="53" t="s">
+        <v>1280</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="4">
+      <c r="A4" s="147" t="s">
+        <v>1281</v>
+      </c>
+      <c r="B4" s="151" t="n">
+        <v>41091</v>
+      </c>
+      <c r="C4" s="151" t="n">
+        <v>41121</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="5">
+      <c r="A5" s="147" t="s">
+        <v>1282</v>
+      </c>
+      <c r="B5" s="151" t="n">
+        <v>41122</v>
+      </c>
+      <c r="C5" s="151" t="n">
+        <v>41152</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="6">
+      <c r="A6" s="147" t="s">
+        <v>1283</v>
+      </c>
+      <c r="B6" s="151" t="n">
+        <v>41153</v>
+      </c>
+      <c r="C6" s="151" t="n">
+        <v>41182</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="F8" activeCellId="0" pane="topLeft" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="40" width="19.5843137254902"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="40" width="27.9725490196078"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="40" width="9.18039215686274"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="1">
-      <c r="A1" s="147" t="s">
+      <c r="A1" s="40" t="s">
         <v>202</v>
       </c>
       <c r="B1" s="40" t="s">
-        <v>1276</v>
+        <v>203</v>
       </c>
       <c r="C1" s="40" t="s">
-        <v>1277</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="26.1" outlineLevel="0" r="2" s="149">
-      <c r="A2" s="148" t="s">
-        <v>1278</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="25.35" outlineLevel="0" r="3" s="53">
-      <c r="A3" s="150" t="s">
+        <v>1284</v>
+      </c>
+      <c r="D1" s="40" t="s">
+        <v>755</v>
+      </c>
+      <c r="E1" s="40" t="s">
+        <v>1285</v>
+      </c>
+      <c r="F1" s="40" t="s">
+        <v>1286</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="38.05" outlineLevel="0" r="2" s="152">
+      <c r="A2" s="152" t="s">
+        <v>1287</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="23.85" outlineLevel="0" r="3" s="53">
+      <c r="A3" s="53" t="s">
         <v>206</v>
       </c>
       <c r="B3" s="53" t="s">
-        <v>1279</v>
-      </c>
-      <c r="C3" s="53" t="s">
-        <v>1280</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="4">
-      <c r="A4" s="147" t="s">
-        <v>1281</v>
-      </c>
-      <c r="B4" s="151" t="n">
-        <v>41091</v>
-      </c>
-      <c r="C4" s="151" t="n">
-        <v>41121</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="5">
-      <c r="A5" s="147" t="s">
-        <v>1282</v>
-      </c>
-      <c r="B5" s="151" t="n">
-        <v>41122</v>
-      </c>
-      <c r="C5" s="151" t="n">
-        <v>41152</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="6">
-      <c r="A6" s="147" t="s">
-        <v>1283</v>
-      </c>
-      <c r="B6" s="151" t="n">
-        <v>41153</v>
-      </c>
-      <c r="C6" s="151" t="n">
-        <v>41182</v>
+        <v>39</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="4">
+      <c r="A4" s="40" t="s">
+        <v>1288</v>
+      </c>
+      <c r="B4" s="40" t="s">
+        <v>1289</v>
+      </c>
+      <c r="C4" s="40" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" s="40" t="s">
+        <v>1290</v>
+      </c>
+      <c r="E4" s="40" t="n">
+        <v>14</v>
+      </c>
+      <c r="F4" s="40" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="5">
+      <c r="A5" s="40" t="s">
+        <v>1291</v>
+      </c>
+      <c r="C5" s="40" t="n">
+        <v>500</v>
+      </c>
+      <c r="D5" s="40" t="s">
+        <v>765</v>
+      </c>
+      <c r="E5" s="40" t="n">
+        <v>14</v>
+      </c>
+      <c r="F5" s="40" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="6">
+      <c r="A6" s="40" t="s">
+        <v>1292</v>
+      </c>
+      <c r="B6" s="40" t="s">
+        <v>1293</v>
+      </c>
+      <c r="C6" s="40" t="n">
+        <v>100</v>
+      </c>
+      <c r="D6" s="40" t="s">
+        <v>765</v>
+      </c>
+      <c r="E6" s="40" t="n">
+        <v>14</v>
+      </c>
+      <c r="F6" s="40" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="7">
+      <c r="A7" s="40" t="s">
+        <v>1294</v>
+      </c>
+      <c r="B7" s="40" t="s">
+        <v>1295</v>
+      </c>
+      <c r="E7" s="40" t="n">
+        <v>14</v>
+      </c>
+      <c r="F7" s="40" t="n">
+        <v>185</v>
       </c>
     </row>
   </sheetData>
@@ -23069,11 +23241,11 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="11.8313725490196"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="22.2666666666667"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="14.556862745098"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="7" width="11.5176470588235"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="7" width="5.78039215686275"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="11.8823529411765"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="22.356862745098"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="14.6196078431373"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="7" width="11.5647058823529"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="7" width="5.8078431372549"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="13.2" outlineLevel="0" r="1" s="6">
@@ -23255,29 +23427,29 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="40" width="15.6823529411765"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="40" width="8.40392156862745"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="41" width="7.97254901960784"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="40" width="10.7411764705882"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="40" width="12.1254901960784"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="40" width="19.5686274509804"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="40" width="11.4078431372549"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="40" width="8.88627450980392"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="40" width="9.68235294117647"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="40" width="8.49019607843137"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="40" width="11.4078431372549"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="40" width="10.2117647058824"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="40" width="7.70196078431373"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="40" width="8.49019607843137"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="40" width="7.29411764705882"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="40" width="10.2117647058824"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="40" width="10.3529411764706"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="40" width="7.82352941176471"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="40" width="8.61960784313725"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="40" width="7.42352941176471"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="40" width="10.3529411764706"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="42" width="11.0156862745098"/>
-    <col collapsed="false" hidden="false" max="1025" min="25" style="40" width="7.42352941176471"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="40" width="15.7490196078431"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="40" width="8.43921568627451"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="41" width="8.00392156862745"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="40" width="10.7843137254902"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="40" width="12.1764705882353"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="40" width="19.6470588235294"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="40" width="11.4588235294118"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="40" width="8.92156862745098"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="40" width="9.72549019607843"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="40" width="8.52549019607843"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="40" width="11.4588235294118"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="40" width="10.2549019607843"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="40" width="7.72941176470588"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="40" width="8.52549019607843"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="40" width="7.32941176470588"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="40" width="10.2549019607843"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="40" width="10.3960784313725"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="40" width="7.85098039215686"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="40" width="8.65490196078431"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="40" width="7.45882352941177"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="40" width="10.3960784313725"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="42" width="11.0627450980392"/>
+    <col collapsed="false" hidden="false" max="1025" min="25" style="40" width="7.45882352941177"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="14.15" outlineLevel="0" r="1" s="43">
@@ -23711,20 +23883,20 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="27" width="10.9725490196078"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="27" width="6.76078431372549"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="27" width="8.55294117647059"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="27" width="9.4078431372549"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="27" width="10.0549019607843"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="27" width="11.2745098039216"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="27" width="10.2901960784314"/>
-    <col collapsed="false" hidden="false" max="12" min="9" style="27" width="8.36862745098039"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="27" width="16.2549019607843"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="27" width="12.1254901960784"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="27" width="12.4549019607843"/>
-    <col collapsed="false" hidden="false" max="26" min="16" style="27" width="7.45882352941177"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="27" width="8.82745098039216"/>
-    <col collapsed="false" hidden="false" max="1025" min="28" style="27" width="5.78039215686275"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="27" width="11.0156862745098"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="27" width="6.7921568627451"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="27" width="8.5921568627451"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="27" width="9.45098039215686"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="27" width="10.0980392156863"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="27" width="11.321568627451"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="27" width="10.3333333333333"/>
+    <col collapsed="false" hidden="false" max="12" min="9" style="27" width="8.40392156862745"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="27" width="16.321568627451"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="27" width="12.1764705882353"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="27" width="12.5058823529412"/>
+    <col collapsed="false" hidden="false" max="26" min="16" style="27" width="7.48627450980392"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="27" width="8.86274509803922"/>
+    <col collapsed="false" hidden="false" max="1025" min="28" style="27" width="5.8078431372549"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="12.2" outlineLevel="0" r="1" s="16">
@@ -24555,9 +24727,9 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="17.8823529411765"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="18.721568627451"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="7" width="5.78039215686275"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="17.956862745098"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="18.7960784313725"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="7" width="5.8078431372549"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="12.2" outlineLevel="0" r="1" s="6">
@@ -24648,10 +24820,10 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="18.5725490196078"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="14.356862745098"/>
-    <col collapsed="false" hidden="false" max="5" min="3" style="7" width="13.6666666666667"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="7" width="5.78039215686275"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="18.6509803921569"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="14.4117647058824"/>
+    <col collapsed="false" hidden="false" max="5" min="3" style="7" width="13.7254901960784"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="7" width="5.8078431372549"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="13.2" outlineLevel="0" r="1" s="6">

</xml_diff>

<commit_message>
Update tests - Including new setup data with corrected templates.
</commit_message>
<xml_diff>
--- a/bika/lims/setupdata/test/test.xlsx
+++ b/bika/lims/setupdata/test/test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="742" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="32" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="742" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" state="visible" r:id="rId2"/>
@@ -85,14 +85,14 @@
               <xdr:from>
                 <xdr:col>7</xdr:col>
                 <xdr:colOff>3</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>24</xdr:rowOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>32</xdr:rowOff>
               </xdr:from>
               <xdr:to>
                 <xdr:col>10</xdr:col>
                 <xdr:colOff>3</xdr:colOff>
-                <xdr:row>6</xdr:row>
-                <xdr:rowOff>14</xdr:rowOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>15</xdr:rowOff>
               </xdr:to>
             </anchor>
           </commentPr>
@@ -220,15 +220,15 @@
             <anchor moveWithCells="false" sizeWithCells="false">
               <xdr:from>
                 <xdr:col>2</xdr:col>
-                <xdr:colOff>26</xdr:colOff>
+                <xdr:colOff>25</xdr:colOff>
                 <xdr:row>-1</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </xdr:from>
               <xdr:to>
                 <xdr:col>5</xdr:col>
-                <xdr:colOff>41</xdr:colOff>
-                <xdr:row>11</xdr:row>
-                <xdr:rowOff>3</xdr:rowOff>
+                <xdr:colOff>39</xdr:colOff>
+                <xdr:row>12</xdr:row>
+                <xdr:rowOff>8</xdr:rowOff>
               </xdr:to>
             </anchor>
           </commentPr>
@@ -267,13 +267,13 @@
                 <xdr:col>1</xdr:col>
                 <xdr:colOff>3</xdr:colOff>
                 <xdr:row>1</xdr:row>
-                <xdr:rowOff>18</xdr:rowOff>
+                <xdr:rowOff>6</xdr:rowOff>
               </xdr:from>
               <xdr:to>
                 <xdr:col>3</xdr:col>
                 <xdr:colOff>3</xdr:colOff>
                 <xdr:row>7</xdr:row>
-                <xdr:rowOff>7</xdr:rowOff>
+                <xdr:rowOff>4</xdr:rowOff>
               </xdr:to>
             </anchor>
           </commentPr>
@@ -4918,11 +4918,11 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="3.56470588235294"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="60.556862745098"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="11.043137254902"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="2" width="8.41176470588235"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="2" width="7.23529411764706"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="3.57647058823529"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="60.8078431372549"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="11.0941176470588"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="2" width="8.44705882352941"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="2" width="7.26274509803922"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="32.05" outlineLevel="0" r="1" s="6">
@@ -5012,10 +5012,10 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="10" width="23.4196078431373"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="18.1137254901961"/>
-    <col collapsed="false" hidden="false" max="5" min="3" style="10" width="17.2392156862745"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="10" width="7.28627450980392"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="10" width="23.521568627451"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="18.1843137254902"/>
+    <col collapsed="false" hidden="false" max="5" min="3" style="10" width="17.3098039215686"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="10" width="7.31372549019608"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="true" ht="12.2" outlineLevel="0" r="1" s="9">
@@ -5348,13 +5348,13 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="10" width="24.7098039215686"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="27.9607843137255"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="8.18823529411765"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="10" width="20"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="10" width="11.1372549019608"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="10" width="13.4666666666667"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="10" width="7.28627450980392"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="10" width="24.8117647058824"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="28.0745098039216"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="8.21960784313725"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="10" width="20.0862745098039"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="10" width="11.1882352941176"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="10" width="13.5254901960784"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="10" width="7.31372549019608"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="true" ht="12.2" outlineLevel="0" r="1" s="9">
@@ -5538,9 +5538,9 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="10" width="14.9372549019608"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="23.8941176470588"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="10" width="7.28627450980392"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="10" width="15"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="23.9921568627451"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="10" width="7.31372549019608"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="true" ht="12.2" outlineLevel="0" r="1" s="9">
@@ -5647,16 +5647,16 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="40" width="16.2627450980392"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="40" width="31.6862745098039"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="40" width="8.18823529411765"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="40" width="5.67058823529412"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="40" width="10.6"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="40" width="8.30196078431373"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="40" width="9.17254901960784"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="40" width="17.3764705882353"/>
-    <col collapsed="false" hidden="false" max="1023" min="9" style="40" width="8.30196078431373"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="10" width="7.09019607843137"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="40" width="16.3294117647059"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="40" width="31.8156862745098"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="40" width="8.21960784313725"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="40" width="5.69411764705882"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="40" width="10.643137254902"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="40" width="8.34117647058824"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="40" width="9.2156862745098"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="40" width="17.4470588235294"/>
+    <col collapsed="false" hidden="false" max="1023" min="9" style="40" width="8.34117647058824"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="10" width="7.12156862745098"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="true" ht="13.2" outlineLevel="0" r="1" s="29">
@@ -6083,14 +6083,14 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="10" width="15.7843137254902"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="30.4823529411765"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="10" width="20.3294117647059"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="10" width="21.5254901960784"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="10" width="9.32941176470588"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="10" width="12.4039215686275"/>
-    <col collapsed="false" hidden="false" max="1018" min="9" style="10" width="7.28627450980392"/>
-    <col collapsed="false" hidden="false" max="1025" min="1019" style="10" width="6.94901960784314"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="10" width="15.8470588235294"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="30.6039215686275"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="10" width="20.4156862745098"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="10" width="21.6117647058824"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="10" width="9.36470588235294"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="10" width="12.4549019607843"/>
+    <col collapsed="false" hidden="false" max="1018" min="9" style="10" width="7.31372549019608"/>
+    <col collapsed="false" hidden="false" max="1025" min="1019" style="10" width="6.97647058823529"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="true" ht="12.2" outlineLevel="0" r="1" s="9">
@@ -6359,11 +6359,11 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="40" width="23.0392156862745"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="40" width="26.4235294117647"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="19.5490196078431"/>
-    <col collapsed="false" hidden="false" max="1018" min="4" style="40" width="7.28627450980392"/>
-    <col collapsed="false" hidden="false" max="1025" min="1019" style="10" width="6.23921568627451"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="40" width="23.1333333333333"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="40" width="26.5333333333333"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="19.6352941176471"/>
+    <col collapsed="false" hidden="false" max="1018" min="4" style="40" width="7.31372549019608"/>
+    <col collapsed="false" hidden="false" max="1025" min="1019" style="10" width="6.26666666666667"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="true" ht="12.2" outlineLevel="0" r="1" s="29">
@@ -6431,10 +6431,10 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="40" width="18.9803921568627"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="40" width="68.7764705882353"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="40" width="30.4823529411765"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="40" width="7.28627450980392"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="40" width="19.0588235294118"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="40" width="69.0627450980392"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="40" width="30.6039215686275"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="40" width="7.31372549019608"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="true" ht="12.2" outlineLevel="0" r="1" s="29">
@@ -6555,9 +6555,9 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="10" width="30.4392156862745"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="20.6313725490196"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="10" width="7.28627450980392"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="10" width="30.5607843137255"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="20.7176470588235"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="10" width="7.31372549019608"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="true" ht="12.2" outlineLevel="0" r="1" s="9">
@@ -6695,11 +6695,11 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="10" width="20.5098039215686"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="10" width="11.7960784313726"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="10" width="18.8509803921569"/>
-    <col collapsed="false" hidden="false" max="21" min="6" style="10" width="11.7960784313726"/>
-    <col collapsed="false" hidden="false" max="1025" min="22" style="10" width="20.5098039215686"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="10" width="20.5960784313725"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="10" width="11.8470588235294"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="10" width="18.9294117647059"/>
+    <col collapsed="false" hidden="false" max="21" min="6" style="10" width="11.8470588235294"/>
+    <col collapsed="false" hidden="false" max="1025" min="22" style="10" width="20.5960784313725"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="true" ht="12.2" outlineLevel="0" r="1" s="9">
@@ -6925,9 +6925,9 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="10" width="28.0588235294118"/>
-    <col collapsed="false" hidden="false" max="21" min="2" style="10" width="9.89019607843137"/>
-    <col collapsed="false" hidden="false" max="1025" min="22" style="10" width="7.28627450980392"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="10" width="28.1725490196078"/>
+    <col collapsed="false" hidden="false" max="21" min="2" style="10" width="9.93333333333333"/>
+    <col collapsed="false" hidden="false" max="1025" min="22" style="10" width="7.31372549019608"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="true" ht="12.2" outlineLevel="0" r="1" s="9">
@@ -7198,18 +7198,18 @@
   </sheetPr>
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="D23" activeCellId="0" pane="topLeft" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <cols>
     <col collapsed="false" hidden="true" max="1" min="1" style="9" width="0"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="33.2352941176471"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="11" width="8.32549019607843"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="10" width="29.7450980392157"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="10" width="25.4627450980392"/>
-    <col collapsed="false" hidden="false" max="1023" min="6" style="10" width="7.28627450980392"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="10" width="6.23921568627451"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="33.3725490196078"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="11" width="8.36078431372549"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="10" width="29.8666666666667"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="10" width="25.5647058823529"/>
+    <col collapsed="false" hidden="false" max="1023" min="6" style="10" width="7.31372549019608"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="10" width="6.26666666666667"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="true" ht="12.2" outlineLevel="0" r="1" s="9">
@@ -7638,10 +7638,10 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.5882352941176"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.9490196078431"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="9.4"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.36470588235294"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.6980392156863"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.0941176470588"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="9.43529411764706"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.4"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13.4" outlineLevel="0" r="1">
@@ -7758,18 +7758,18 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="96" width="24.7098039215686"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="96" width="29.1725490196078"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="96" width="21.2274509803922"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="96" width="21.0549019607843"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="96" width="15.5960784313726"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="97" width="28.2745098039216"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="97" width="13.6588235294118"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="97" width="14.0196078431373"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="98" width="15.2588235294118"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="96" width="9.4"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="96" width="13.9333333333333"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="96" width="7.28627450980392"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="96" width="24.8117647058824"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="96" width="29.2941176470588"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="96" width="21.3137254901961"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="96" width="21.1450980392157"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="96" width="15.6627450980392"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="97" width="28.3882352941176"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="97" width="13.7176470588235"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="97" width="14.0745098039216"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="98" width="15.3254901960784"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="96" width="9.43529411764706"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="96" width="13.9921568627451"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="96" width="7.31372549019608"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="true" ht="13.4" outlineLevel="0" r="1" s="99">
@@ -8996,15 +8996,15 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.0705882352941"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.3372549019608"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.156862745098"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.6745098039216"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.5372549019608"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.2823529411765"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="20.6313725490196"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="35.4039215686275"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.4"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.1490196078431"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.4235294117647"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.2156862745098"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.7254901960784"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.6078431372549"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.3686274509804"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="20.7176470588235"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="35.5529411764706"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.43529411764706"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="15.1" outlineLevel="0" r="1" s="99">
@@ -9142,15 +9142,15 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.0705882352941"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.321568627451"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.156862745098"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.6745098039216"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.5372549019608"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.2823529411765"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="20.6313725490196"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="35.4039215686275"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.4"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.1490196078431"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.3764705882353"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.2156862745098"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.7254901960784"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.6078431372549"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.3686274509804"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="20.7176470588235"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="35.5529411764706"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.43529411764706"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="15.1" outlineLevel="0" r="1" s="99">
@@ -9281,14 +9281,14 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.443137254902"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.4235294117647"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.4"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.9490196078431"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.4"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.0941176470588"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.6862745098039"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="9.4"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.5137254901961"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.5254901960784"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.43529411764706"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.9921568627451"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.43529411764706"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.1764705882353"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.8156862745098"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="9.43529411764706"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="14.9" outlineLevel="0" r="1">
@@ -10271,18 +10271,18 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.3686274509804"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.556862745098"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.3803921568627"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.4705882352941"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.8392156862745"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.4"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.4901960784314"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.5764705882353"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.8823529411765"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="6.50588235294118"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="113" width="9.4"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="9.4"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.4392156862745"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.678431372549"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.4745098039216"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.521568627451"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.8980392156863"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.43529411764706"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.5607843137255"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.6470588235294"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.9607843137255"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="6.53333333333333"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="113" width="9.43529411764706"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="9.43529411764706"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="14.9" outlineLevel="0" r="1" s="99">
@@ -10498,17 +10498,17 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.4352941176471"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.6823529411765"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.2823529411765"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.4705882352941"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.8392156862745"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.3058823529412"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.5764705882353"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.1058823529412"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="34.0470588235294"/>
-    <col collapsed="false" hidden="false" max="1023" min="10" style="0" width="9.4"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="9.36470588235294"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.5254901960784"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.7960784313725"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.3803921568627"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.521568627451"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.8980392156863"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.3843137254902"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.6470588235294"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.1607843137255"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="34.1921568627451"/>
+    <col collapsed="false" hidden="false" max="1023" min="10" style="0" width="9.43529411764706"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="9.4"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="14.9" outlineLevel="0" r="1" s="99">
@@ -10600,10 +10600,10 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="10" width="35.4941176470588"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="39.9647058823529"/>
-    <col collapsed="false" hidden="false" max="5" min="3" style="10" width="25.7921568627451"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="10" width="7.28627450980392"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="10" width="35.6392156862745"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="40.1294117647059"/>
+    <col collapsed="false" hidden="false" max="5" min="3" style="10" width="25.9019607843137"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="10" width="7.31372549019608"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="true" ht="12.2" outlineLevel="0" r="1" s="9">
@@ -10702,27 +10702,27 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="40" width="25.5803921568627"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="40" width="35.7254901960784"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="40" width="10.1686274509804"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="40" width="6.43921568627451"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="40" width="21.5254901960784"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="40" width="12.6"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="119" width="12.3686274509804"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="40" width="9.02745098039216"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="29" width="7.45882352941177"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="40" width="9.34901960784314"/>
-    <col collapsed="false" hidden="false" max="13" min="11" style="40" width="4.47450980392157"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="40" width="4.82745098039216"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="40" width="7.83921568627451"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="40" width="4.06666666666667"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="40" width="16.5058823529412"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="40" width="11.8313725490196"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="40" width="16.3843137254902"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="119" width="13.9960784313726"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="40" width="11.2509803921569"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="40" width="10.2117647058824"/>
-    <col collapsed="false" hidden="false" max="1025" min="23" style="40" width="9.36470588235294"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="40" width="25.6862745098039"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="40" width="35.8745098039216"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="40" width="10.2117647058824"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="40" width="6.46274509803922"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="40" width="21.6117647058824"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="40" width="12.6509803921569"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="119" width="12.4196078431373"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="40" width="9.06274509803922"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="29" width="7.48627450980392"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="40" width="9.38823529411765"/>
+    <col collapsed="false" hidden="false" max="13" min="11" style="40" width="4.49019607843137"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="40" width="4.84705882352941"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="40" width="7.87450980392157"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="40" width="4.07843137254902"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="40" width="16.5725490196078"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="40" width="11.8823529411765"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="40" width="16.4509803921569"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="119" width="14.0549019607843"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="40" width="11.2941176470588"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="40" width="10.2549019607843"/>
+    <col collapsed="false" hidden="false" max="1025" min="23" style="40" width="9.4"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="true" ht="24.5" outlineLevel="0" r="1" s="29">
@@ -12341,12 +12341,12 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="10" width="34.4274509803922"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="10.8196078431373"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="10.556862745098"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="10" width="17.4823529411765"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="10" width="4.06666666666667"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="10" width="7.28627450980392"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="10" width="34.5725490196078"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="10.8627450980392"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="10.6039215686275"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="10" width="17.5529411764706"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="10" width="4.07843137254902"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="10" width="7.31372549019608"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="true" ht="12.2" outlineLevel="0" r="1" s="9">
@@ -12413,10 +12413,10 @@
   </sheetViews>
   <cols>
     <col collapsed="false" hidden="true" max="1" min="1" style="9" width="0"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="9" width="19.2549019607843"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="7.74509803921569"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="10" width="5.7921568627451"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="10" width="8.26666666666667"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="9" width="19.3333333333333"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="7.78039215686275"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="10" width="5.8156862745098"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="10" width="8.30196078431373"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="true" ht="12.2" outlineLevel="0" r="1" s="9">
@@ -12610,12 +12610,12 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="40" width="12.9019607843137"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="40" width="14.2117647058824"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="130" width="10.4117647058824"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="40" width="17.4901960784314"/>
-    <col collapsed="false" hidden="false" max="973" min="5" style="40" width="7.28627450980392"/>
-    <col collapsed="false" hidden="false" max="1025" min="974" style="10" width="6.23921568627451"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="40" width="12.956862745098"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="40" width="14.2705882352941"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="130" width="10.4549019607843"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="40" width="17.5607843137255"/>
+    <col collapsed="false" hidden="false" max="973" min="5" style="40" width="7.31372549019608"/>
+    <col collapsed="false" hidden="false" max="1025" min="974" style="10" width="6.26666666666667"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="true" ht="13.2" outlineLevel="0" r="1" s="29">
@@ -12818,12 +12818,12 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="40" width="44.1450980392157"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="40" width="11.5254901960784"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="40" width="11.9176470588235"/>
-    <col collapsed="false" hidden="false" max="997" min="5" style="40" width="7.28627450980392"/>
-    <col collapsed="false" hidden="false" max="1023" min="998" style="10" width="6.23921568627451"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="6.23921568627451"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="40" width="44.3294117647059"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="40" width="11.5725490196078"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="40" width="11.9686274509804"/>
+    <col collapsed="false" hidden="false" max="997" min="5" style="40" width="7.31372549019608"/>
+    <col collapsed="false" hidden="false" max="1023" min="998" style="10" width="6.26666666666667"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="6.26666666666667"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="true" ht="24.5" outlineLevel="0" r="1" s="29">
@@ -14295,10 +14295,10 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="132" width="21.1686274509804"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="132" width="57.3176470588235"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="132" width="58.0196078431373"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="132" width="7.76078431372549"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="132" width="21.2549019607843"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="132" width="57.5529411764706"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="132" width="58.2627450980392"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="132" width="7.79607843137255"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="true" ht="14.15" outlineLevel="0" r="1" s="133">
@@ -14425,17 +14425,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F99"/>
+  <dimension ref="A1:G99"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A17" activeCellId="0" pane="topLeft" sqref="A17"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="C34" activeCellId="0" pane="topLeft" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="10" width="30.5490196078431"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="10" width="8.8"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="10" width="4.06666666666667"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="10" width="7.28627450980392"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="10" width="30.678431372549"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="10" width="8.84313725490196"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="10" width="4.07843137254902"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="10" width="7.31372549019608"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="true" ht="12.2" outlineLevel="0" r="1" s="9">
@@ -14497,11 +14497,14 @@
       <c r="D4" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="E4" s="137" t="s">
+      <c r="E4" s="137" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" s="10" t="s">
         <v>929</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.2" outlineLevel="0" r="5">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="5">
       <c r="A5" s="88" t="s">
         <v>553</v>
       </c>
@@ -14514,9 +14517,11 @@
       <c r="D5" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="E5" s="137"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="6">
+      <c r="E5" s="137" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="6">
       <c r="A6" s="88" t="s">
         <v>848</v>
       </c>
@@ -14529,11 +14534,14 @@
       <c r="D6" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="E6" s="137" t="s">
+      <c r="E6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="45" t="s">
         <v>934</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="7">
       <c r="A7" s="88" t="s">
         <v>848</v>
       </c>
@@ -14546,12 +14554,14 @@
       <c r="D7" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="E7" s="137" t="s">
+      <c r="E7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" s="45" t="s">
         <v>934</v>
       </c>
-      <c r="F7" s="45"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="8">
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="8">
       <c r="A8" s="88" t="s">
         <v>848</v>
       </c>
@@ -14564,12 +14574,14 @@
       <c r="D8" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="E8" s="137" t="s">
+      <c r="E8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" s="45" t="s">
         <v>934</v>
       </c>
-      <c r="F8" s="45"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="9">
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="9">
       <c r="A9" s="88" t="s">
         <v>910</v>
       </c>
@@ -14582,12 +14594,14 @@
       <c r="D9" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="E9" s="137" t="s">
+      <c r="E9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" s="45" t="s">
         <v>934</v>
       </c>
-      <c r="F9" s="45"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="10">
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="10">
       <c r="A10" s="88" t="s">
         <v>910</v>
       </c>
@@ -14600,12 +14614,14 @@
       <c r="D10" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="E10" s="137" t="s">
+      <c r="E10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" s="45" t="s">
         <v>934</v>
       </c>
-      <c r="F10" s="45"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="11">
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="11">
       <c r="A11" s="88" t="s">
         <v>910</v>
       </c>
@@ -14618,12 +14634,14 @@
       <c r="D11" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="E11" s="137" t="s">
+      <c r="E11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" s="45" t="s">
         <v>934</v>
       </c>
-      <c r="F11" s="45"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="12">
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="12">
       <c r="A12" s="88" t="s">
         <v>913</v>
       </c>
@@ -14636,12 +14654,14 @@
       <c r="D12" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="E12" s="137" t="s">
+      <c r="E12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" s="45" t="s">
         <v>934</v>
       </c>
-      <c r="F12" s="45"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="13">
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="13">
       <c r="A13" s="88" t="s">
         <v>913</v>
       </c>
@@ -14651,15 +14671,18 @@
       <c r="C13" s="45" t="s">
         <v>936</v>
       </c>
-      <c r="D13" s="45" t="n">
+      <c r="D13" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="E13" s="45" t="s">
+      <c r="E13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" s="45" t="s">
         <v>934</v>
       </c>
-      <c r="F13" s="45"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="14">
+      <c r="G13" s="45"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="14">
       <c r="A14" s="88" t="s">
         <v>913</v>
       </c>
@@ -14669,15 +14692,18 @@
       <c r="C14" s="45" t="s">
         <v>938</v>
       </c>
-      <c r="D14" s="45" t="n">
+      <c r="D14" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="E14" s="45" t="s">
+      <c r="E14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" s="45" t="s">
         <v>934</v>
       </c>
-      <c r="F14" s="45"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="15">
+      <c r="G14" s="45"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="15">
       <c r="A15" s="88" t="s">
         <v>916</v>
       </c>
@@ -14687,15 +14713,18 @@
       <c r="C15" s="45" t="s">
         <v>940</v>
       </c>
-      <c r="D15" s="45" t="n">
+      <c r="D15" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="E15" s="45" t="s">
+      <c r="E15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" s="45" t="s">
         <v>934</v>
       </c>
-      <c r="F15" s="45"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="16">
+      <c r="G15" s="45"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="16">
       <c r="A16" s="88" t="s">
         <v>916</v>
       </c>
@@ -14705,15 +14734,18 @@
       <c r="C16" s="45" t="s">
         <v>936</v>
       </c>
-      <c r="D16" s="45" t="n">
+      <c r="D16" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="E16" s="45" t="s">
+      <c r="E16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" s="45" t="s">
         <v>934</v>
       </c>
-      <c r="F16" s="45"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="17">
+      <c r="G16" s="45"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="17">
       <c r="A17" s="88" t="s">
         <v>916</v>
       </c>
@@ -14723,13 +14755,16 @@
       <c r="C17" s="45" t="s">
         <v>938</v>
       </c>
-      <c r="D17" s="45" t="n">
+      <c r="D17" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="E17" s="45" t="s">
+      <c r="E17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" s="45" t="s">
         <v>934</v>
       </c>
-      <c r="F17" s="45"/>
+      <c r="G17" s="45"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.2" outlineLevel="0" r="18">
       <c r="A18" s="88"/>
@@ -15009,13 +15044,13 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="53" width="20.7607843137255"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="53" width="17.8980392156863"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="53" width="33.2313725490196"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="53" width="14.643137254902"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="53" width="13.0156862745098"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="53" width="6.71372549019608"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="53" width="7.28627450980392"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="53" width="20.8470588235294"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="53" width="17.9686274509804"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="53" width="33.3647058823529"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="53" width="14.7058823529412"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="53" width="13.0705882352941"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="53" width="6.74117647058824"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="53" width="7.31372549019608"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="true" ht="12.2" outlineLevel="0" r="1" s="56">
@@ -15144,10 +15179,10 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="53" width="27.3137254901961"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="53" width="33.8745098039216"/>
-    <col collapsed="false" hidden="false" max="6" min="3" style="53" width="35.8313725490196"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="53" width="7.28627450980392"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="53" width="27.4274509803922"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="53" width="34.0117647058824"/>
+    <col collapsed="false" hidden="false" max="6" min="3" style="53" width="35.9764705882353"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="53" width="7.31372549019608"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.2" outlineLevel="0" r="1" s="56">
@@ -15336,11 +15371,11 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="10" width="6.77647058823529"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="13.8313725490196"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="24.5450980392157"/>
-    <col collapsed="false" hidden="false" max="6" min="4" style="10" width="12.3411764705882"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="10" width="7.28627450980392"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="10" width="6.80392156862745"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="13.8901960784314"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="24.6470588235294"/>
+    <col collapsed="false" hidden="false" max="6" min="4" style="10" width="12.3921568627451"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="10" width="7.31372549019608"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="true" ht="12.2" outlineLevel="0" r="1" s="9">
@@ -18976,7 +19011,7 @@
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="greaterThan" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E4:E203" type="decimal">
-      <formula1>#REF!</formula1>
+      <formula1>#ref!</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" error="Value must be between 0 and 100" errorTitle="Invalid entry" operator="between" prompt="Value must be between 0 and 100" promptTitle="Enter a percentage" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="F4:F203" type="decimal">
@@ -19013,14 +19048,14 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="10" width="30.9294117647059"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="13.2823529411765"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="15.2235294117647"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="10" width="12.4901960784314"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="10" width="19.2666666666667"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="10" width="17.7137254901961"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="10" width="16.2549019607843"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="10" width="7.28627450980392"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="10" width="31.0588235294118"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="13.3372549019608"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="15.2901960784314"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="10" width="12.5411764705882"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="10" width="19.3450980392157"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="10" width="17.7843137254902"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="10" width="16.321568627451"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="10" width="7.31372549019608"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.2" outlineLevel="0" r="1" s="9">
@@ -19175,10 +19210,10 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="10" width="19.4745098039216"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="16.6588235294118"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="19.3686274509804"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="10" width="7.28627450980392"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="10" width="19.556862745098"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="16.7294117647059"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="19.4470588235294"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="10" width="7.31372549019608"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="true" ht="12.2" outlineLevel="0" r="1" s="9">
@@ -19352,12 +19387,12 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="10" width="18.2078431372549"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="15.1803921568627"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="15.0588235294118"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="10" width="17.0235294117647"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="10" width="22.6509803921569"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="10" width="7.28627450980392"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="10" width="18.278431372549"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="15.2470588235294"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="15.121568627451"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="10" width="17.0941176470588"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="10" width="22.7450980392157"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="10" width="7.31372549019608"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="true" ht="12.2" outlineLevel="0" r="1" s="9">
@@ -19421,9 +19456,9 @@
   </sheetViews>
   <cols>
     <col collapsed="false" hidden="true" max="1" min="1" style="9" width="0"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="9" width="40.4235294117647"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="21.4901960784314"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="10" width="8.30196078431373"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="9" width="40.5960784313726"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="21.5764705882353"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="10" width="8.34117647058824"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="true" ht="12.2" outlineLevel="0" r="1" s="9">
@@ -19822,11 +19857,11 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="10" width="22.9176470588235"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="28.8274509803922"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="10" width="12.6509803921569"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="10" width="13.9333333333333"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="10" width="7.28627450980392"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="10" width="23.0117647058824"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="28.9490196078431"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="10" width="12.7058823529412"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="10" width="13.9921568627451"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="10" width="7.31372549019608"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="true" ht="12.2" outlineLevel="0" r="1" s="9">
@@ -19955,13 +19990,13 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="10" width="21.2627450980392"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="38"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="7.28627450980392"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="10" width="7.35686274509804"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="10" width="7.28627450980392"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="10" width="22.9843137254902"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="10" width="7.28627450980392"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="10" width="21.3529411764706"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="38.156862745098"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="7.31372549019608"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="10" width="7.3843137254902"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="10" width="7.31372549019608"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="10" width="23.0745098039216"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="10" width="7.31372549019608"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="true" ht="12.2" outlineLevel="0" r="1" s="9">
@@ -20285,9 +20320,9 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="10" width="25.3686274509804"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="48.1529411764706"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="10" width="7.28627450980392"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="10" width="25.4705882352941"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="48.3529411764706"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="10" width="7.31372549019608"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="true" ht="12.2" outlineLevel="0" r="1" s="9">
@@ -20359,10 +20394,10 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="10" width="20.3019607843137"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="25.5058823529412"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="18.3843137254902"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="10" width="7.28627450980392"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="10" width="20.3882352941176"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="25.6156862745098"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="18.4588235294118"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="10" width="7.31372549019608"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="true" ht="12.2" outlineLevel="0" r="1" s="9">
@@ -20436,9 +20471,9 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="10" width="22.1647058823529"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="21.2980392156863"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="10" width="7.28627450980392"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="10" width="22.2588235294118"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="21.3921568627451"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="10" width="7.31372549019608"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="true" ht="12.2" outlineLevel="0" r="1" s="9">
@@ -20515,12 +20550,12 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="10" width="27.9607843137255"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="19.2745098039216"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="13.3725490196078"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="10" width="13.1372549019608"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="10" width="12.4901960784314"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="10" width="7.28627450980392"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="10" width="28.0745098039216"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="19.3529411764706"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="13.4313725490196"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="10" width="13.1960784313725"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="10" width="12.5411764705882"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="10" width="7.31372549019608"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.2" outlineLevel="0" r="1" s="9">
@@ -20911,15 +20946,15 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="16" width="12.4901960784314"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="16" width="10.921568627451"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="16" width="12.4901960784314"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="143" width="8.81960784313726"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="16" width="10.5921568627451"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="16" width="9.85882352941177"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="16" width="8.32549019607843"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="16" width="12.4901960784314"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="16" width="10.2274509803922"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="16" width="12.5411764705882"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="16" width="10.9725490196078"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="16" width="12.5411764705882"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="143" width="8.85490196078431"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="16" width="10.6352941176471"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="16" width="9.89411764705882"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="16" width="8.36078431372549"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="16" width="12.5411764705882"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="16" width="10.2705882352941"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="44.75" outlineLevel="0" r="1" s="81">
@@ -22181,21 +22216,21 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="40" width="5.50588235294118"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="40" width="8.74117647058823"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="40" width="12.4039215686275"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="40" width="21.0901960784314"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="40" width="18.6745098039216"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="40" width="11.9843137254902"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="40" width="15.6470588235294"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="40" width="13.2823529411765"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="40" width="12.843137254902"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="40" width="11.2156862745098"/>
-    <col collapsed="false" hidden="false" max="12" min="11" style="40" width="18.6745098039216"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="40" width="14.678431372549"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="40" width="12.7372549019608"/>
-    <col collapsed="false" hidden="false" max="16" min="15" style="40" width="36.8235294117647"/>
-    <col collapsed="false" hidden="false" max="1025" min="17" style="40" width="18.6745098039216"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="40" width="5.52941176470588"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="40" width="8.7764705882353"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="40" width="12.4549019607843"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="40" width="21.1764705882353"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="40" width="18.7529411764706"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="40" width="12.0313725490196"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="40" width="15.7098039215686"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="40" width="13.3372549019608"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="40" width="12.8941176470588"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="40" width="11.2588235294118"/>
+    <col collapsed="false" hidden="false" max="12" min="11" style="40" width="18.7529411764706"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="40" width="14.7450980392157"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="40" width="12.7921568627451"/>
+    <col collapsed="false" hidden="false" max="16" min="15" style="40" width="36.9725490196078"/>
+    <col collapsed="false" hidden="false" max="1025" min="17" style="40" width="18.7529411764706"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.2" outlineLevel="0" r="1" s="29">
@@ -23255,11 +23290,11 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="10" width="14.921568627451"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="28.0823529411765"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="18.356862745098"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="10" width="14.521568627451"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="10" width="7.28627450980392"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="10" width="14.9882352941176"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="28.1960784313725"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="10" width="18.4274509803922"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="10" width="14.5843137254902"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="10" width="7.31372549019608"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="true" ht="12.2" outlineLevel="0" r="1" s="9">
@@ -23441,29 +23476,29 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="53" width="19.7764705882353"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="53" width="10.6"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="54" width="10.0549019607843"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="53" width="13.5529411764706"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="53" width="15.2941176470588"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="53" width="24.6823529411765"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="53" width="14.3921568627451"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="53" width="11.2078431372549"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="53" width="12.2196078431373"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="53" width="10.7058823529412"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="53" width="14.3921568627451"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="53" width="12.8705882352941"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="53" width="9.70980392156863"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="53" width="10.7058823529412"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="53" width="9.1921568627451"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="53" width="12.8705882352941"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="53" width="13.0588235294118"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="53" width="9.85882352941177"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="53" width="10.8705882352941"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="53" width="9.36470588235294"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="53" width="13.0588235294118"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="55" width="13.8980392156863"/>
-    <col collapsed="false" hidden="false" max="1025" min="25" style="53" width="9.36470588235294"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="53" width="19.8549019607843"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="53" width="10.643137254902"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="54" width="10.0980392156863"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="53" width="13.6117647058824"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="53" width="15.3607843137255"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="53" width="24.7882352941176"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="53" width="14.4509803921569"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="53" width="11.2509803921569"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="53" width="12.2705882352941"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="53" width="10.7490196078431"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="53" width="14.4509803921569"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="53" width="12.921568627451"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="53" width="9.74509803921569"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="53" width="10.7490196078431"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="53" width="9.22745098039216"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="53" width="12.921568627451"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="53" width="13.1137254901961"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="53" width="9.89411764705882"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="53" width="10.9137254901961"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="53" width="9.4"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="53" width="13.1137254901961"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="55" width="13.9529411764706"/>
+    <col collapsed="false" hidden="false" max="1025" min="25" style="53" width="9.4"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="true" ht="12.2" outlineLevel="0" r="1" s="56">
@@ -23897,20 +23932,20 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="40" width="13.8313725490196"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="40" width="8.52549019607843"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="40" width="10.7921568627451"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="40" width="11.8666666666667"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="40" width="12.678431372549"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="40" width="14.2117647058824"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="40" width="12.9803921568627"/>
-    <col collapsed="false" hidden="false" max="12" min="9" style="40" width="10.556862745098"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="40" width="20.5098039215686"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="40" width="15.2941176470588"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="40" width="15.7058823529412"/>
-    <col collapsed="false" hidden="false" max="26" min="16" style="40" width="9.4"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="40" width="11.1372549019608"/>
-    <col collapsed="false" hidden="false" max="1025" min="28" style="40" width="7.28627450980392"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="40" width="13.8901960784314"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="40" width="8.56078431372549"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="40" width="10.8352941176471"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="40" width="11.9176470588235"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="40" width="12.7372549019608"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="40" width="14.2705882352941"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="40" width="13.0352941176471"/>
+    <col collapsed="false" hidden="false" max="12" min="9" style="40" width="10.6039215686275"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="40" width="20.5960784313725"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="40" width="15.3607843137255"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="40" width="15.7686274509804"/>
+    <col collapsed="false" hidden="false" max="26" min="16" style="40" width="9.43529411764706"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="40" width="11.1882352941176"/>
+    <col collapsed="false" hidden="false" max="1025" min="28" style="40" width="7.31372549019608"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="true" ht="12.2" outlineLevel="0" r="1" s="29">
@@ -24741,9 +24776,9 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="10" width="22.5607843137255"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="23.6117647058824"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="10" width="7.28627450980392"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="10" width="22.6509803921569"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="23.7058823529412"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="10" width="7.31372549019608"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="true" ht="12.2" outlineLevel="0" r="1" s="9">

</xml_diff>

<commit_message>
Got arimport test with priorities working
</commit_message>
<xml_diff>
--- a/bika/lims/setupdata/test/test.xlsx
+++ b/bika/lims/setupdata/test/test.xlsx
@@ -864,10 +864,10 @@
     <t>Normal</t>
   </si>
   <si>
-    <t>priority_norm.png</t>
-  </si>
-  <si>
-    <t>priority_norm_big.png</t>
+    <t>priority_normal.png</t>
+  </si>
+  <si>
+    <t>priority_normal_big.png</t>
   </si>
   <si>
     <t>High</t>
@@ -5263,7 +5263,7 @@
       </c>
       <c r="B1" s="2"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="18.85" outlineLevel="0" r="2" s="3">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="18.85" outlineLevel="0" r="2">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -21731,7 +21731,7 @@
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.5060728744939"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.6113360323887"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.2672064777328"/>
-    <col collapsed="false" hidden="false" max="12" min="11" style="0" width="8.5748987854251"/>
+    <col collapsed="false" hidden="false" max="12" min="10" style="0" width="8.5748987854251"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="0" width="11.7408906882591"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="10.1821862348178"/>
     <col collapsed="false" hidden="false" max="16" min="15" style="0" width="29.4372469635628"/>
@@ -26931,16 +26931,17 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="G7" activeCellId="0" pane="topLeft" sqref="G7"/>
+      <selection activeCell="G6" activeCellId="0" pane="topLeft" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.3"/>
   <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.5748987854251"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.93927125506073"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.1052631578947"/>
     <col collapsed="false" hidden="false" max="5" min="4" style="0" width="6.66396761133603"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.3117408906883"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.5546558704453"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.5101214574899"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="38" width="9.1417004048583"/>
   </cols>
   <sheetData>
@@ -27064,7 +27065,7 @@
         <v>231</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="7">
       <c r="A7" s="38" t="s">
         <v>232</v>
       </c>

</xml_diff>

<commit_message>
REmoved getStorageLocation indexes changed getStorageLocationTitle to getStorageLocation throughout Removed ClientStorageLocations Added getter/setter for SL in AR Removed StorageLocation from registry Removed transition URLs from inactive and cancel workflows Fixed update step
</commit_message>
<xml_diff>
--- a/bika/lims/setupdata/test/test.xlsx
+++ b/bika/lims/setupdata/test/test.xlsx
@@ -182,7 +182,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3551" uniqueCount="1396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3548" uniqueCount="1396">
   <si>
     <t>Instructions</t>
   </si>
@@ -4918,10 +4918,6 @@
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="13" numFmtId="164" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
       <protection hidden="false" locked="true"/>
@@ -4984,6 +4980,10 @@
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="13" numFmtId="164" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="13" numFmtId="164" xfId="0">
+      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="5" numFmtId="164" xfId="0">
@@ -5821,66 +5821,63 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:14"/>
+  <dimension ref="1:4"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="D14" activeCellId="0" pane="topLeft" sqref="D14"/>
+      <selection activeCell="C11" activeCellId="0" pane="topLeft" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.3"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5708502024291"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.06882591093117"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.48582995951417"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.69230769230769"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.8097165991903"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.86234817813765"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="9.37651821862348"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.995951417004"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.2753036437247"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="6.89878542510122"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="7.41295546558704"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="23.7368421052632"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.06882591093117"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.48582995951417"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.69230769230769"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.8097165991903"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.86234817813765"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.37651821862348"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.995951417004"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.2753036437247"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="6.89878542510122"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="7.41295546558704"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="23.7368421052632"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="9.1417004048583"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="1" s="5">
-      <c r="A1" s="5" t="s">
-        <v>275</v>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="true" ht="13.3" outlineLevel="0" r="1" s="5">
+      <c r="A1" s="65" t="s">
+        <v>135</v>
       </c>
       <c r="B1" s="65" t="s">
-        <v>135</v>
+        <v>384</v>
       </c>
       <c r="C1" s="65" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="D1" s="65" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="E1" s="65" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="F1" s="65" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="G1" s="65" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="H1" s="65" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="I1" s="65" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="J1" s="65" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="K1" s="65" t="s">
-        <v>392</v>
-      </c>
-      <c r="L1" s="65" t="s">
         <v>393</v>
       </c>
+      <c r="L1" s="65"/>
       <c r="M1" s="65"/>
       <c r="N1" s="65"/>
       <c r="O1" s="65"/>
@@ -5890,7 +5887,7 @@
       <c r="S1" s="65"/>
       <c r="T1" s="65"/>
       <c r="U1" s="65"/>
-      <c r="V1" s="65"/>
+      <c r="AMI1" s="0"/>
       <c r="AMJ1" s="0"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="16.9" outlineLevel="0" r="2" s="6">
@@ -5917,46 +5914,44 @@
       <c r="S2" s="65"/>
       <c r="T2" s="65"/>
       <c r="U2" s="65"/>
-      <c r="V2" s="65"/>
+      <c r="AMI2" s="0"/>
       <c r="AMJ2" s="0"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="3" s="5">
-      <c r="A3" s="5" t="s">
-        <v>275</v>
+      <c r="A3" s="65" t="s">
+        <v>135</v>
       </c>
       <c r="B3" s="65" t="s">
-        <v>135</v>
+        <v>384</v>
       </c>
       <c r="C3" s="65" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="D3" s="65" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="E3" s="65" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="F3" s="65" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="G3" s="65" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="H3" s="65" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="I3" s="65" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="J3" s="65" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="K3" s="65" t="s">
-        <v>392</v>
-      </c>
-      <c r="L3" s="65" t="s">
         <v>393</v>
       </c>
+      <c r="L3" s="65"/>
       <c r="M3" s="65"/>
       <c r="N3" s="65"/>
       <c r="O3" s="65"/>
@@ -5966,84 +5961,45 @@
       <c r="S3" s="65"/>
       <c r="T3" s="65"/>
       <c r="U3" s="65"/>
-      <c r="V3" s="65"/>
+      <c r="AMI3" s="0"/>
       <c r="AMJ3" s="0"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="4">
-      <c r="A4" s="66" t="s">
-        <v>247</v>
+      <c r="A4" s="65" t="s">
+        <v>395</v>
       </c>
       <c r="B4" s="65" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="C4" s="65" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="D4" s="65" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="E4" s="65" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="F4" s="65" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="G4" s="65" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="H4" s="65" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="I4" s="65" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="J4" s="65" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="K4" s="65" t="s">
-        <v>404</v>
-      </c>
-      <c r="L4" s="65" t="s">
         <v>405</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="5">
-      <c r="A5" s="66"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="6">
-      <c r="A6" s="66"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="7">
-      <c r="A7" s="66"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="8">
-      <c r="A8" s="66"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="9">
-      <c r="A9" s="66"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="10">
-      <c r="A10" s="66"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="11">
-      <c r="A11" s="66"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="12">
-      <c r="A12" s="66"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="13">
-      <c r="A13" s="66"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="14">
-      <c r="A14" s="66"/>
-    </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation allowBlank="false" error="Select a valid entry from the drop-down  list of all clients listed on the Clients sheet" errorTitle="Invalid entry" operator="equal" prompt="Select a Client if it is a specific client's private sampling point not available to others. Leave blank if it is a general sampling point that can be used by all clients.  The options on the drop-down list of all clients are maintained on the Clients sheet." promptTitle="Select a valid Client if required" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="A4:A14" type="list">
-      <formula1>Clients!$A$4:$A$181</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-  </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
@@ -6100,27 +6056,27 @@
       <c r="A2" s="7" t="s">
         <v>410</v>
       </c>
-      <c r="C2" s="67" t="s">
+      <c r="C2" s="66" t="s">
         <v>411</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="18.65" outlineLevel="0" r="3" s="68">
-      <c r="A3" s="68" t="s">
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="18.65" outlineLevel="0" r="3" s="67">
+      <c r="A3" s="67" t="s">
         <v>206</v>
       </c>
-      <c r="B3" s="68" t="s">
+      <c r="B3" s="67" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="68" t="s">
+      <c r="C3" s="67" t="s">
         <v>406</v>
       </c>
-      <c r="D3" s="68" t="s">
+      <c r="D3" s="67" t="s">
         <v>412</v>
       </c>
-      <c r="E3" s="68" t="s">
+      <c r="E3" s="67" t="s">
         <v>413</v>
       </c>
-      <c r="F3" s="68" t="s">
+      <c r="F3" s="67" t="s">
         <v>414</v>
       </c>
     </row>
@@ -6131,126 +6087,126 @@
       <c r="B4" s="3" t="s">
         <v>415</v>
       </c>
-      <c r="C4" s="69" t="s">
+      <c r="C4" s="68" t="s">
         <v>416</v>
       </c>
-      <c r="D4" s="70" t="s">
+      <c r="D4" s="69" t="s">
         <v>358</v>
       </c>
-      <c r="E4" s="71" t="n">
+      <c r="E4" s="70" t="n">
         <v>0</v>
       </c>
-      <c r="F4" s="70"/>
+      <c r="F4" s="69"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="5">
-      <c r="A5" s="72" t="s">
+      <c r="A5" s="71" t="s">
         <v>417</v>
       </c>
-      <c r="B5" s="72" t="s">
+      <c r="B5" s="71" t="s">
         <v>418</v>
       </c>
-      <c r="C5" s="69" t="s">
+      <c r="C5" s="68" t="s">
         <v>419</v>
       </c>
-      <c r="D5" s="73" t="s">
+      <c r="D5" s="72" t="s">
         <v>358</v>
       </c>
-      <c r="E5" s="71" t="n">
+      <c r="E5" s="70" t="n">
         <v>0</v>
       </c>
-      <c r="F5" s="70"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="6" s="71">
-      <c r="A6" s="72" t="s">
+      <c r="F5" s="69"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="6" s="70">
+      <c r="A6" s="71" t="s">
         <v>420</v>
       </c>
-      <c r="B6" s="72" t="s">
+      <c r="B6" s="71" t="s">
         <v>420</v>
       </c>
-      <c r="C6" s="69" t="s">
+      <c r="C6" s="68" t="s">
         <v>419</v>
       </c>
-      <c r="D6" s="74" t="s">
+      <c r="D6" s="73" t="s">
         <v>360</v>
       </c>
-      <c r="E6" s="71" t="n">
+      <c r="E6" s="70" t="n">
         <v>0</v>
       </c>
-      <c r="F6" s="75"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="7" s="71">
-      <c r="A7" s="72" t="s">
+      <c r="F6" s="74"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="7" s="70">
+      <c r="A7" s="71" t="s">
         <v>421</v>
       </c>
-      <c r="B7" s="72" t="s">
+      <c r="B7" s="71" t="s">
         <v>421</v>
       </c>
-      <c r="C7" s="69" t="s">
+      <c r="C7" s="68" t="s">
         <v>422</v>
       </c>
-      <c r="D7" s="74" t="s">
+      <c r="D7" s="73" t="s">
         <v>360</v>
       </c>
-      <c r="E7" s="71" t="n">
+      <c r="E7" s="70" t="n">
         <v>0</v>
       </c>
-      <c r="F7" s="75"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="8" s="71">
-      <c r="A8" s="72" t="s">
+      <c r="F7" s="74"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="8" s="70">
+      <c r="A8" s="71" t="s">
         <v>423</v>
       </c>
-      <c r="B8" s="72" t="s">
+      <c r="B8" s="71" t="s">
         <v>424</v>
       </c>
-      <c r="C8" s="69" t="s">
+      <c r="C8" s="68" t="s">
         <v>416</v>
       </c>
-      <c r="D8" s="74" t="s">
+      <c r="D8" s="73" t="s">
         <v>358</v>
       </c>
-      <c r="E8" s="71" t="n">
+      <c r="E8" s="70" t="n">
         <v>0</v>
       </c>
-      <c r="F8" s="75"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="9" s="71">
-      <c r="A9" s="72" t="s">
+      <c r="F8" s="74"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="9" s="70">
+      <c r="A9" s="71" t="s">
         <v>425</v>
       </c>
-      <c r="B9" s="72" t="s">
+      <c r="B9" s="71" t="s">
         <v>426</v>
       </c>
-      <c r="C9" s="69" t="s">
+      <c r="C9" s="68" t="s">
         <v>416</v>
       </c>
-      <c r="D9" s="74" t="s">
+      <c r="D9" s="73" t="s">
         <v>358</v>
       </c>
-      <c r="E9" s="71" t="n">
+      <c r="E9" s="70" t="n">
         <v>1</v>
       </c>
-      <c r="F9" s="75" t="s">
+      <c r="F9" s="74" t="s">
         <v>380</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="10">
-      <c r="A10" s="71" t="s">
+      <c r="A10" s="70" t="s">
         <v>427</v>
       </c>
-      <c r="B10" s="71" t="s">
+      <c r="B10" s="70" t="s">
         <v>369</v>
       </c>
-      <c r="C10" s="71" t="s">
+      <c r="C10" s="70" t="s">
         <v>428</v>
       </c>
-      <c r="D10" s="74" t="s">
+      <c r="D10" s="73" t="s">
         <v>368</v>
       </c>
-      <c r="E10" s="71" t="n">
+      <c r="E10" s="70" t="n">
         <v>0</v>
       </c>
-      <c r="F10" s="70"/>
+      <c r="F10" s="69"/>
     </row>
   </sheetData>
   <dataValidations count="3">
@@ -6446,31 +6402,31 @@
         <v>444</v>
       </c>
       <c r="C2" s="7"/>
-      <c r="F2" s="76"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="36.55" outlineLevel="0" r="3" s="77">
-      <c r="A3" s="77" t="s">
+      <c r="F2" s="75"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="36.55" outlineLevel="0" r="3" s="76">
+      <c r="A3" s="76" t="s">
         <v>206</v>
       </c>
-      <c r="B3" s="77" t="s">
+      <c r="B3" s="76" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="77" t="s">
+      <c r="C3" s="76" t="s">
         <v>445</v>
       </c>
-      <c r="D3" s="77" t="s">
+      <c r="D3" s="76" t="s">
         <v>441</v>
       </c>
-      <c r="E3" s="77" t="s">
+      <c r="E3" s="76" t="s">
         <v>446</v>
       </c>
-      <c r="F3" s="78" t="s">
+      <c r="F3" s="77" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="77" t="s">
+      <c r="G3" s="76" t="s">
         <v>447</v>
       </c>
-      <c r="H3" s="77" t="s">
+      <c r="H3" s="76" t="s">
         <v>448</v>
       </c>
     </row>
@@ -6481,22 +6437,22 @@
       <c r="B4" s="63" t="s">
         <v>450</v>
       </c>
-      <c r="C4" s="79" t="n">
+      <c r="C4" s="78" t="n">
         <v>10</v>
       </c>
       <c r="D4" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="E4" s="69" t="s">
+      <c r="E4" s="68" t="s">
         <v>430</v>
       </c>
       <c r="F4" s="63" t="s">
         <v>451</v>
       </c>
-      <c r="G4" s="80" t="s">
+      <c r="G4" s="79" t="s">
         <v>452</v>
       </c>
-      <c r="H4" s="80" t="s">
+      <c r="H4" s="79" t="s">
         <v>362</v>
       </c>
     </row>
@@ -6507,22 +6463,22 @@
       <c r="B5" s="63" t="s">
         <v>454</v>
       </c>
-      <c r="C5" s="79" t="n">
+      <c r="C5" s="78" t="n">
         <v>10</v>
       </c>
       <c r="D5" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="E5" s="69" t="s">
+      <c r="E5" s="68" t="s">
         <v>435</v>
       </c>
       <c r="F5" s="63" t="s">
         <v>455</v>
       </c>
-      <c r="G5" s="80" t="s">
+      <c r="G5" s="79" t="s">
         <v>452</v>
       </c>
-      <c r="H5" s="80" t="s">
+      <c r="H5" s="79" t="s">
         <v>362</v>
       </c>
     </row>
@@ -6533,22 +6489,22 @@
       <c r="B6" s="63" t="s">
         <v>457</v>
       </c>
-      <c r="C6" s="81" t="n">
+      <c r="C6" s="80" t="n">
         <v>10</v>
       </c>
       <c r="D6" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="E6" s="69" t="s">
+      <c r="E6" s="68" t="s">
         <v>435</v>
       </c>
       <c r="F6" s="63" t="s">
         <v>458</v>
       </c>
-      <c r="G6" s="80" t="s">
+      <c r="G6" s="79" t="s">
         <v>452</v>
       </c>
-      <c r="H6" s="69" t="s">
+      <c r="H6" s="68" t="s">
         <v>362</v>
       </c>
     </row>
@@ -6559,22 +6515,22 @@
       <c r="B7" s="63" t="s">
         <v>460</v>
       </c>
-      <c r="C7" s="81" t="n">
+      <c r="C7" s="80" t="n">
         <v>10</v>
       </c>
       <c r="D7" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="E7" s="69" t="s">
+      <c r="E7" s="68" t="s">
         <v>435</v>
       </c>
       <c r="F7" s="63" t="s">
         <v>461</v>
       </c>
-      <c r="G7" s="80" t="s">
+      <c r="G7" s="79" t="s">
         <v>452</v>
       </c>
-      <c r="H7" s="69" t="s">
+      <c r="H7" s="68" t="s">
         <v>362</v>
       </c>
     </row>
@@ -6585,22 +6541,22 @@
       <c r="B8" s="61" t="s">
         <v>462</v>
       </c>
-      <c r="C8" s="82" t="n">
+      <c r="C8" s="81" t="n">
         <v>10</v>
       </c>
       <c r="D8" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="E8" s="80" t="s">
+      <c r="E8" s="79" t="s">
         <v>432</v>
       </c>
       <c r="F8" s="61" t="s">
         <v>463</v>
       </c>
-      <c r="G8" s="80" t="s">
+      <c r="G8" s="79" t="s">
         <v>452</v>
       </c>
-      <c r="H8" s="80" t="s">
+      <c r="H8" s="79" t="s">
         <v>362</v>
       </c>
     </row>
@@ -6611,22 +6567,22 @@
       <c r="B9" s="32" t="s">
         <v>464</v>
       </c>
-      <c r="C9" s="81" t="n">
-        <v>10</v>
-      </c>
-      <c r="D9" s="66" t="n">
+      <c r="C9" s="80" t="n">
+        <v>10</v>
+      </c>
+      <c r="D9" s="82" t="n">
         <v>1</v>
       </c>
-      <c r="E9" s="69" t="s">
+      <c r="E9" s="68" t="s">
         <v>438</v>
       </c>
       <c r="F9" s="30" t="s">
         <v>465</v>
       </c>
-      <c r="G9" s="69" t="s">
+      <c r="G9" s="68" t="s">
         <v>466</v>
       </c>
-      <c r="H9" s="69" t="s">
+      <c r="H9" s="68" t="s">
         <v>358</v>
       </c>
     </row>
@@ -6637,22 +6593,22 @@
       <c r="B10" s="63" t="s">
         <v>468</v>
       </c>
-      <c r="C10" s="82" t="n">
+      <c r="C10" s="81" t="n">
         <v>10</v>
       </c>
       <c r="D10" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="E10" s="69" t="s">
+      <c r="E10" s="68" t="s">
         <v>433</v>
       </c>
       <c r="F10" s="63" t="s">
         <v>469</v>
       </c>
-      <c r="G10" s="80" t="s">
+      <c r="G10" s="79" t="s">
         <v>452</v>
       </c>
-      <c r="H10" s="80" t="s">
+      <c r="H10" s="79" t="s">
         <v>362</v>
       </c>
     </row>
@@ -6663,22 +6619,22 @@
       <c r="B11" s="61" t="s">
         <v>471</v>
       </c>
-      <c r="C11" s="82" t="n">
+      <c r="C11" s="81" t="n">
         <v>10</v>
       </c>
       <c r="D11" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="E11" s="80" t="s">
+      <c r="E11" s="79" t="s">
         <v>430</v>
       </c>
       <c r="F11" s="61" t="s">
         <v>472</v>
       </c>
-      <c r="G11" s="69" t="s">
+      <c r="G11" s="68" t="s">
         <v>452</v>
       </c>
-      <c r="H11" s="69" t="s">
+      <c r="H11" s="68" t="s">
         <v>362</v>
       </c>
     </row>
@@ -6689,22 +6645,22 @@
       <c r="B12" s="61" t="s">
         <v>474</v>
       </c>
-      <c r="C12" s="82" t="n">
+      <c r="C12" s="81" t="n">
         <v>10</v>
       </c>
       <c r="D12" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="E12" s="80" t="s">
+      <c r="E12" s="79" t="s">
         <v>433</v>
       </c>
       <c r="F12" s="61" t="s">
         <v>475</v>
       </c>
-      <c r="G12" s="80" t="s">
+      <c r="G12" s="79" t="s">
         <v>452</v>
       </c>
-      <c r="H12" s="69" t="s">
+      <c r="H12" s="68" t="s">
         <v>362</v>
       </c>
     </row>
@@ -6715,22 +6671,22 @@
       <c r="B13" s="32" t="s">
         <v>454</v>
       </c>
-      <c r="C13" s="81" t="n">
+      <c r="C13" s="80" t="n">
         <v>10</v>
       </c>
       <c r="D13" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="E13" s="69" t="s">
+      <c r="E13" s="68" t="s">
         <v>435</v>
       </c>
       <c r="F13" s="30" t="s">
         <v>477</v>
       </c>
-      <c r="G13" s="69" t="s">
+      <c r="G13" s="68" t="s">
         <v>452</v>
       </c>
-      <c r="H13" s="69" t="s">
+      <c r="H13" s="68" t="s">
         <v>362</v>
       </c>
     </row>
@@ -6741,22 +6697,22 @@
       <c r="B14" s="32" t="s">
         <v>479</v>
       </c>
-      <c r="C14" s="81" t="n">
+      <c r="C14" s="80" t="n">
         <v>10</v>
       </c>
       <c r="D14" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="E14" s="69" t="s">
+      <c r="E14" s="68" t="s">
         <v>435</v>
       </c>
       <c r="F14" s="30" t="s">
         <v>480</v>
       </c>
-      <c r="G14" s="69" t="s">
+      <c r="G14" s="68" t="s">
         <v>452</v>
       </c>
-      <c r="H14" s="69" t="s">
+      <c r="H14" s="68" t="s">
         <v>362</v>
       </c>
     </row>
@@ -6767,22 +6723,22 @@
       <c r="B15" s="32" t="s">
         <v>454</v>
       </c>
-      <c r="C15" s="81" t="n">
-        <v>10</v>
-      </c>
-      <c r="D15" s="66" t="n">
+      <c r="C15" s="80" t="n">
+        <v>10</v>
+      </c>
+      <c r="D15" s="82" t="n">
         <v>1</v>
       </c>
-      <c r="E15" s="69" t="s">
+      <c r="E15" s="68" t="s">
         <v>435</v>
       </c>
       <c r="F15" s="30" t="s">
         <v>482</v>
       </c>
-      <c r="G15" s="69" t="s">
+      <c r="G15" s="68" t="s">
         <v>452</v>
       </c>
-      <c r="H15" s="69" t="s">
+      <c r="H15" s="68" t="s">
         <v>362</v>
       </c>
     </row>
@@ -6909,7 +6865,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="4">
-      <c r="A4" s="66"/>
+      <c r="A4" s="82"/>
       <c r="B4" s="65" t="s">
         <v>491</v>
       </c>
@@ -6919,7 +6875,7 @@
       <c r="D4" s="29"/>
       <c r="E4" s="29"/>
       <c r="F4" s="29"/>
-      <c r="G4" s="66" t="n">
+      <c r="G4" s="82" t="n">
         <v>0</v>
       </c>
       <c r="H4" s="83" t="s">
@@ -6927,7 +6883,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="5">
-      <c r="A5" s="66"/>
+      <c r="A5" s="82"/>
       <c r="B5" s="65" t="s">
         <v>493</v>
       </c>
@@ -6937,13 +6893,13 @@
       <c r="D5" s="29"/>
       <c r="E5" s="29"/>
       <c r="F5" s="29"/>
-      <c r="G5" s="66" t="n">
+      <c r="G5" s="82" t="n">
         <v>0</v>
       </c>
       <c r="H5" s="83"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="6">
-      <c r="A6" s="66"/>
+      <c r="A6" s="82"/>
       <c r="B6" s="65" t="s">
         <v>495</v>
       </c>
@@ -6953,13 +6909,13 @@
       <c r="D6" s="29"/>
       <c r="E6" s="29"/>
       <c r="F6" s="29"/>
-      <c r="G6" s="66" t="n">
+      <c r="G6" s="82" t="n">
         <v>0</v>
       </c>
       <c r="H6" s="83"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="7">
-      <c r="A7" s="66"/>
+      <c r="A7" s="82"/>
       <c r="B7" s="65" t="s">
         <v>497</v>
       </c>
@@ -6968,13 +6924,13 @@
       </c>
       <c r="E7" s="29"/>
       <c r="F7" s="29"/>
-      <c r="G7" s="66" t="n">
+      <c r="G7" s="82" t="n">
         <v>0</v>
       </c>
       <c r="H7" s="83"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="8">
-      <c r="A8" s="66"/>
+      <c r="A8" s="82"/>
       <c r="B8" s="29" t="s">
         <v>499</v>
       </c>
@@ -6984,13 +6940,13 @@
       <c r="D8" s="29"/>
       <c r="E8" s="29"/>
       <c r="F8" s="29"/>
-      <c r="G8" s="66" t="n">
+      <c r="G8" s="82" t="n">
         <v>0</v>
       </c>
       <c r="H8" s="83"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="9">
-      <c r="A9" s="66"/>
+      <c r="A9" s="82"/>
       <c r="B9" s="29" t="s">
         <v>500</v>
       </c>
@@ -7000,46 +6956,46 @@
       <c r="D9" s="29"/>
       <c r="E9" s="29"/>
       <c r="F9" s="29"/>
-      <c r="G9" s="66" t="n">
+      <c r="G9" s="82" t="n">
         <v>0</v>
       </c>
       <c r="H9" s="83"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="10">
-      <c r="A10" s="66"/>
+      <c r="A10" s="82"/>
       <c r="B10" s="65" t="s">
         <v>501</v>
       </c>
       <c r="C10" s="65" t="s">
         <v>498</v>
       </c>
-      <c r="G10" s="66" t="n">
+      <c r="G10" s="82" t="n">
         <v>0</v>
       </c>
       <c r="H10" s="83"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="11">
-      <c r="A11" s="66"/>
+      <c r="A11" s="82"/>
       <c r="B11" s="65" t="s">
         <v>502</v>
       </c>
       <c r="C11" s="65" t="s">
         <v>498</v>
       </c>
-      <c r="G11" s="66" t="n">
+      <c r="G11" s="82" t="n">
         <v>0</v>
       </c>
       <c r="H11" s="83"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="12">
-      <c r="A12" s="66"/>
+      <c r="A12" s="82"/>
       <c r="B12" s="65" t="s">
         <v>503</v>
       </c>
       <c r="C12" s="65" t="s">
         <v>504</v>
       </c>
-      <c r="G12" s="66" t="n">
+      <c r="G12" s="82" t="n">
         <v>0</v>
       </c>
       <c r="H12" s="83" t="s">
@@ -7047,27 +7003,27 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="13">
-      <c r="A13" s="66"/>
+      <c r="A13" s="82"/>
       <c r="B13" s="65" t="s">
         <v>505</v>
       </c>
       <c r="C13" s="65" t="s">
         <v>506</v>
       </c>
-      <c r="G13" s="66" t="n">
+      <c r="G13" s="82" t="n">
         <v>0</v>
       </c>
       <c r="H13" s="83"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="14">
-      <c r="A14" s="66"/>
+      <c r="A14" s="82"/>
       <c r="B14" s="65" t="s">
         <v>507</v>
       </c>
       <c r="C14" s="65" t="s">
         <v>508</v>
       </c>
-      <c r="G14" s="66" t="n">
+      <c r="G14" s="82" t="n">
         <v>0</v>
       </c>
       <c r="H14" s="83"/>
@@ -12448,77 +12404,77 @@
       <c r="AMI2" s="48"/>
       <c r="AMJ2" s="48"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="35.05" outlineLevel="0" r="3" s="68">
-      <c r="A3" s="68" t="s">
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="35.05" outlineLevel="0" r="3" s="67">
+      <c r="A3" s="67" t="s">
         <v>206</v>
       </c>
-      <c r="B3" s="68" t="s">
+      <c r="B3" s="67" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="68" t="s">
+      <c r="C3" s="67" t="s">
         <v>793</v>
       </c>
-      <c r="D3" s="68" t="s">
+      <c r="D3" s="67" t="s">
         <v>831</v>
       </c>
-      <c r="E3" s="68" t="s">
+      <c r="E3" s="67" t="s">
         <v>832</v>
       </c>
-      <c r="F3" s="68" t="s">
+      <c r="F3" s="67" t="s">
         <v>833</v>
       </c>
-      <c r="G3" s="77" t="s">
+      <c r="G3" s="76" t="s">
         <v>834</v>
       </c>
-      <c r="H3" s="68" t="s">
+      <c r="H3" s="67" t="s">
         <v>835</v>
       </c>
-      <c r="I3" s="68" t="s">
+      <c r="I3" s="67" t="s">
         <v>797</v>
       </c>
-      <c r="J3" s="68" t="s">
+      <c r="J3" s="67" t="s">
         <v>816</v>
       </c>
-      <c r="K3" s="68" t="s">
+      <c r="K3" s="67" t="s">
         <v>836</v>
       </c>
-      <c r="L3" s="68" t="s">
+      <c r="L3" s="67" t="s">
         <v>837</v>
       </c>
-      <c r="M3" s="68" t="s">
+      <c r="M3" s="67" t="s">
         <v>838</v>
       </c>
-      <c r="N3" s="68" t="s">
+      <c r="N3" s="67" t="s">
         <v>820</v>
       </c>
-      <c r="O3" s="68" t="s">
+      <c r="O3" s="67" t="s">
         <v>839</v>
       </c>
-      <c r="P3" s="68" t="s">
+      <c r="P3" s="67" t="s">
         <v>840</v>
       </c>
-      <c r="Q3" s="68" t="s">
+      <c r="Q3" s="67" t="s">
         <v>823</v>
       </c>
-      <c r="R3" s="68" t="s">
+      <c r="R3" s="67" t="s">
         <v>700</v>
       </c>
-      <c r="S3" s="68" t="s">
+      <c r="S3" s="67" t="s">
         <v>841</v>
       </c>
-      <c r="T3" s="77" t="s">
+      <c r="T3" s="76" t="s">
         <v>842</v>
       </c>
-      <c r="U3" s="68" t="s">
+      <c r="U3" s="67" t="s">
         <v>826</v>
       </c>
-      <c r="V3" s="68" t="s">
+      <c r="V3" s="67" t="s">
         <v>827</v>
       </c>
-      <c r="W3" s="68" t="s">
+      <c r="W3" s="67" t="s">
         <v>843</v>
       </c>
-      <c r="X3" s="68" t="s">
+      <c r="X3" s="67" t="s">
         <v>844</v>
       </c>
       <c r="AMH3" s="3"/>
@@ -12580,10 +12536,10 @@
       <c r="T4" s="121" t="n">
         <v>10</v>
       </c>
-      <c r="U4" s="80" t="n">
+      <c r="U4" s="79" t="n">
         <v>0</v>
       </c>
-      <c r="V4" s="80" t="n">
+      <c r="V4" s="79" t="n">
         <v>0</v>
       </c>
       <c r="W4" s="120"/>
@@ -12642,10 +12598,10 @@
       <c r="T5" s="121" t="n">
         <v>10</v>
       </c>
-      <c r="U5" s="80" t="n">
+      <c r="U5" s="79" t="n">
         <v>0</v>
       </c>
-      <c r="V5" s="80" t="n">
+      <c r="V5" s="79" t="n">
         <v>0</v>
       </c>
       <c r="W5" s="120"/>
@@ -12703,10 +12659,10 @@
       <c r="T6" s="121" t="n">
         <v>10</v>
       </c>
-      <c r="U6" s="80" t="n">
+      <c r="U6" s="79" t="n">
         <v>0</v>
       </c>
-      <c r="V6" s="80" t="n">
+      <c r="V6" s="79" t="n">
         <v>0</v>
       </c>
       <c r="W6" s="120"/>
@@ -12764,10 +12720,10 @@
       <c r="T7" s="121" t="n">
         <v>10</v>
       </c>
-      <c r="U7" s="80" t="n">
+      <c r="U7" s="79" t="n">
         <v>0</v>
       </c>
-      <c r="V7" s="80" t="n">
+      <c r="V7" s="79" t="n">
         <v>0</v>
       </c>
       <c r="W7" s="120"/>
@@ -12825,10 +12781,10 @@
       <c r="T8" s="121" t="n">
         <v>10</v>
       </c>
-      <c r="U8" s="80" t="n">
+      <c r="U8" s="79" t="n">
         <v>1</v>
       </c>
-      <c r="V8" s="80" t="n">
+      <c r="V8" s="79" t="n">
         <v>0</v>
       </c>
       <c r="W8" s="120"/>
@@ -12886,10 +12842,10 @@
       <c r="T9" s="121" t="n">
         <v>10</v>
       </c>
-      <c r="U9" s="80" t="n">
+      <c r="U9" s="79" t="n">
         <v>0</v>
       </c>
-      <c r="V9" s="80" t="n">
+      <c r="V9" s="79" t="n">
         <v>0</v>
       </c>
       <c r="W9" s="120"/>
@@ -12947,10 +12903,10 @@
       <c r="T10" s="121" t="n">
         <v>10</v>
       </c>
-      <c r="U10" s="80" t="n">
+      <c r="U10" s="79" t="n">
         <v>0</v>
       </c>
-      <c r="V10" s="80" t="n">
+      <c r="V10" s="79" t="n">
         <v>0</v>
       </c>
       <c r="W10" s="120"/>
@@ -13008,10 +12964,10 @@
       <c r="T11" s="121" t="n">
         <v>10</v>
       </c>
-      <c r="U11" s="80" t="n">
+      <c r="U11" s="79" t="n">
         <v>0</v>
       </c>
-      <c r="V11" s="80" t="n">
+      <c r="V11" s="79" t="n">
         <v>0</v>
       </c>
       <c r="W11" s="120"/>
@@ -13069,10 +13025,10 @@
       <c r="T12" s="121" t="n">
         <v>10</v>
       </c>
-      <c r="U12" s="80" t="n">
+      <c r="U12" s="79" t="n">
         <v>0</v>
       </c>
-      <c r="V12" s="80" t="n">
+      <c r="V12" s="79" t="n">
         <v>0</v>
       </c>
       <c r="W12" s="120"/>
@@ -13135,10 +13091,10 @@
       <c r="T13" s="121" t="n">
         <v>10</v>
       </c>
-      <c r="U13" s="80" t="n">
+      <c r="U13" s="79" t="n">
         <v>1</v>
       </c>
-      <c r="V13" s="80" t="n">
+      <c r="V13" s="79" t="n">
         <v>0</v>
       </c>
       <c r="W13" s="120"/>
@@ -13196,10 +13152,10 @@
       <c r="T14" s="121" t="n">
         <v>10</v>
       </c>
-      <c r="U14" s="80" t="n">
+      <c r="U14" s="79" t="n">
         <v>0</v>
       </c>
-      <c r="V14" s="80" t="n">
+      <c r="V14" s="79" t="n">
         <v>0</v>
       </c>
       <c r="W14" s="120"/>
@@ -13255,10 +13211,10 @@
       <c r="T15" s="121" t="n">
         <v>10</v>
       </c>
-      <c r="U15" s="80" t="n">
+      <c r="U15" s="79" t="n">
         <v>0</v>
       </c>
-      <c r="V15" s="80" t="n">
+      <c r="V15" s="79" t="n">
         <v>0</v>
       </c>
       <c r="W15" s="120"/>
@@ -13316,10 +13272,10 @@
       <c r="T16" s="121" t="n">
         <v>10</v>
       </c>
-      <c r="U16" s="80" t="n">
+      <c r="U16" s="79" t="n">
         <v>0</v>
       </c>
-      <c r="V16" s="80" t="n">
+      <c r="V16" s="79" t="n">
         <v>0</v>
       </c>
       <c r="W16" s="120"/>
@@ -13377,10 +13333,10 @@
       <c r="T17" s="121" t="n">
         <v>10</v>
       </c>
-      <c r="U17" s="80" t="n">
+      <c r="U17" s="79" t="n">
         <v>0</v>
       </c>
-      <c r="V17" s="80" t="n">
+      <c r="V17" s="79" t="n">
         <v>0</v>
       </c>
       <c r="W17" s="120"/>
@@ -13440,10 +13396,10 @@
       <c r="T18" s="121" t="n">
         <v>10</v>
       </c>
-      <c r="U18" s="80" t="n">
+      <c r="U18" s="79" t="n">
         <v>1</v>
       </c>
-      <c r="V18" s="80" t="n">
+      <c r="V18" s="79" t="n">
         <v>0</v>
       </c>
       <c r="W18" s="120"/>
@@ -13501,10 +13457,10 @@
       <c r="T19" s="121" t="n">
         <v>10</v>
       </c>
-      <c r="U19" s="80" t="n">
+      <c r="U19" s="79" t="n">
         <v>1</v>
       </c>
-      <c r="V19" s="80" t="n">
+      <c r="V19" s="79" t="n">
         <v>0</v>
       </c>
       <c r="W19" s="120"/>
@@ -13567,10 +13523,10 @@
       <c r="T20" s="121" t="n">
         <v>10</v>
       </c>
-      <c r="U20" s="80" t="n">
+      <c r="U20" s="79" t="n">
         <v>0</v>
       </c>
-      <c r="V20" s="80" t="n">
+      <c r="V20" s="79" t="n">
         <v>0</v>
       </c>
       <c r="W20" s="120"/>
@@ -13629,10 +13585,10 @@
       <c r="T21" s="121" t="n">
         <v>10</v>
       </c>
-      <c r="U21" s="80" t="n">
+      <c r="U21" s="79" t="n">
         <v>0</v>
       </c>
-      <c r="V21" s="80" t="n">
+      <c r="V21" s="79" t="n">
         <v>0</v>
       </c>
       <c r="W21" s="120"/>
@@ -13691,10 +13647,10 @@
       <c r="T22" s="121" t="n">
         <v>10</v>
       </c>
-      <c r="U22" s="80" t="n">
+      <c r="U22" s="79" t="n">
         <v>1</v>
       </c>
-      <c r="V22" s="80" t="n">
+      <c r="V22" s="79" t="n">
         <v>0</v>
       </c>
       <c r="W22" s="120"/>
@@ -13753,10 +13709,10 @@
       <c r="T23" s="121" t="n">
         <v>10</v>
       </c>
-      <c r="U23" s="80" t="n">
+      <c r="U23" s="79" t="n">
         <v>0</v>
       </c>
-      <c r="V23" s="80" t="n">
+      <c r="V23" s="79" t="n">
         <v>0</v>
       </c>
       <c r="W23" s="120"/>
@@ -13815,10 +13771,10 @@
       <c r="T24" s="121" t="n">
         <v>10</v>
       </c>
-      <c r="U24" s="80" t="n">
+      <c r="U24" s="79" t="n">
         <v>0</v>
       </c>
-      <c r="V24" s="80" t="n">
+      <c r="V24" s="79" t="n">
         <v>0</v>
       </c>
       <c r="W24" s="120"/>
@@ -13877,10 +13833,10 @@
       <c r="T25" s="121" t="n">
         <v>10</v>
       </c>
-      <c r="U25" s="80" t="n">
+      <c r="U25" s="79" t="n">
         <v>1</v>
       </c>
-      <c r="V25" s="80" t="n">
+      <c r="V25" s="79" t="n">
         <v>0</v>
       </c>
       <c r="W25" s="120"/>
@@ -13939,10 +13895,10 @@
       <c r="T26" s="121" t="n">
         <v>10</v>
       </c>
-      <c r="U26" s="80" t="n">
+      <c r="U26" s="79" t="n">
         <v>0</v>
       </c>
-      <c r="V26" s="80" t="n">
+      <c r="V26" s="79" t="n">
         <v>0</v>
       </c>
       <c r="W26" s="120"/>
@@ -14001,10 +13957,10 @@
       <c r="T27" s="121" t="n">
         <v>10</v>
       </c>
-      <c r="U27" s="80" t="n">
+      <c r="U27" s="79" t="n">
         <v>1</v>
       </c>
-      <c r="V27" s="80" t="n">
+      <c r="V27" s="79" t="n">
         <v>0</v>
       </c>
       <c r="W27" s="120"/>
@@ -14219,134 +14175,134 @@
       <c r="AMJ3" s="2"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="4">
-      <c r="A4" s="69" t="s">
+      <c r="A4" s="68" t="s">
         <v>887</v>
       </c>
       <c r="B4" s="32" t="s">
         <v>909</v>
       </c>
-      <c r="C4" s="81" t="n">
+      <c r="C4" s="80" t="n">
         <v>0</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="5">
-      <c r="A5" s="69" t="s">
+      <c r="A5" s="68" t="s">
         <v>887</v>
       </c>
       <c r="B5" s="32" t="s">
         <v>910</v>
       </c>
-      <c r="C5" s="81" t="n">
+      <c r="C5" s="80" t="n">
         <v>1</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="6">
-      <c r="A6" s="69" t="s">
+      <c r="A6" s="68" t="s">
         <v>887</v>
       </c>
       <c r="B6" s="32" t="s">
         <v>911</v>
       </c>
-      <c r="C6" s="81" t="n">
+      <c r="C6" s="80" t="n">
         <v>2</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="7">
-      <c r="A7" s="69" t="s">
+      <c r="A7" s="68" t="s">
         <v>890</v>
       </c>
       <c r="B7" s="32" t="s">
         <v>909</v>
       </c>
-      <c r="C7" s="81" t="n">
+      <c r="C7" s="80" t="n">
         <v>0</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="8">
-      <c r="A8" s="69" t="s">
+      <c r="A8" s="68" t="s">
         <v>890</v>
       </c>
       <c r="B8" s="32" t="s">
         <v>910</v>
       </c>
-      <c r="C8" s="81" t="n">
+      <c r="C8" s="80" t="n">
         <v>1</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="9">
-      <c r="A9" s="69" t="s">
+      <c r="A9" s="68" t="s">
         <v>890</v>
       </c>
       <c r="B9" s="32" t="s">
         <v>911</v>
       </c>
-      <c r="C9" s="81" t="n">
+      <c r="C9" s="80" t="n">
         <v>2</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="10">
-      <c r="A10" s="69" t="s">
+      <c r="A10" s="68" t="s">
         <v>892</v>
       </c>
       <c r="B10" s="32" t="s">
         <v>909</v>
       </c>
-      <c r="C10" s="81" t="n">
+      <c r="C10" s="80" t="n">
         <v>0</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="11">
-      <c r="A11" s="69" t="s">
+      <c r="A11" s="68" t="s">
         <v>892</v>
       </c>
       <c r="B11" s="32" t="s">
         <v>910</v>
       </c>
-      <c r="C11" s="81" t="n">
+      <c r="C11" s="80" t="n">
         <v>1</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="12">
-      <c r="A12" s="69" t="s">
+      <c r="A12" s="68" t="s">
         <v>892</v>
       </c>
       <c r="B12" s="32" t="s">
         <v>911</v>
       </c>
-      <c r="C12" s="81" t="n">
+      <c r="C12" s="80" t="n">
         <v>2</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="13">
-      <c r="A13" s="69" t="s">
+      <c r="A13" s="68" t="s">
         <v>893</v>
       </c>
       <c r="B13" s="32" t="s">
         <v>909</v>
       </c>
-      <c r="C13" s="81" t="n">
+      <c r="C13" s="80" t="n">
         <v>0</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="14">
-      <c r="A14" s="69" t="s">
+      <c r="A14" s="68" t="s">
         <v>893</v>
       </c>
       <c r="B14" s="32" t="s">
         <v>910</v>
       </c>
-      <c r="C14" s="81" t="n">
+      <c r="C14" s="80" t="n">
         <v>1</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="15">
-      <c r="A15" s="69" t="s">
+      <c r="A15" s="68" t="s">
         <v>893</v>
       </c>
       <c r="B15" s="32" t="s">
         <v>911</v>
       </c>
-      <c r="C15" s="81" t="n">
+      <c r="C15" s="80" t="n">
         <v>2</v>
       </c>
     </row>
@@ -14413,27 +14369,27 @@
       <c r="A2" s="7" t="s">
         <v>915</v>
       </c>
-      <c r="B2" s="76"/>
+      <c r="B2" s="75"/>
       <c r="C2" s="12"/>
-      <c r="D2" s="76"/>
+      <c r="D2" s="75"/>
       <c r="AMJ2" s="48"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="31.3" outlineLevel="0" r="3" s="6">
       <c r="A3" s="6" t="s">
         <v>916</v>
       </c>
-      <c r="B3" s="78" t="s">
+      <c r="B3" s="77" t="s">
         <v>917</v>
       </c>
-      <c r="C3" s="78" t="s">
+      <c r="C3" s="77" t="s">
         <v>918</v>
       </c>
-      <c r="D3" s="78" t="s">
+      <c r="D3" s="77" t="s">
         <v>919</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="4">
-      <c r="A4" s="69" t="s">
+      <c r="A4" s="68" t="s">
         <v>845</v>
       </c>
       <c r="B4" s="19" t="n">
@@ -14447,7 +14403,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="5">
-      <c r="A5" s="69" t="s">
+      <c r="A5" s="68" t="s">
         <v>845</v>
       </c>
       <c r="B5" s="19" t="n">
@@ -14461,7 +14417,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="6">
-      <c r="A6" s="69" t="s">
+      <c r="A6" s="68" t="s">
         <v>845</v>
       </c>
       <c r="B6" s="19" t="n">
@@ -14475,7 +14431,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="7">
-      <c r="A7" s="69" t="s">
+      <c r="A7" s="68" t="s">
         <v>845</v>
       </c>
       <c r="B7" s="19" t="n">
@@ -14489,7 +14445,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="8">
-      <c r="A8" s="69" t="s">
+      <c r="A8" s="68" t="s">
         <v>845</v>
       </c>
       <c r="B8" s="19" t="s">
@@ -14503,7 +14459,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="9">
-      <c r="A9" s="69" t="s">
+      <c r="A9" s="68" t="s">
         <v>850</v>
       </c>
       <c r="B9" s="19" t="n">
@@ -14517,7 +14473,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="10">
-      <c r="A10" s="69" t="s">
+      <c r="A10" s="68" t="s">
         <v>850</v>
       </c>
       <c r="B10" s="19" t="n">
@@ -14531,7 +14487,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="11">
-      <c r="A11" s="69" t="s">
+      <c r="A11" s="68" t="s">
         <v>850</v>
       </c>
       <c r="B11" s="19" t="n">
@@ -14545,7 +14501,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="12">
-      <c r="A12" s="69" t="s">
+      <c r="A12" s="68" t="s">
         <v>850</v>
       </c>
       <c r="B12" s="19" t="n">
@@ -14559,7 +14515,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="13">
-      <c r="A13" s="69" t="s">
+      <c r="A13" s="68" t="s">
         <v>850</v>
       </c>
       <c r="B13" s="19" t="s">
@@ -14573,7 +14529,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="14">
-      <c r="A14" s="69" t="s">
+      <c r="A14" s="68" t="s">
         <v>853</v>
       </c>
       <c r="B14" s="19" t="n">
@@ -14587,7 +14543,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="15">
-      <c r="A15" s="69" t="s">
+      <c r="A15" s="68" t="s">
         <v>853</v>
       </c>
       <c r="B15" s="19" t="n">
@@ -14601,7 +14557,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="16">
-      <c r="A16" s="69" t="s">
+      <c r="A16" s="68" t="s">
         <v>853</v>
       </c>
       <c r="B16" s="19" t="n">
@@ -14615,7 +14571,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="17">
-      <c r="A17" s="69" t="s">
+      <c r="A17" s="68" t="s">
         <v>853</v>
       </c>
       <c r="B17" s="19" t="n">
@@ -14629,7 +14585,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="18">
-      <c r="A18" s="69" t="s">
+      <c r="A18" s="68" t="s">
         <v>853</v>
       </c>
       <c r="B18" s="19" t="s">
@@ -14643,7 +14599,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="19">
-      <c r="A19" s="69" t="s">
+      <c r="A19" s="68" t="s">
         <v>857</v>
       </c>
       <c r="B19" s="19" t="n">
@@ -14657,7 +14613,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="20">
-      <c r="A20" s="69" t="s">
+      <c r="A20" s="68" t="s">
         <v>857</v>
       </c>
       <c r="B20" s="19" t="n">
@@ -14671,7 +14627,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="21">
-      <c r="A21" s="69" t="s">
+      <c r="A21" s="68" t="s">
         <v>857</v>
       </c>
       <c r="B21" s="19" t="n">
@@ -14685,7 +14641,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="22">
-      <c r="A22" s="69" t="s">
+      <c r="A22" s="68" t="s">
         <v>857</v>
       </c>
       <c r="B22" s="19" t="n">
@@ -14699,7 +14655,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="23">
-      <c r="A23" s="69" t="s">
+      <c r="A23" s="68" t="s">
         <v>857</v>
       </c>
       <c r="B23" s="19" t="s">
@@ -14713,7 +14669,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="24">
-      <c r="A24" s="69" t="s">
+      <c r="A24" s="68" t="s">
         <v>858</v>
       </c>
       <c r="B24" s="19" t="n">
@@ -14727,7 +14683,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="25">
-      <c r="A25" s="69" t="s">
+      <c r="A25" s="68" t="s">
         <v>858</v>
       </c>
       <c r="B25" s="19" t="n">
@@ -14741,7 +14697,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="26">
-      <c r="A26" s="69" t="s">
+      <c r="A26" s="68" t="s">
         <v>858</v>
       </c>
       <c r="B26" s="19" t="n">
@@ -14755,7 +14711,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="27">
-      <c r="A27" s="69" t="s">
+      <c r="A27" s="68" t="s">
         <v>858</v>
       </c>
       <c r="B27" s="19" t="n">
@@ -14769,7 +14725,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="28">
-      <c r="A28" s="69" t="s">
+      <c r="A28" s="68" t="s">
         <v>858</v>
       </c>
       <c r="B28" s="19" t="s">
@@ -14783,7 +14739,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="29">
-      <c r="A29" s="69" t="s">
+      <c r="A29" s="68" t="s">
         <v>861</v>
       </c>
       <c r="B29" s="19" t="n">
@@ -14797,7 +14753,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="30">
-      <c r="A30" s="69" t="s">
+      <c r="A30" s="68" t="s">
         <v>861</v>
       </c>
       <c r="B30" s="19" t="n">
@@ -14811,7 +14767,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="31">
-      <c r="A31" s="69" t="s">
+      <c r="A31" s="68" t="s">
         <v>861</v>
       </c>
       <c r="B31" s="19" t="n">
@@ -14825,7 +14781,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="32">
-      <c r="A32" s="69" t="s">
+      <c r="A32" s="68" t="s">
         <v>861</v>
       </c>
       <c r="B32" s="19" t="n">
@@ -14839,7 +14795,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="33">
-      <c r="A33" s="69" t="s">
+      <c r="A33" s="68" t="s">
         <v>861</v>
       </c>
       <c r="B33" s="19" t="s">
@@ -14853,7 +14809,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="34">
-      <c r="A34" s="69" t="s">
+      <c r="A34" s="68" t="s">
         <v>863</v>
       </c>
       <c r="B34" s="19" t="n">
@@ -14867,7 +14823,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="35">
-      <c r="A35" s="69" t="s">
+      <c r="A35" s="68" t="s">
         <v>863</v>
       </c>
       <c r="B35" s="19" t="n">
@@ -14881,7 +14837,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="36">
-      <c r="A36" s="69" t="s">
+      <c r="A36" s="68" t="s">
         <v>863</v>
       </c>
       <c r="B36" s="19" t="n">
@@ -14895,7 +14851,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="37">
-      <c r="A37" s="69" t="s">
+      <c r="A37" s="68" t="s">
         <v>863</v>
       </c>
       <c r="B37" s="19" t="n">
@@ -14909,7 +14865,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="38">
-      <c r="A38" s="69" t="s">
+      <c r="A38" s="68" t="s">
         <v>863</v>
       </c>
       <c r="B38" s="19" t="s">
@@ -14923,7 +14879,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="39">
-      <c r="A39" s="69" t="s">
+      <c r="A39" s="68" t="s">
         <v>865</v>
       </c>
       <c r="B39" s="19" t="n">
@@ -14937,7 +14893,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="40">
-      <c r="A40" s="69" t="s">
+      <c r="A40" s="68" t="s">
         <v>865</v>
       </c>
       <c r="B40" s="19" t="n">
@@ -14951,7 +14907,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="41">
-      <c r="A41" s="69" t="s">
+      <c r="A41" s="68" t="s">
         <v>865</v>
       </c>
       <c r="B41" s="19" t="n">
@@ -14965,7 +14921,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="42">
-      <c r="A42" s="69" t="s">
+      <c r="A42" s="68" t="s">
         <v>865</v>
       </c>
       <c r="B42" s="19" t="n">
@@ -14979,7 +14935,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="43">
-      <c r="A43" s="69" t="s">
+      <c r="A43" s="68" t="s">
         <v>865</v>
       </c>
       <c r="B43" s="19" t="s">
@@ -14993,7 +14949,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="44">
-      <c r="A44" s="69" t="s">
+      <c r="A44" s="68" t="s">
         <v>867</v>
       </c>
       <c r="B44" s="19" t="n">
@@ -15007,7 +14963,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="45">
-      <c r="A45" s="69" t="s">
+      <c r="A45" s="68" t="s">
         <v>867</v>
       </c>
       <c r="B45" s="19" t="n">
@@ -15021,7 +14977,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="46">
-      <c r="A46" s="69" t="s">
+      <c r="A46" s="68" t="s">
         <v>867</v>
       </c>
       <c r="B46" s="19" t="n">
@@ -15035,7 +14991,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="47">
-      <c r="A47" s="69" t="s">
+      <c r="A47" s="68" t="s">
         <v>867</v>
       </c>
       <c r="B47" s="19" t="n">
@@ -15049,7 +15005,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="48">
-      <c r="A48" s="69" t="s">
+      <c r="A48" s="68" t="s">
         <v>867</v>
       </c>
       <c r="B48" s="19" t="s">
@@ -15063,7 +15019,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="49">
-      <c r="A49" s="69" t="s">
+      <c r="A49" s="68" t="s">
         <v>869</v>
       </c>
       <c r="B49" s="19" t="n">
@@ -15077,7 +15033,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="50">
-      <c r="A50" s="69" t="s">
+      <c r="A50" s="68" t="s">
         <v>869</v>
       </c>
       <c r="B50" s="19" t="n">
@@ -15091,7 +15047,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="51">
-      <c r="A51" s="69" t="s">
+      <c r="A51" s="68" t="s">
         <v>869</v>
       </c>
       <c r="B51" s="19" t="n">
@@ -15105,7 +15061,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="52">
-      <c r="A52" s="69" t="s">
+      <c r="A52" s="68" t="s">
         <v>869</v>
       </c>
       <c r="B52" s="19" t="n">
@@ -15119,7 +15075,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="53">
-      <c r="A53" s="69" t="s">
+      <c r="A53" s="68" t="s">
         <v>869</v>
       </c>
       <c r="B53" s="19" t="s">
@@ -15133,7 +15089,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="54">
-      <c r="A54" s="69" t="s">
+      <c r="A54" s="68" t="s">
         <v>873</v>
       </c>
       <c r="B54" s="19" t="n">
@@ -15147,7 +15103,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="55">
-      <c r="A55" s="69" t="s">
+      <c r="A55" s="68" t="s">
         <v>873</v>
       </c>
       <c r="B55" s="19" t="n">
@@ -15161,7 +15117,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="56">
-      <c r="A56" s="69" t="s">
+      <c r="A56" s="68" t="s">
         <v>873</v>
       </c>
       <c r="B56" s="19" t="n">
@@ -15175,7 +15131,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="57">
-      <c r="A57" s="69" t="s">
+      <c r="A57" s="68" t="s">
         <v>873</v>
       </c>
       <c r="B57" s="19" t="n">
@@ -15189,7 +15145,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="58">
-      <c r="A58" s="69" t="s">
+      <c r="A58" s="68" t="s">
         <v>873</v>
       </c>
       <c r="B58" s="19" t="s">
@@ -15203,7 +15159,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="59">
-      <c r="A59" s="69" t="s">
+      <c r="A59" s="68" t="s">
         <v>875</v>
       </c>
       <c r="B59" s="19" t="n">
@@ -15217,7 +15173,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="60">
-      <c r="A60" s="69" t="s">
+      <c r="A60" s="68" t="s">
         <v>875</v>
       </c>
       <c r="B60" s="19" t="n">
@@ -15231,7 +15187,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="61">
-      <c r="A61" s="69" t="s">
+      <c r="A61" s="68" t="s">
         <v>875</v>
       </c>
       <c r="B61" s="19" t="n">
@@ -15245,7 +15201,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="62">
-      <c r="A62" s="69" t="s">
+      <c r="A62" s="68" t="s">
         <v>875</v>
       </c>
       <c r="B62" s="19" t="n">
@@ -15259,7 +15215,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="63">
-      <c r="A63" s="69" t="s">
+      <c r="A63" s="68" t="s">
         <v>875</v>
       </c>
       <c r="B63" s="19" t="s">
@@ -15273,7 +15229,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="64">
-      <c r="A64" s="69" t="s">
+      <c r="A64" s="68" t="s">
         <v>877</v>
       </c>
       <c r="B64" s="19" t="n">
@@ -15287,7 +15243,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="65">
-      <c r="A65" s="69" t="s">
+      <c r="A65" s="68" t="s">
         <v>877</v>
       </c>
       <c r="B65" s="19" t="n">
@@ -15301,7 +15257,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="66">
-      <c r="A66" s="69" t="s">
+      <c r="A66" s="68" t="s">
         <v>877</v>
       </c>
       <c r="B66" s="19" t="n">
@@ -15315,7 +15271,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="67">
-      <c r="A67" s="69" t="s">
+      <c r="A67" s="68" t="s">
         <v>877</v>
       </c>
       <c r="B67" s="19" t="n">
@@ -15329,7 +15285,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="68">
-      <c r="A68" s="69" t="s">
+      <c r="A68" s="68" t="s">
         <v>877</v>
       </c>
       <c r="B68" s="19" t="s">
@@ -15343,7 +15299,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="69">
-      <c r="A69" s="69" t="s">
+      <c r="A69" s="68" t="s">
         <v>879</v>
       </c>
       <c r="B69" s="19" t="n">
@@ -15357,7 +15313,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="70">
-      <c r="A70" s="69" t="s">
+      <c r="A70" s="68" t="s">
         <v>879</v>
       </c>
       <c r="B70" s="19" t="n">
@@ -15371,7 +15327,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="71">
-      <c r="A71" s="69" t="s">
+      <c r="A71" s="68" t="s">
         <v>879</v>
       </c>
       <c r="B71" s="19" t="n">
@@ -15385,7 +15341,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="72">
-      <c r="A72" s="69" t="s">
+      <c r="A72" s="68" t="s">
         <v>879</v>
       </c>
       <c r="B72" s="19" t="n">
@@ -15399,7 +15355,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="73">
-      <c r="A73" s="69" t="s">
+      <c r="A73" s="68" t="s">
         <v>879</v>
       </c>
       <c r="B73" s="19" t="s">
@@ -15413,7 +15369,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="74">
-      <c r="A74" s="69" t="s">
+      <c r="A74" s="68" t="s">
         <v>881</v>
       </c>
       <c r="B74" s="19" t="n">
@@ -15427,7 +15383,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="75">
-      <c r="A75" s="69" t="s">
+      <c r="A75" s="68" t="s">
         <v>881</v>
       </c>
       <c r="B75" s="19" t="n">
@@ -15441,7 +15397,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="76">
-      <c r="A76" s="69" t="s">
+      <c r="A76" s="68" t="s">
         <v>881</v>
       </c>
       <c r="B76" s="19" t="n">
@@ -15455,7 +15411,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="77">
-      <c r="A77" s="69" t="s">
+      <c r="A77" s="68" t="s">
         <v>881</v>
       </c>
       <c r="B77" s="19" t="n">
@@ -15469,7 +15425,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="78">
-      <c r="A78" s="69" t="s">
+      <c r="A78" s="68" t="s">
         <v>881</v>
       </c>
       <c r="B78" s="19" t="s">
@@ -15483,7 +15439,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="79">
-      <c r="A79" s="69" t="s">
+      <c r="A79" s="68" t="s">
         <v>883</v>
       </c>
       <c r="B79" s="19" t="n">
@@ -15497,7 +15453,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="80">
-      <c r="A80" s="69" t="s">
+      <c r="A80" s="68" t="s">
         <v>883</v>
       </c>
       <c r="B80" s="19" t="n">
@@ -15511,7 +15467,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="81">
-      <c r="A81" s="69" t="s">
+      <c r="A81" s="68" t="s">
         <v>883</v>
       </c>
       <c r="B81" s="19" t="n">
@@ -15525,7 +15481,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="82">
-      <c r="A82" s="69" t="s">
+      <c r="A82" s="68" t="s">
         <v>883</v>
       </c>
       <c r="B82" s="19" t="n">
@@ -15539,7 +15495,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="83">
-      <c r="A83" s="69" t="s">
+      <c r="A83" s="68" t="s">
         <v>883</v>
       </c>
       <c r="B83" s="19" t="s">
@@ -15553,7 +15509,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="84">
-      <c r="A84" s="69" t="s">
+      <c r="A84" s="68" t="s">
         <v>780</v>
       </c>
       <c r="B84" s="19" t="n">
@@ -15567,7 +15523,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="85">
-      <c r="A85" s="69" t="s">
+      <c r="A85" s="68" t="s">
         <v>780</v>
       </c>
       <c r="B85" s="19" t="n">
@@ -15581,7 +15537,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="86">
-      <c r="A86" s="69" t="s">
+      <c r="A86" s="68" t="s">
         <v>780</v>
       </c>
       <c r="B86" s="19" t="n">
@@ -15595,7 +15551,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="87">
-      <c r="A87" s="69" t="s">
+      <c r="A87" s="68" t="s">
         <v>780</v>
       </c>
       <c r="B87" s="19" t="n">
@@ -15609,7 +15565,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="88">
-      <c r="A88" s="69" t="s">
+      <c r="A88" s="68" t="s">
         <v>780</v>
       </c>
       <c r="B88" s="19" t="s">
@@ -15623,7 +15579,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="89">
-      <c r="A89" s="69" t="s">
+      <c r="A89" s="68" t="s">
         <v>895</v>
       </c>
       <c r="B89" s="19" t="n">
@@ -15637,7 +15593,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="90">
-      <c r="A90" s="69" t="s">
+      <c r="A90" s="68" t="s">
         <v>895</v>
       </c>
       <c r="B90" s="19" t="n">
@@ -15651,7 +15607,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="91">
-      <c r="A91" s="69" t="s">
+      <c r="A91" s="68" t="s">
         <v>895</v>
       </c>
       <c r="B91" s="19" t="n">
@@ -15665,7 +15621,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="92">
-      <c r="A92" s="69" t="s">
+      <c r="A92" s="68" t="s">
         <v>895</v>
       </c>
       <c r="B92" s="19" t="n">
@@ -15679,7 +15635,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="93">
-      <c r="A93" s="69" t="s">
+      <c r="A93" s="68" t="s">
         <v>895</v>
       </c>
       <c r="B93" s="19" t="s">
@@ -15693,7 +15649,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="94">
-      <c r="A94" s="69" t="s">
+      <c r="A94" s="68" t="s">
         <v>897</v>
       </c>
       <c r="B94" s="19" t="n">
@@ -15707,7 +15663,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="95">
-      <c r="A95" s="69" t="s">
+      <c r="A95" s="68" t="s">
         <v>897</v>
       </c>
       <c r="B95" s="19" t="n">
@@ -15721,7 +15677,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="96">
-      <c r="A96" s="69" t="s">
+      <c r="A96" s="68" t="s">
         <v>897</v>
       </c>
       <c r="B96" s="19" t="n">
@@ -15735,7 +15691,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="97">
-      <c r="A97" s="69" t="s">
+      <c r="A97" s="68" t="s">
         <v>897</v>
       </c>
       <c r="B97" s="19" t="n">
@@ -15749,7 +15705,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="98">
-      <c r="A98" s="69" t="s">
+      <c r="A98" s="68" t="s">
         <v>897</v>
       </c>
       <c r="B98" s="19" t="s">
@@ -15763,7 +15719,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="99">
-      <c r="A99" s="69" t="s">
+      <c r="A99" s="68" t="s">
         <v>899</v>
       </c>
       <c r="B99" s="19" t="n">
@@ -15777,7 +15733,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="100">
-      <c r="A100" s="69" t="s">
+      <c r="A100" s="68" t="s">
         <v>899</v>
       </c>
       <c r="B100" s="19" t="n">
@@ -15791,7 +15747,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="101">
-      <c r="A101" s="69" t="s">
+      <c r="A101" s="68" t="s">
         <v>899</v>
       </c>
       <c r="B101" s="19" t="n">
@@ -15805,7 +15761,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="102">
-      <c r="A102" s="69" t="s">
+      <c r="A102" s="68" t="s">
         <v>899</v>
       </c>
       <c r="B102" s="19" t="n">
@@ -15819,7 +15775,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="103">
-      <c r="A103" s="69" t="s">
+      <c r="A103" s="68" t="s">
         <v>899</v>
       </c>
       <c r="B103" s="19" t="s">
@@ -21774,7 +21730,7 @@
       <c r="F4" s="83" t="s">
         <v>783</v>
       </c>
-      <c r="H4" s="66" t="s">
+      <c r="H4" s="82" t="s">
         <v>503</v>
       </c>
     </row>
@@ -21792,7 +21748,7 @@
       <c r="F5" s="83" t="s">
         <v>930</v>
       </c>
-      <c r="H5" s="66" t="n">
+      <c r="H5" s="82" t="n">
         <v>0</v>
       </c>
     </row>
@@ -23230,10 +23186,10 @@
       <c r="B4" s="65" t="s">
         <v>991</v>
       </c>
-      <c r="C4" s="66" t="n">
+      <c r="C4" s="82" t="n">
         <v>0</v>
       </c>
-      <c r="D4" s="66" t="n">
+      <c r="D4" s="82" t="n">
         <v>1</v>
       </c>
       <c r="E4" s="95" t="n">
@@ -23250,10 +23206,10 @@
       <c r="B5" s="65" t="s">
         <v>993</v>
       </c>
-      <c r="C5" s="66" t="n">
+      <c r="C5" s="82" t="n">
         <v>0</v>
       </c>
-      <c r="D5" s="66" t="n">
+      <c r="D5" s="82" t="n">
         <v>0</v>
       </c>
       <c r="E5" s="95" t="n">
@@ -23900,6 +23856,7 @@
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.61133603238866"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.33603238866397"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.3967611336032"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.53441295546559"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="10.9271255060729"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.40485829959514"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="29.0364372469636"/>
@@ -24665,6 +24622,7 @@
     <col collapsed="false" hidden="false" max="7" min="6" style="0" width="8.61133603238866"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="7.33603238866397"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.3967611336032"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.53441295546559"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.9271255060729"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.40485829959514"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="0" width="29.0364372469636"/>
@@ -25973,46 +25931,47 @@
     <col collapsed="false" hidden="false" max="4" min="3" style="0" width="10.0404858299595"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="7.07692307692308"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.50607287449393"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="8.53441295546559"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="6.68421052631579"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="10.0404858299595"/>
     <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.20647773279352"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="44.75" outlineLevel="0" r="1" s="77">
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="44.75" outlineLevel="0" r="1" s="76">
       <c r="A1" s="137" t="s">
         <v>123</v>
       </c>
       <c r="B1" s="137" t="s">
         <v>122</v>
       </c>
-      <c r="C1" s="78" t="s">
+      <c r="C1" s="77" t="s">
         <v>1162</v>
       </c>
-      <c r="D1" s="78" t="s">
+      <c r="D1" s="77" t="s">
         <v>1163</v>
       </c>
-      <c r="E1" s="78" t="s">
+      <c r="E1" s="77" t="s">
         <v>1164</v>
       </c>
-      <c r="F1" s="77" t="s">
+      <c r="F1" s="76" t="s">
         <v>1165</v>
       </c>
       <c r="G1" s="138" t="s">
         <v>1166</v>
       </c>
-      <c r="H1" s="78" t="s">
+      <c r="H1" s="77" t="s">
         <v>1167</v>
       </c>
-      <c r="I1" s="78" t="s">
+      <c r="I1" s="77" t="s">
         <v>1168</v>
       </c>
-      <c r="J1" s="78" t="s">
+      <c r="J1" s="77" t="s">
         <v>1169</v>
       </c>
-      <c r="K1" s="78" t="s">
+      <c r="K1" s="77" t="s">
         <v>831</v>
       </c>
-      <c r="L1" s="78"/>
+      <c r="L1" s="77"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="2">
       <c r="A2" s="30" t="s">
@@ -26189,31 +26148,31 @@
       <c r="L20" s="140"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="69.8" outlineLevel="0" r="21" s="143">
-      <c r="A21" s="77" t="s">
+      <c r="A21" s="76" t="s">
         <v>1188</v>
       </c>
-      <c r="B21" s="78" t="s">
+      <c r="B21" s="77" t="s">
         <v>1109</v>
       </c>
-      <c r="C21" s="77" t="s">
+      <c r="C21" s="76" t="s">
         <v>1189</v>
       </c>
-      <c r="D21" s="77" t="s">
+      <c r="D21" s="76" t="s">
         <v>1190</v>
       </c>
       <c r="E21" s="142" t="s">
         <v>1191</v>
       </c>
-      <c r="F21" s="77" t="s">
+      <c r="F21" s="76" t="s">
         <v>1192</v>
       </c>
-      <c r="G21" s="77" t="s">
+      <c r="G21" s="76" t="s">
         <v>1193</v>
       </c>
-      <c r="H21" s="77" t="s">
+      <c r="H21" s="76" t="s">
         <v>1194</v>
       </c>
-      <c r="I21" s="77" t="s">
+      <c r="I21" s="76" t="s">
         <v>1195</v>
       </c>
     </row>
@@ -27431,6 +27390,7 @@
     <col collapsed="false" hidden="false" max="17" min="17" style="0" width="7.38461538461539"/>
     <col collapsed="false" hidden="false" max="18" min="18" style="0" width="10.3400809716599"/>
     <col collapsed="false" hidden="false" max="19" min="19" style="0" width="10.4817813765182"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="8.53441295546559"/>
     <col collapsed="false" hidden="false" max="21" min="21" style="0" width="8.7246963562753"/>
     <col collapsed="false" hidden="false" max="22" min="22" style="0" width="7.51417004048583"/>
     <col collapsed="false" hidden="false" max="23" min="23" style="0" width="10.4817813765182"/>

</xml_diff>

<commit_message>
Future-date instrument certifications in test.xlsx
</commit_message>
<xml_diff>
--- a/bika/lims/setupdata/test/test.xlsx
+++ b/bika/lims/setupdata/test/test.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="11" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="751" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="25" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="751" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" state="visible" r:id="rId2"/>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/comments15.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:v2="http://schemas.openxmlformats.org/spreadsheetml/2006/main/v2" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" mc:Ignorable="v2">
   <authors>
     <author/>
   </authors>
@@ -80,21 +80,42 @@
       <text>
         <r>
           <rPr>
+            <rFont val="Arial"/>
+            <charset val="1"/>
+            <family val="2"/>
             <sz val="10"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">The sample type abbreviation must be unique – it is used as prefix to sample records</t>
         </r>
       </text>
+      <mc:AlternateContent>
+        <mc:Choice Requires="v2">
+          <commentPr autoFill="true" autoScale="false" colHidden="false" locked="false" rowHidden="false" textHAlign="justify" textVAlign="justify">
+            <anchor moveWithCells="false" sizeWithCells="false">
+              <xdr:from>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>3</xdr:colOff>
+                <xdr:row>-1</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </xdr:from>
+              <xdr:to>
+                <xdr:col>13</xdr:col>
+                <xdr:colOff>3</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>2</xdr:rowOff>
+              </xdr:to>
+            </anchor>
+          </commentPr>
+        </mc:Choice>
+        <mc:Fallback/>
+      </mc:AlternateContent>
     </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/comments17.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:v2="http://schemas.openxmlformats.org/spreadsheetml/2006/main/v2" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" mc:Ignorable="v2">
   <authors>
     <author/>
   </authors>
@@ -103,23 +124,44 @@
       <text>
         <r>
           <rPr>
+            <rFont val="Calibri"/>
+            <charset val="1"/>
+            <family val="2"/>
+            <color rgb="00000000"/>
             <sz val="11"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">If more than one Sample Type can be sampled at a Sample Point, please add entries for the extra combinations in this sheet.
 Single Sample Types per Sample Point can be entered 'Sample Points' sheet.</t>
         </r>
       </text>
+      <mc:AlternateContent>
+        <mc:Choice Requires="v2">
+          <commentPr autoFill="true" autoScale="false" colHidden="false" locked="false" rowHidden="false" textHAlign="justify" textVAlign="justify">
+            <anchor moveWithCells="false" sizeWithCells="false">
+              <xdr:from>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>3</xdr:colOff>
+                <xdr:row>-1</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </xdr:from>
+              <xdr:to>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>3</xdr:colOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>16</xdr:rowOff>
+              </xdr:to>
+            </anchor>
+          </commentPr>
+        </mc:Choice>
+        <mc:Fallback/>
+      </mc:AlternateContent>
     </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/comments34.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:v2="http://schemas.openxmlformats.org/spreadsheetml/2006/main/v2" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" mc:Ignorable="v2">
   <authors>
     <author/>
   </authors>
@@ -128,23 +170,44 @@
       <text>
         <r>
           <rPr>
+            <rFont val="Calibri"/>
+            <charset val="1"/>
+            <family val="2"/>
+            <color rgb="00000000"/>
             <sz val="11"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">From the manual: 'Some Analyses requiring text input as results is best limited to a number of known possible outcomes to prevent typos and irrelevant input skewing reporting. 
 The known outcomes, e.g. 'Positive' or 'Negative',  can be pre-configured here and only these allowed when results are captured. These will be offered as options on a drop-down menu on the data capturing screens'</t>
         </r>
       </text>
+      <mc:AlternateContent>
+        <mc:Choice Requires="v2">
+          <commentPr autoFill="true" autoScale="false" colHidden="false" locked="false" rowHidden="false" textHAlign="justify" textVAlign="justify">
+            <anchor moveWithCells="false" sizeWithCells="false">
+              <xdr:from>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>75</xdr:colOff>
+                <xdr:row>-1</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </xdr:from>
+              <xdr:to>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>44</xdr:colOff>
+                <xdr:row>11</xdr:row>
+                <xdr:rowOff>12</xdr:rowOff>
+              </xdr:to>
+            </anchor>
+          </commentPr>
+        </mc:Choice>
+        <mc:Fallback/>
+      </mc:AlternateContent>
     </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/comments8.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:v2="http://schemas.openxmlformats.org/spreadsheetml/2006/main/v2" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" mc:Ignorable="v2">
   <authors>
     <author/>
   </authors>
@@ -153,29 +216,71 @@
       <text>
         <r>
           <rPr>
+            <rFont val="Calibri"/>
+            <charset val="1"/>
+            <family val="2"/>
+            <color rgb="00000000"/>
             <sz val="11"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Only if a Client Contact is a LIMS user too, does he/she get given a (unique) user name and password</t>
         </r>
       </text>
+      <mc:AlternateContent>
+        <mc:Choice Requires="v2">
+          <commentPr autoFill="true" autoScale="false" colHidden="false" locked="false" rowHidden="false" textHAlign="justify" textVAlign="justify">
+            <anchor moveWithCells="false" sizeWithCells="false">
+              <xdr:from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>3</xdr:colOff>
+                <xdr:row>8</xdr:row>
+                <xdr:rowOff>13</xdr:rowOff>
+              </xdr:from>
+              <xdr:to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>3</xdr:colOff>
+                <xdr:row>21</xdr:row>
+                <xdr:rowOff>2</xdr:rowOff>
+              </xdr:to>
+            </anchor>
+          </commentPr>
+        </mc:Choice>
+        <mc:Fallback/>
+      </mc:AlternateContent>
     </comment>
     <comment authorId="0" ref="N3">
       <text>
         <r>
           <rPr>
+            <rFont val="Calibri"/>
+            <charset val="1"/>
+            <family val="2"/>
+            <color rgb="00000000"/>
             <sz val="11"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Please copy from other contacts for the same Client on this sheet: Use contact Fullname (Firstname + “ “ + Lastname). If more than one needs to be cc'd, please separate with commas. Only contacts for the same client are valid.</t>
         </r>
       </text>
+      <mc:AlternateContent>
+        <mc:Choice Requires="v2">
+          <commentPr autoFill="true" autoScale="false" colHidden="false" locked="true" rowHidden="false" textHAlign="justify" textVAlign="justify">
+            <anchor moveWithCells="false" sizeWithCells="false">
+              <xdr:from>
+                <xdr:col>14</xdr:col>
+                <xdr:colOff>3</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>6</xdr:rowOff>
+              </xdr:from>
+              <xdr:to>
+                <xdr:col>17</xdr:col>
+                <xdr:colOff>3</xdr:colOff>
+                <xdr:row>9</xdr:row>
+                <xdr:rowOff>13</xdr:rowOff>
+              </xdr:to>
+            </anchor>
+          </commentPr>
+        </mc:Choice>
+        <mc:Fallback/>
+      </mc:AlternateContent>
     </comment>
   </commentList>
 </comments>
@@ -4387,203 +4492,203 @@
   </numFmts>
   <fonts count="28">
     <font>
+      <name val="Calibri"/>
+      <charset val="1"/>
+      <family val="2"/>
+      <color rgb="00000000"/>
       <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+      <sz val="10"/>
     </font>
     <font>
-      <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+      <sz val="10"/>
     </font>
     <font>
-      <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+      <sz val="10"/>
     </font>
     <font>
+      <name val="Arial"/>
+      <charset val="1"/>
+      <family val="2"/>
       <b val="true"/>
+      <color rgb="00000000"/>
       <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
+      <name val="Arial"/>
+      <charset val="1"/>
+      <family val="2"/>
+      <color rgb="00000000"/>
       <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
+      <name val="Arial"/>
+      <charset val="1"/>
+      <family val="2"/>
+      <color rgb="00000000"/>
       <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
+      <name val="Arial"/>
+      <charset val="1"/>
+      <family val="2"/>
+      <b val="true"/>
+      <color rgb="00000000"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <charset val="1"/>
+      <family val="2"/>
+      <b val="true"/>
+      <color rgb="00000000"/>
+      <sz val="14"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <charset val="1"/>
+      <family val="2"/>
       <b val="true"/>
       <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
+      <name val="Arial"/>
+      <charset val="1"/>
+      <family val="2"/>
+      <color rgb="000000FF"/>
+      <sz val="10"/>
+      <u val="single"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <charset val="1"/>
+      <family val="2"/>
       <b val="true"/>
       <sz val="14"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
+      <name val="Arial"/>
+      <charset val="1"/>
+      <family val="2"/>
+      <color rgb="000000FF"/>
+      <sz val="14"/>
+      <u val="single"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <charset val="1"/>
+      <family val="2"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <charset val="1"/>
+      <family val="2"/>
+      <color rgb="000000FF"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <charset val="1"/>
+      <family val="2"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <charset val="1"/>
+      <family val="2"/>
+      <b val="true"/>
+      <color rgb="00000000"/>
+      <sz val="13"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="1"/>
+      <family val="2"/>
+      <b val="true"/>
+      <color rgb="00000000"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="1"/>
+      <family val="2"/>
+      <color rgb="00000000"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <charset val="1"/>
+      <family val="2"/>
+      <color rgb="00000000"/>
+      <sz val="13"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="1"/>
+      <family val="2"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <charset val="1"/>
+      <family val="2"/>
+      <b val="true"/>
+      <sz val="13"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="1"/>
+      <family val="2"/>
+      <b val="true"/>
+      <color rgb="00000000"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="1"/>
+      <family val="2"/>
+      <b val="true"/>
+      <color rgb="00000000"/>
+      <sz val="14"/>
+    </font>
+    <font>
+      <name val="Arla"/>
+      <charset val="1"/>
+      <family val="0"/>
+      <b val="true"/>
+      <color rgb="00000000"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arla"/>
+      <charset val="1"/>
+      <family val="0"/>
+      <color rgb="00000000"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <charset val="1"/>
+      <family val="2"/>
+      <b val="true"/>
+      <i val="true"/>
+      <color rgb="002323DC"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="1"/>
+      <family val="2"/>
       <b val="true"/>
       <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <u val="single"/>
-      <sz val="10"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="14"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <u val="single"/>
-      <sz val="14"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="13"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="13"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="13"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="14"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arla"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arla"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <i val="true"/>
-      <sz val="10"/>
-      <color rgb="FF2323DC"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -4595,20 +4700,20 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFE6E6FF"/>
-        <bgColor rgb="FFE6E6E6"/>
+        <fgColor rgb="00E6E6FF"/>
+        <bgColor rgb="00E6E6E6"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFE6E6E6"/>
-        <bgColor rgb="FFE6E6FF"/>
+        <fgColor rgb="00E6E6E6"/>
+        <bgColor rgb="00E6E6FF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor rgb="FF993300"/>
+        <fgColor rgb="00FF0000"/>
+        <bgColor rgb="00993300"/>
       </patternFill>
     </fill>
   </fills>
@@ -4654,49 +4759,32 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
   <cellXfs count="145">
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="7" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="7" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="7" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="8" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="5" numFmtId="164" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="9" numFmtId="165" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="10" numFmtId="165" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
@@ -4704,7 +4792,6 @@
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="11" numFmtId="165" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="12" numFmtId="165" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
@@ -4712,527 +4799,370 @@
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="7" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="7" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="13" numFmtId="165" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="165" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="14" numFmtId="165" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="13" numFmtId="165" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="13" numFmtId="164" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="165" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="13" numFmtId="165" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="8" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="7" numFmtId="164" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="7" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="13" numFmtId="165" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="13" numFmtId="164" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="13" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="3" fontId="13" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="15" numFmtId="164" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="13" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="13" numFmtId="166" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="16" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="13" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="17" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="17" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="17" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="17" numFmtId="167" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="17" numFmtId="164" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="18" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="18" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="8" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="16" numFmtId="167" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="16" numFmtId="164" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="16" numFmtId="164" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="19" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="17" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="17" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="17" numFmtId="167" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="17" numFmtId="164" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="18" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="20" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="3" fontId="13" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="20" numFmtId="164" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="16" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="16" numFmtId="164" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="19" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="3" fontId="13" numFmtId="164" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="13" numFmtId="165" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="13" numFmtId="164" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="13" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="3" fontId="13" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="7" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="5" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="5" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="13" numFmtId="165" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="13" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="13" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="5" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="21" numFmtId="165" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="7" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="9" numFmtId="165" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="13" numFmtId="165" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="13" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="5" numFmtId="164" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="13" numFmtId="164" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="13" numFmtId="164" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="5" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="165" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="22" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="5" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="165" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="22" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="22" numFmtId="164" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="22" numFmtId="168" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="22" numFmtId="168" xfId="0"/>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="16" numFmtId="168" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="22" numFmtId="164" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="22" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="22" numFmtId="168" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="13" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="13" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="13" numFmtId="164" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="13" numFmtId="169" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="22" numFmtId="166" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="23" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="22" numFmtId="166" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="23" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="22" numFmtId="165" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="18" numFmtId="164" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="13" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="22" numFmtId="170" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="22" numFmtId="170" xfId="0"/>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="24" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="16" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="8" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="24" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="25" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0">
       <alignment horizontal="right" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="13" numFmtId="164" xfId="0">
       <alignment horizontal="right" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="7" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="9" numFmtId="165" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="16" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="16" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="21" numFmtId="165" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="13" numFmtId="165" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="26" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="13" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="26" numFmtId="165" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="9" numFmtId="165" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="27" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="18" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="20" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="18" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="20" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="18" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="22" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="13" numFmtId="165" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="7" numFmtId="164" xfId="0">
       <alignment horizontal="right" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="7" numFmtId="164" xfId="0">
       <alignment horizontal="right" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="5" numFmtId="164" xfId="0">
       <alignment horizontal="right" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="13" numFmtId="164" xfId="0">
       <alignment horizontal="right" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="13" numFmtId="164" xfId="0">
       <alignment horizontal="right" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="5" numFmtId="164" xfId="0">
       <alignment horizontal="right" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="13" numFmtId="164" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="9" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="9" numFmtId="167" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="167" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="5" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="5" numFmtId="167" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="7" numFmtId="167" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="4" fontId="5" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -5245,62 +5175,62 @@
   </cellStyles>
   <colors>
     <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFE6E6FF"/>
-      <rgbColor rgb="FFFF0000"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008000"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF808000"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
-      <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF9999FF"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFE6E6E6"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFCCCCFF"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
-      <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
-      <rgbColor rgb="FF3366FF"/>
-      <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
-      <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
-      <rgbColor rgb="FF003300"/>
-      <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF2323DC"/>
-      <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00E6E6FF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00E6E6E6"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="002323DC"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -5317,11 +5247,10 @@
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="94.4372469635628"/>
-    <col collapsed="false" hidden="false" max="1023" min="2" style="0" width="8.61133603238866"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="8.64777327935223"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="94.8274509803922"/>
+    <col collapsed="false" hidden="false" max="1023" min="2" style="0" width="8.64705882352941"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="8.68235294117647"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="32.05" outlineLevel="0" r="1" s="3">
@@ -5388,11 +5317,10 @@
       <selection activeCell="B9" activeCellId="0" pane="topLeft" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.1012145748988"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.9514170040486"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="5.85425101214575"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.1764705882353"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.0313725490196"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="5.87843137254902"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="true" ht="12.2" outlineLevel="0" r="1" s="5">
@@ -5490,12 +5418,11 @@
       <selection activeCell="A11" activeCellId="0" pane="topLeft" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.8097165991903"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.5344129554656"/>
-    <col collapsed="false" hidden="false" max="5" min="3" style="0" width="13.8380566801619"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="5.85425101214575"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.8862745098039"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.5921568627451"/>
+    <col collapsed="false" hidden="false" max="5" min="3" style="0" width="13.8980392156863"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="5.87843137254902"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="19.8" outlineLevel="0" r="1" s="5">
@@ -5821,29 +5748,28 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:4"/>
+  <dimension ref="A1:U4"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="C11" activeCellId="0" pane="topLeft" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.3"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.06882591093117"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.48582995951417"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.69230769230769"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.8097165991903"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.86234817813765"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.37651821862348"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.995951417004"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.2753036437247"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="6.89878542510122"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="7.41295546558704"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="23.7368421052632"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.10588235294118"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.50980392156863"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.71764705882353"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.9019607843137"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.89803921568628"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.4156862745098"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.0509803921569"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.31372549019608"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="6.92549019607843"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="7.44313725490196"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="23.8352941176471"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="9.18039215686274"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="true" ht="13.3" outlineLevel="0" r="1" s="5">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="true" ht="12.2" outlineLevel="0" r="1" s="5">
       <c r="A1" s="65" t="s">
         <v>135</v>
       </c>
@@ -5887,37 +5813,33 @@
       <c r="S1" s="65"/>
       <c r="T1" s="65"/>
       <c r="U1" s="65"/>
-      <c r="AMI1" s="0"/>
-      <c r="AMJ1" s="0"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="16.9" outlineLevel="0" r="2" s="6">
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="17" outlineLevel="0" r="2" s="6">
       <c r="A2" s="7" t="s">
         <v>394</v>
       </c>
-      <c r="B2" s="65"/>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="65"/>
-      <c r="H2" s="65"/>
-      <c r="I2" s="65"/>
-      <c r="J2" s="65"/>
-      <c r="K2" s="65"/>
-      <c r="L2" s="65"/>
-      <c r="M2" s="65"/>
-      <c r="N2" s="65"/>
-      <c r="O2" s="65"/>
-      <c r="P2" s="65"/>
-      <c r="Q2" s="65"/>
-      <c r="R2" s="65"/>
-      <c r="S2" s="65"/>
-      <c r="T2" s="65"/>
-      <c r="U2" s="65"/>
-      <c r="AMI2" s="0"/>
-      <c r="AMJ2" s="0"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="3" s="5">
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+      <c r="U2" s="2"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.2" outlineLevel="0" r="3" s="5">
       <c r="A3" s="65" t="s">
         <v>135</v>
       </c>
@@ -5961,10 +5883,8 @@
       <c r="S3" s="65"/>
       <c r="T3" s="65"/>
       <c r="U3" s="65"/>
-      <c r="AMI3" s="0"/>
-      <c r="AMJ3" s="0"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="4">
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="4">
       <c r="A4" s="65" t="s">
         <v>395</v>
       </c>
@@ -6021,15 +5941,14 @@
       <selection activeCell="B9" activeCellId="0" pane="topLeft" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.8461538461538"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.4372469635628"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.57894736842105"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.0526315789474"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.0971659919028"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.8947368421053"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="5.85425101214575"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.9294117647059"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.5294117647059"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.60392156862745"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.121568627451"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.156862745098"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.956862745098"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="5.87843137254902"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="true" ht="12.2" outlineLevel="0" r="1" s="5">
@@ -6247,11 +6166,10 @@
       <selection activeCell="A2" activeCellId="0" pane="topLeft" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.9919028340081"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.1821862348178"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="5.85425101214575"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.0392156862745"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.2627450980392"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="5.87843137254902"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="true" ht="12.2" outlineLevel="0" r="1" s="5">
@@ -6357,18 +6275,17 @@
       <selection activeCell="A2" activeCellId="0" pane="topLeft" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.0526315789474"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.4372469635628"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.57894736842105"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="4.56275303643725"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.50607287449393"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.66801619433198"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.35627530364372"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.9473684210526"/>
-    <col collapsed="false" hidden="false" max="1023" min="9" style="0" width="6.66801619433198"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="5.69230769230769"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.1098039215686"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.5411764705882"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.60392156862745"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="4.58039215686275"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.54117647058824"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.69803921568628"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.3843137254902"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.0039215686275"/>
+    <col collapsed="false" hidden="false" max="1023" min="9" style="0" width="6.69803921568628"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="5.71372549019608"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="true" ht="13.2" outlineLevel="0" r="1" s="14">
@@ -6794,16 +6711,15 @@
       <selection activeCell="B14" activeCellId="0" pane="topLeft" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="12.6599190283401"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.4736842105263"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.3117408906883"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="17.2874493927125"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.48582995951417"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.96761133603239"/>
-    <col collapsed="false" hidden="false" max="1018" min="9" style="0" width="5.85425101214575"/>
-    <col collapsed="false" hidden="false" max="1025" min="1019" style="0" width="5.57085020242915"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="12.7137254901961"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.5764705882353"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.3764705882353"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="17.3607843137255"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.51372549019608"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.0117647058824"/>
+    <col collapsed="false" hidden="false" max="1018" min="9" style="0" width="5.87843137254902"/>
+    <col collapsed="false" hidden="false" max="1025" min="1019" style="0" width="5.5921568627451"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="true" ht="12.2" outlineLevel="0" r="1" s="5">
@@ -7071,13 +6987,12 @@
       <selection activeCell="A2" activeCellId="0" pane="topLeft" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.4939271255061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.2105263157895"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.6963562753036"/>
-    <col collapsed="false" hidden="false" max="1018" min="4" style="0" width="5.85425101214575"/>
-    <col collapsed="false" hidden="false" max="1025" min="1019" style="0" width="5.01214574898785"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.5725490196078"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.2980392156863"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.7607843137255"/>
+    <col collapsed="false" hidden="false" max="1018" min="4" style="0" width="5.87843137254902"/>
+    <col collapsed="false" hidden="false" max="1025" min="1019" style="0" width="5.03529411764706"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="true" ht="12.2" outlineLevel="0" r="1" s="14">
@@ -7144,12 +7059,11 @@
       <selection activeCell="A4" activeCellId="0" pane="topLeft" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.246963562753"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="55.2226720647773"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.4736842105263"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="5.85425101214575"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.3098039215686"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="55.4509803921569"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.5764705882353"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="5.87843137254902"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="true" ht="12.2" outlineLevel="0" r="1" s="14">
@@ -7337,11 +7251,10 @@
       <selection activeCell="A2" activeCellId="0" pane="topLeft" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.4372469635628"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.5587044534413"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="5.85425101214575"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.5372549019608"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.6274509803922"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="5.87843137254902"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="true" ht="12.2" outlineLevel="0" r="1" s="5">
@@ -7478,13 +7391,12 @@
       <selection activeCell="B2" activeCellId="0" pane="topLeft" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="true" max="1" min="1" style="0" width="0"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.4534412955466"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.23481781376518"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="4.65587044534413"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="6.63967611336032"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.5176470588235"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.25882352941177"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="4.67450980392157"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="6.67058823529412"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="true" ht="12.2" outlineLevel="0" r="1" s="5">
@@ -7677,13 +7589,12 @@
       <selection activeCell="A4" activeCellId="0" pane="topLeft" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.4453441295547"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="9.47773279352227"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.1376518218623"/>
-    <col collapsed="false" hidden="false" max="21" min="6" style="0" width="9.47773279352227"/>
-    <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="16.4453441295547"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.5137254901961"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="9.51764705882353"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.2039215686275"/>
+    <col collapsed="false" hidden="false" max="21" min="6" style="0" width="9.51764705882353"/>
+    <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="16.5137254901961"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="true" ht="12.2" outlineLevel="0" r="1" s="5">
@@ -7908,11 +7819,10 @@
       <selection activeCell="A25" activeCellId="0" pane="topLeft" sqref="A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.5303643724696"/>
-    <col collapsed="false" hidden="false" max="21" min="2" style="0" width="7.93927125506073"/>
-    <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="5.85425101214575"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.6235294117647"/>
+    <col collapsed="false" hidden="false" max="21" min="2" style="0" width="7.97254901960784"/>
+    <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="5.87843137254902"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="true" ht="12.2" outlineLevel="0" r="1" s="5">
@@ -8187,12 +8097,11 @@
       <selection activeCell="A4" activeCellId="0" pane="topLeft" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.3400809716599"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.0526315789474"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="7.54655870445344"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="7.51417004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.4274509803922"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.1686274509804"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="7.58039215686275"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="7.54509803921569"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13.4" outlineLevel="0" r="1">
@@ -8308,20 +8217,19 @@
       <selection activeCell="A4" activeCellId="0" pane="topLeft" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.8461538461538"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.4008097165992"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.0445344129555"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.9028340080972"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.5101214574899"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.6882591093117"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.9554655870445"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.2388663967611"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.246963562753"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="7.54655870445344"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="11.1821862348178"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="5.85425101214575"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.9294117647059"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.4980392156863"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.1176470588235"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.9725490196078"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.5647058823529"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.7803921568627"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.2862745098039"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.2980392156863"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="7.58039215686275"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="11.2313725490196"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="5.87843137254902"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="true" ht="13.4" outlineLevel="0" r="1" s="85">
@@ -9429,17 +9337,16 @@
       <selection activeCell="A2" activeCellId="0" pane="topLeft" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.1093117408907"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.3157894736842"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.5708502024292"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.36032388663968"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.2834008097166"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.0971659919028"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.5587044534413"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="28.4210526315789"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="7.54655870445344"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.1764705882353"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.3843137254902"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.6117647058824"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.4"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.3372549019608"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.1686274509804"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.6274509803922"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="28.5411764705882"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="7.58039215686275"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="15.1" outlineLevel="0" r="1" s="85">
@@ -9572,17 +9479,16 @@
       <selection activeCell="A2" activeCellId="0" pane="topLeft" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.1093117408907"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.4817813765182"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.5708502024292"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.36032388663968"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.2834008097166"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.0971659919028"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.5587044534413"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="28.4210526315789"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="7.54655870445344"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.1764705882353"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.5294117647059"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.6117647058824"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.4"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.3372549019608"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.1686274509804"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.6274509803922"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="28.5411764705882"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="7.58039215686275"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="15.1" outlineLevel="0" r="1" s="85">
@@ -9708,20 +9614,19 @@
   </sheetPr>
   <dimension ref="A1:G100"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A12" activeCellId="0" pane="topLeft" sqref="A12"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="G22" activeCellId="0" pane="topLeft" sqref="G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.8097165991903"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.5951417004049"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.54655870445344"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.78947368421053"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="7.54655870445344"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.3238866396761"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.4372469635628"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="7.54655870445344"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.8705882352941"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.678431372549"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.58039215686275"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.1607843137255"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.2509803921569"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.3882352941176"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.5411764705882"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="7.58039215686275"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="14.9" outlineLevel="0" r="1">
@@ -9785,13 +9690,13 @@
         <v>634</v>
       </c>
       <c r="C4" s="95" t="n">
-        <v>40910</v>
+        <v>41642</v>
       </c>
       <c r="D4" s="95" t="n">
-        <v>40911</v>
+        <v>41642</v>
       </c>
       <c r="E4" s="95" t="n">
-        <v>41985</v>
+        <v>42350</v>
       </c>
       <c r="F4" s="0" t="s">
         <v>730</v>
@@ -9805,13 +9710,13 @@
         <v>638</v>
       </c>
       <c r="C5" s="95" t="n">
-        <v>40910</v>
+        <v>41643</v>
       </c>
       <c r="D5" s="95" t="n">
-        <v>40911</v>
+        <v>41643</v>
       </c>
       <c r="E5" s="95" t="n">
-        <v>41986</v>
+        <v>42351</v>
       </c>
       <c r="F5" s="0" t="s">
         <v>730</v>
@@ -9825,13 +9730,13 @@
         <v>560</v>
       </c>
       <c r="C6" s="95" t="n">
-        <v>40910</v>
+        <v>41644</v>
       </c>
       <c r="D6" s="95" t="n">
-        <v>40911</v>
+        <v>41644</v>
       </c>
       <c r="E6" s="95" t="n">
-        <v>41987</v>
+        <v>42352</v>
       </c>
       <c r="F6" s="0" t="s">
         <v>730</v>
@@ -9845,13 +9750,13 @@
         <v>683</v>
       </c>
       <c r="C7" s="95" t="n">
-        <v>40910</v>
+        <v>41645</v>
       </c>
       <c r="D7" s="95" t="n">
-        <v>40911</v>
+        <v>41645</v>
       </c>
       <c r="E7" s="95" t="n">
-        <v>41988</v>
+        <v>42353</v>
       </c>
       <c r="F7" s="0" t="s">
         <v>730</v>
@@ -9865,13 +9770,13 @@
         <v>630</v>
       </c>
       <c r="C8" s="95" t="n">
-        <v>40910</v>
+        <v>41646</v>
       </c>
       <c r="D8" s="95" t="n">
-        <v>40911</v>
+        <v>41646</v>
       </c>
       <c r="E8" s="95" t="n">
-        <v>41989</v>
+        <v>42354</v>
       </c>
       <c r="F8" s="0" t="s">
         <v>730</v>
@@ -9885,13 +9790,13 @@
         <v>642</v>
       </c>
       <c r="C9" s="95" t="n">
-        <v>40910</v>
+        <v>41647</v>
       </c>
       <c r="D9" s="95" t="n">
-        <v>40911</v>
+        <v>41647</v>
       </c>
       <c r="E9" s="95" t="n">
-        <v>41990</v>
+        <v>42355</v>
       </c>
       <c r="F9" s="0" t="s">
         <v>730</v>
@@ -9905,13 +9810,13 @@
         <v>626</v>
       </c>
       <c r="C10" s="95" t="n">
-        <v>40910</v>
+        <v>41648</v>
       </c>
       <c r="D10" s="95" t="n">
-        <v>40911</v>
+        <v>41648</v>
       </c>
       <c r="E10" s="95" t="n">
-        <v>41991</v>
+        <v>42356</v>
       </c>
       <c r="F10" s="0" t="s">
         <v>730</v>
@@ -9925,13 +9830,13 @@
         <v>626</v>
       </c>
       <c r="C11" s="95" t="n">
-        <v>41275</v>
+        <v>41649</v>
       </c>
       <c r="D11" s="95" t="n">
-        <v>41277</v>
+        <v>41649</v>
       </c>
       <c r="E11" s="95" t="n">
-        <v>41992</v>
+        <v>42357</v>
       </c>
       <c r="F11" s="0" t="s">
         <v>730</v>
@@ -9945,13 +9850,13 @@
         <v>607</v>
       </c>
       <c r="C12" s="95" t="n">
-        <v>40910</v>
+        <v>41650</v>
       </c>
       <c r="D12" s="95" t="n">
-        <v>40911</v>
+        <v>41650</v>
       </c>
       <c r="E12" s="95" t="n">
-        <v>41993</v>
+        <v>42358</v>
       </c>
       <c r="F12" s="0" t="s">
         <v>730</v>
@@ -9965,13 +9870,13 @@
         <v>675</v>
       </c>
       <c r="C13" s="95" t="n">
-        <v>40910</v>
+        <v>41651</v>
       </c>
       <c r="D13" s="95" t="n">
-        <v>40911</v>
+        <v>41651</v>
       </c>
       <c r="E13" s="95" t="n">
-        <v>41994</v>
+        <v>42359</v>
       </c>
       <c r="F13" s="0" t="s">
         <v>730</v>
@@ -9985,13 +9890,13 @@
         <v>679</v>
       </c>
       <c r="C14" s="95" t="n">
-        <v>40910</v>
+        <v>41652</v>
       </c>
       <c r="D14" s="95" t="n">
-        <v>40911</v>
+        <v>41652</v>
       </c>
       <c r="E14" s="95" t="n">
-        <v>41995</v>
+        <v>42360</v>
       </c>
       <c r="F14" s="0" t="s">
         <v>730</v>
@@ -10005,13 +9910,13 @@
         <v>686</v>
       </c>
       <c r="C15" s="95" t="n">
-        <v>40910</v>
+        <v>41653</v>
       </c>
       <c r="D15" s="95" t="n">
-        <v>40911</v>
+        <v>41653</v>
       </c>
       <c r="E15" s="95" t="n">
-        <v>41996</v>
+        <v>42361</v>
       </c>
       <c r="F15" s="0" t="s">
         <v>730</v>
@@ -10025,13 +9930,13 @@
         <v>688</v>
       </c>
       <c r="C16" s="95" t="n">
-        <v>40910</v>
+        <v>41654</v>
       </c>
       <c r="D16" s="95" t="n">
-        <v>40911</v>
+        <v>41654</v>
       </c>
       <c r="E16" s="95" t="n">
-        <v>41997</v>
+        <v>42362</v>
       </c>
       <c r="F16" s="0" t="s">
         <v>730</v>
@@ -10045,13 +9950,13 @@
         <v>648</v>
       </c>
       <c r="C17" s="95" t="n">
-        <v>40910</v>
+        <v>41655</v>
       </c>
       <c r="D17" s="95" t="n">
-        <v>40911</v>
+        <v>41655</v>
       </c>
       <c r="E17" s="95" t="n">
-        <v>41998</v>
+        <v>42363</v>
       </c>
       <c r="F17" s="0" t="s">
         <v>730</v>
@@ -10065,13 +9970,13 @@
         <v>652</v>
       </c>
       <c r="C18" s="95" t="n">
-        <v>40910</v>
+        <v>41656</v>
       </c>
       <c r="D18" s="95" t="n">
-        <v>40911</v>
+        <v>41656</v>
       </c>
       <c r="E18" s="95" t="n">
-        <v>41999</v>
+        <v>42364</v>
       </c>
       <c r="F18" s="0" t="s">
         <v>730</v>
@@ -10085,13 +9990,13 @@
         <v>556</v>
       </c>
       <c r="C19" s="95" t="n">
-        <v>40910</v>
+        <v>41657</v>
       </c>
       <c r="D19" s="95" t="n">
-        <v>40911</v>
+        <v>41657</v>
       </c>
       <c r="E19" s="95" t="n">
-        <v>42000</v>
+        <v>42365</v>
       </c>
       <c r="F19" s="0" t="s">
         <v>730</v>
@@ -10105,13 +10010,13 @@
         <v>601</v>
       </c>
       <c r="C20" s="95" t="n">
-        <v>40910</v>
+        <v>41658</v>
       </c>
       <c r="D20" s="95" t="n">
-        <v>40911</v>
+        <v>41658</v>
       </c>
       <c r="E20" s="95" t="n">
-        <v>42001</v>
+        <v>42366</v>
       </c>
       <c r="F20" s="0" t="s">
         <v>730</v>
@@ -10125,13 +10030,13 @@
         <v>645</v>
       </c>
       <c r="C21" s="95" t="n">
-        <v>40910</v>
+        <v>41659</v>
       </c>
       <c r="D21" s="95" t="n">
-        <v>40911</v>
+        <v>41659</v>
       </c>
       <c r="E21" s="95" t="n">
-        <v>42002</v>
+        <v>42367</v>
       </c>
       <c r="F21" s="0" t="s">
         <v>730</v>
@@ -10145,13 +10050,13 @@
         <v>661</v>
       </c>
       <c r="C22" s="95" t="n">
-        <v>40910</v>
+        <v>41660</v>
       </c>
       <c r="D22" s="95" t="n">
-        <v>40911</v>
+        <v>41660</v>
       </c>
       <c r="E22" s="95" t="n">
-        <v>42003</v>
+        <v>42368</v>
       </c>
       <c r="F22" s="0" t="s">
         <v>730</v>
@@ -10165,13 +10070,13 @@
         <v>664</v>
       </c>
       <c r="C23" s="95" t="n">
-        <v>40910</v>
+        <v>41661</v>
       </c>
       <c r="D23" s="95" t="n">
-        <v>40911</v>
+        <v>41661</v>
       </c>
       <c r="E23" s="95" t="n">
-        <v>42004</v>
+        <v>42369</v>
       </c>
       <c r="F23" s="0" t="s">
         <v>730</v>
@@ -10185,13 +10090,13 @@
         <v>668</v>
       </c>
       <c r="C24" s="95" t="n">
-        <v>40910</v>
+        <v>41662</v>
       </c>
       <c r="D24" s="95" t="n">
-        <v>40911</v>
+        <v>41662</v>
       </c>
       <c r="E24" s="95" t="n">
-        <v>42005</v>
+        <v>42370</v>
       </c>
       <c r="F24" s="0" t="s">
         <v>730</v>
@@ -10205,13 +10110,13 @@
         <v>671</v>
       </c>
       <c r="C25" s="95" t="n">
-        <v>40910</v>
+        <v>41663</v>
       </c>
       <c r="D25" s="95" t="n">
-        <v>40911</v>
+        <v>41663</v>
       </c>
       <c r="E25" s="95" t="n">
-        <v>42006</v>
+        <v>42371</v>
       </c>
       <c r="F25" s="0" t="s">
         <v>730</v>
@@ -10699,19 +10604,18 @@
       <selection activeCell="A2" activeCellId="0" pane="topLeft" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.9311740890688"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.7368421052632"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.9595141700405"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.0202429149798"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.1133603238866"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="7.54655870445344"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.0404858299595"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.1052631578947"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.17004048583"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="5.21862348178138"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="7.54655870445344"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.9921568627451"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.8352941176471"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.0352941176471"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.0588235294118"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.156862745098"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="7.58039215686275"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.0980392156863"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.1607843137255"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.2313725490196"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="5.24313725490196"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="7.58039215686275"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="14.9" outlineLevel="0" r="1" s="85">
@@ -10926,19 +10830,18 @@
       <selection activeCell="A2" activeCellId="0" pane="topLeft" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.2105263157895"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.4089068825911"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.4817813765182"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.0202429149798"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.1133603238866"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.6882591093117"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.1052631578947"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.3198380566802"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="27.3279352226721"/>
-    <col collapsed="false" hidden="false" max="1023" min="10" style="0" width="7.54655870445344"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="7.51417004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.2823529411765"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.4980392156863"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.5607843137255"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.0588235294118"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.156862745098"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.7490196078431"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.1607843137255"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.3647058823529"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="27.443137254902"/>
+    <col collapsed="false" hidden="false" max="1023" min="10" style="0" width="7.58039215686275"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="7.54509803921569"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="14.9" outlineLevel="0" r="1" s="85">
@@ -11029,12 +10932,11 @@
       <selection activeCell="A2" activeCellId="0" pane="topLeft" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.502024291498"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.0728744939271"/>
-    <col collapsed="false" hidden="false" max="5" min="3" style="0" width="20.7085020242915"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="5.85425101214575"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.6196078431373"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.2039215686274"/>
+    <col collapsed="false" hidden="false" max="5" min="3" style="0" width="20.7960784313725"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="5.87843137254902"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="true" ht="12.2" outlineLevel="0" r="1" s="5">
@@ -11132,12 +11034,11 @@
       <selection activeCell="B2" activeCellId="0" pane="topLeft" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="true" max="1" min="1" style="0" width="0"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.4412955465587"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.246963562753"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="6.66801619433198"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.5764705882353"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.3176470588235"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="6.69803921568628"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="true" ht="12.2" outlineLevel="0" r="1" s="5">
@@ -11535,12 +11436,11 @@
       <selection activeCell="A2" activeCellId="0" pane="topLeft" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.995951417004"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="45.9959514170041"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="46.5748987854251"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="6.24291497975709"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0666666666667"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="46.1882352941177"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="46.7686274509804"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="6.26666666666667"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="true" ht="14.15" outlineLevel="0" r="1" s="104">
@@ -11673,12 +11573,11 @@
       <selection activeCell="B18" activeCellId="0" pane="topLeft" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="24.5222672064777"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="7.06072874493927"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="3.27125506072874"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="5.85425101214575"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="24.6235294117647"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="7.09019607843137"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="3.28235294117647"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="5.87843137254902"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="true" ht="12.2" outlineLevel="0" r="1" s="5">
@@ -12281,30 +12180,29 @@
       <selection activeCell="C14" activeCellId="0" pane="topLeft" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.5222672064777"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.6801619433198"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.16194331983806"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="5.16194331983806"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.2874493927125"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.0971659919028"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="9.93522267206478"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="7.24291497975709"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="5.98380566801619"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="7.51417004048583"/>
-    <col collapsed="false" hidden="false" max="13" min="11" style="0" width="3.59109311740891"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="3.86234817813765"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="6.29959514170041"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="3.27125506072874"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="13.2550607287449"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="9.50607287449393"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="13.1619433198381"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="11.2348178137652"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="9.03238866396761"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="8.19028340080972"/>
-    <col collapsed="false" hidden="false" max="24" min="23" style="0" width="10.5060728744939"/>
-    <col collapsed="false" hidden="false" max="1025" min="25" style="0" width="7.51417004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.6078431372549"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.8"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.19607843137255"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="5.1843137254902"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.3607843137255"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.1411764705882"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="9.97647058823529"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="7.27058823529412"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="6.0078431372549"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="7.54509803921569"/>
+    <col collapsed="false" hidden="false" max="13" min="11" style="0" width="3.6078431372549"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="3.87843137254902"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="6.32549019607843"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="3.28235294117647"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="13.3098039215686"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="9.54509803921569"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="13.2156862745098"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="11.278431372549"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="9.07058823529412"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="8.22352941176471"/>
+    <col collapsed="false" hidden="false" max="24" min="23" style="0" width="10.5490196078431"/>
+    <col collapsed="false" hidden="false" max="1025" min="25" style="0" width="7.54509803921569"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="34.9" outlineLevel="0" r="1" s="14">
@@ -14061,14 +13959,13 @@
       <selection activeCell="B22" activeCellId="0" pane="topLeft" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.6437246963563"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.68421052631579"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.46963562753036"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.0404858299595"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="3.27125506072874"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="5.85425101214575"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.756862745098"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.72156862745098"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.50588235294118"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.0980392156863"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="3.28235294117647"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="5.87843137254902"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="true" ht="12.2" outlineLevel="0" r="1" s="5">
@@ -14133,14 +14030,13 @@
       <selection activeCell="A2" activeCellId="0" pane="topLeft" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.3562753036437"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.412955465587"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.36437246963563"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.0404858299595"/>
-    <col collapsed="false" hidden="false" max="973" min="5" style="0" width="5.85425101214575"/>
-    <col collapsed="false" hidden="false" max="1025" min="974" style="0" width="5.01214574898785"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.3960784313725"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.4588235294118"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.39607843137255"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.0980392156863"/>
+    <col collapsed="false" hidden="false" max="973" min="5" style="0" width="5.87843137254902"/>
+    <col collapsed="false" hidden="false" max="1025" min="974" style="0" width="5.03529411764706"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="true" ht="24.5" outlineLevel="0" r="1" s="14">
@@ -14342,13 +14238,12 @@
       <selection activeCell="A2" activeCellId="0" pane="topLeft" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.4331983805668"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="9.26315789473684"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.56275303643725"/>
-    <col collapsed="false" hidden="false" max="997" min="5" style="0" width="5.85425101214575"/>
-    <col collapsed="false" hidden="false" max="1025" min="998" style="0" width="5.01214574898785"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.5803921568627"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="9.30196078431373"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.6"/>
+    <col collapsed="false" hidden="false" max="997" min="5" style="0" width="5.87843137254902"/>
+    <col collapsed="false" hidden="false" max="1025" min="998" style="0" width="5.03529411764706"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="true" ht="24.5" outlineLevel="0" r="1" s="14">
@@ -15819,15 +15714,14 @@
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.668016194332"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.3684210526316"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.6720647773279"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.748987854251"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.4493927125506"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="5.38461538461539"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="5.85425101214575"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.7372549019608"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.4274509803922"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.7843137254902"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.7960784313726"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.4901960784314"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="5.4078431372549"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="5.87843137254902"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="true" ht="12.2" outlineLevel="0" r="1" s="39">
@@ -15955,12 +15849,11 @@
       <selection activeCell="D26" activeCellId="0" pane="topLeft" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.9392712550607"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.2024291497976"/>
-    <col collapsed="false" hidden="false" max="6" min="3" style="0" width="28.7854251012146"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="5.85425101214575"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.0274509803922"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.3137254901961"/>
+    <col collapsed="false" hidden="false" max="6" min="3" style="0" width="28.9058823529412"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="5.87843137254902"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.2" outlineLevel="0" r="1" s="39">
@@ -16148,15 +16041,14 @@
       <selection activeCell="B39" activeCellId="0" pane="topLeft" sqref="B39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.0971659919028"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.4412955465587"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.5060728744939"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.7044534412955"/>
-    <col collapsed="false" hidden="false" max="7" min="5" style="0" width="9.91902834008097"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.3481781376518"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="5.85425101214575"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.156862745098"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.47843137254902"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.556862745098"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.7843137254902"/>
+    <col collapsed="false" hidden="false" max="7" min="5" style="0" width="9.96078431372549"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.3960784313726"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="5.87843137254902"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="15.05" outlineLevel="0" r="1" s="5">
@@ -21640,16 +21532,15 @@
       <selection activeCell="C15" activeCellId="0" pane="topLeft" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.8178137651822"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.6558704453441"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.2105263157895"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="10.0404858299595"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.4534412955466"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.2186234817814"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.0485829959514"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="5.85425101214575"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.9176470588235"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.6980392156863"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.2627450980392"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="10.0823529411765"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.5176470588235"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.278431372549"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.1019607843137"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="5.87843137254902"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.2" outlineLevel="0" r="1" s="5">
@@ -21803,22 +21694,21 @@
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.42105263157895"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.02024291497976"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.96761133603239"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.9311740890688"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.61133603238866"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.60323886639676"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.5627530364372"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.6558704453441"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.3117408906883"/>
-    <col collapsed="false" hidden="false" max="12" min="10" style="0" width="8.61133603238866"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="11.7894736842105"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="10.2267206477733"/>
-    <col collapsed="false" hidden="false" max="16" min="15" style="0" width="29.5587044534413"/>
-    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="8.61133603238866"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.43921568627451"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.04705882352941"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.0117647058824"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.0039215686275"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.64705882352941"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.64313725490196"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.6117647058824"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.6980392156863"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.3529411764706"/>
+    <col collapsed="false" hidden="false" max="12" min="10" style="0" width="8.64705882352941"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="11.8392156862745"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="10.2705882352941"/>
+    <col collapsed="false" hidden="false" max="16" min="15" style="0" width="29.678431372549"/>
+    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="8.64705882352941"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.2" outlineLevel="0" r="1" s="14">
@@ -22877,12 +22767,11 @@
       <selection activeCell="B12" activeCellId="0" pane="topLeft" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.6315789473684"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.3765182186235"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.5546558704453"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="5.85425101214575"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.6980392156863"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.4313725490196"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.6196078431373"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="5.87843137254902"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="true" ht="12.2" outlineLevel="0" r="1" s="5">
@@ -23055,14 +22944,13 @@
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.6194331983806"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.1902834008097"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.0890688259109"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.6761133603239"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.1902834008097"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="5.85425101214575"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.678431372549"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.2392156862745"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.1411764705882"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.7333333333333"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.2627450980392"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="5.87843137254902"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="true" ht="12.2" outlineLevel="0" r="1" s="5">
@@ -23124,13 +23012,12 @@
       <selection activeCell="A2" activeCellId="0" pane="topLeft" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.4048582995951"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.1295546558704"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="10.1619433198381"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="11.1821862348178"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="5.85425101214575"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.478431372549"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.2274509803922"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="10.2039215686275"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="11.2313725490196"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="5.87843137254902"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="true" ht="12.2" outlineLevel="0" r="1" s="5">
@@ -23258,15 +23145,14 @@
       <selection activeCell="A2" activeCellId="0" pane="topLeft" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0728744939271"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.5141700404858"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="5.85425101214575"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="5.90688259109312"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="5.85425101214575"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.4615384615385"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="5.85425101214575"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.1450980392157"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.6392156862745"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="5.87843137254902"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="5.92941176470588"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="5.87843137254902"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.5372549019608"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="5.87843137254902"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="true" ht="12.2" outlineLevel="0" r="1" s="5">
@@ -23589,23 +23475,22 @@
       <selection activeCell="B3" activeCellId="0" pane="topLeft" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.8461538461538"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.7246963562753"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.6518218623482"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.4372469635628"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.3724696356275"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="5.34008097165992"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.61133603238866"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.5344129554656"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.59919028340081"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="10.9271255060729"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="11.1902834008097"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="10.2672064777328"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="10.004048582996"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="11.4534412955466"/>
-    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="9.34008097165992"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.9294117647059"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.76862745098039"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.7294117647059"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.5176470588235"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.4666666666667"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="5.36470588235294"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.64705882352941"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.5921568627451"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.63921568627451"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="10.9725490196078"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="11.2352941176471"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="10.3098039215686"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="10.0470588235294"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="11.5019607843137"/>
+    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="9.38039215686275"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="18.85" outlineLevel="0" r="1" s="5">
@@ -23736,14 +23621,13 @@
       <selection activeCell="A12" activeCellId="0" pane="topLeft" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.0080971659919"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.4696356275304"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.12550607287449"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.2753036437247"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.54251012145749"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.34008097165992"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.1529411764706"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.5254901960784"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.15294117647059"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.30980392156863"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.57647058823529"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.38039215686275"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="22.6" outlineLevel="0" r="1" s="5">
@@ -23846,22 +23730,21 @@
       <selection activeCell="A9" activeCellId="0" pane="topLeft" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.246963562753"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.63967611336032"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.7246963562753"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.9797570850202"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.2753036437247"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.61133603238866"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.33603238866397"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.3967611336032"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.53441295546559"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="10.9271255060729"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.40485829959514"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="29.0364372469636"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="93.8137651821862"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="9.34008097165992"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.321568627451"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.67843137254902"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.7843137254902"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.0549019607843"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.30980392156863"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.64705882352941"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.36470588235294"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.4392156862745"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.56862745098039"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="10.9725490196078"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.43921568627451"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="29.156862745098"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="94.2039215686274"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="9.38039215686275"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="25.45" outlineLevel="0" r="1">
@@ -23998,14 +23881,13 @@
       <selection activeCell="A21" activeCellId="0" pane="topLeft" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.6437246963563"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.68421052631579"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.46963562753036"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.0404858299595"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="3.27125506072874"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="5.85425101214575"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.756862745098"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.72156862745098"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.50588235294118"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.0980392156863"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="3.28235294117647"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="5.87843137254902"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="true" ht="12.2" outlineLevel="0" r="1" s="5">
@@ -24076,11 +23958,10 @@
       <selection activeCell="A8" activeCellId="0" pane="topLeft" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.3684210526316"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="38.6477732793522"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="5.85425101214575"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.4509803921569"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="38.8078431372549"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="5.87843137254902"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="true" ht="12.2" outlineLevel="0" r="1" s="5">
@@ -24159,22 +24040,21 @@
       <selection activeCell="E4" activeCellId="0" pane="topLeft" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.6599190283401"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.40485829959514"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.1821862348178"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.7408906882591"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.3198380566802"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.5748987854251"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.3967611336032"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.8623481781377"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="6.42105263157895"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.46153846153846"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.7894736842105"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.9271255060729"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="15.1821862348178"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="9.34008097165992"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.7058823529412"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.43921568627451"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.2392156862745"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.7882352941176"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.3647058823529"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.6235294117647"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.4392156862745"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.9098039215686"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="6.44705882352941"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.50196078431373"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.8352941176471"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.9725490196078"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="15.2470588235294"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="9.38039215686275"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="1">
@@ -24295,13 +24175,12 @@
       <selection activeCell="A2" activeCellId="0" pane="topLeft" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.9838056680162"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.5465587044534"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.7449392712551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.6558704453441"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="5.85425101214575"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.0313725490196"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.6392156862745"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.8078431372549"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.7019607843137"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="5.87843137254902"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="true" ht="12.2" outlineLevel="0" r="1" s="5">
@@ -24482,19 +24361,18 @@
       <selection activeCell="A4" activeCellId="0" pane="topLeft" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.3684210526316"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.59919028340081"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.40485829959514"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.1538461538462"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.502024291498"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.66801619433198"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.8623481781377"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.9919028340081"/>
-    <col collapsed="false" hidden="false" max="11" min="9" style="0" width="9.34008097165992"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="11.5748987854251"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="9.34008097165992"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.4274509803922"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.63921568627451"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.43921568627451"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.2235294117647"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.5725490196078"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.70588235294118"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.9176470588235"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.0392156862745"/>
+    <col collapsed="false" hidden="false" max="11" min="9" style="0" width="9.38039215686275"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="11.6235294117647"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="9.38039215686275"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="17.9" outlineLevel="0" r="1">
@@ -24613,20 +24491,19 @@
       <selection activeCell="A12" activeCellId="0" pane="topLeft" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.246963562753"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.63967611336032"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.9797570850202"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="8.2753036437247"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="8.61133603238866"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="7.33603238866397"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.3967611336032"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.53441295546559"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.9271255060729"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.40485829959514"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="29.0364372469636"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="9.34008097165992"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.321568627451"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.67843137254902"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.0549019607843"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="8.30980392156863"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="8.64705882352941"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="7.36470588235294"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.4392156862745"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.56862745098039"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.9725490196078"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.43921568627451"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="29.156862745098"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="9.38039215686275"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="21.65" outlineLevel="0" r="1">
@@ -24833,14 +24710,13 @@
       <selection activeCell="B3" activeCellId="0" pane="topLeft" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.6437246963563"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.68421052631579"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.46963562753036"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.0404858299595"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="3.27125506072874"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="5.85425101214575"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.756862745098"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.72156862745098"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.50588235294118"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.0980392156863"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="3.28235294117647"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="5.87843137254902"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="26.4" outlineLevel="0" r="1" s="5">
@@ -24911,12 +24787,11 @@
       <selection activeCell="A2" activeCellId="0" pane="topLeft" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.2955465587045"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.4817813765182"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.7692307692308"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="5.85425101214575"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.3647058823529"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.5647058823529"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.8274509803922"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="5.87843137254902"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="true" ht="12.2" outlineLevel="0" r="1" s="5">
@@ -24989,11 +24864,10 @@
       <selection activeCell="A2" activeCellId="0" pane="topLeft" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.7975708502024"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.0971659919028"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="5.85425101214575"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.8705882352941"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.1686274509804"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="5.87843137254902"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="true" ht="12.2" outlineLevel="0" r="1" s="5">
@@ -25069,14 +24943,13 @@
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.4372469635628"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.4817813765182"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.7327935222672"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="10.5465587044534"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.0404858299595"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="5.85425101214575"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.5294117647059"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.5450980392157"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.7764705882353"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="10.5921568627451"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.0823529411765"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="5.87843137254902"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.2" outlineLevel="0" r="1" s="5">
@@ -25466,15 +25339,14 @@
       <selection activeCell="B30" activeCellId="0" pane="topLeft" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="true" max="1" min="1" style="0" width="0"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.6720647773279"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.68421052631579"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.8785425101215"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.4372469635628"/>
-    <col collapsed="false" hidden="false" max="1023" min="6" style="0" width="5.85425101214575"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="5.01214574898785"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.7843137254902"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.71372549019608"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.9803921568627"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.521568627451"/>
+    <col collapsed="false" hidden="false" max="1023" min="6" style="0" width="5.87843137254902"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="5.03529411764706"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="true" ht="12.2" outlineLevel="0" r="1" s="5">
@@ -25924,17 +25796,16 @@
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.0404858299595"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.76923076923077"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="10.0404858299595"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="7.07692307692308"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.50607287449393"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="8.53441295546559"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="6.68421052631579"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="10.0404858299595"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.20647773279352"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.0823529411765"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.80392156862745"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="10.0823529411765"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="7.10588235294118"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.54117647058824"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="8.56862745098039"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="6.71372549019608"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="10.0823529411765"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.23921568627451"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="44.75" outlineLevel="0" r="1" s="76">
@@ -27195,15 +27066,14 @@
       <selection activeCell="G6" activeCellId="0" pane="topLeft" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.61133603238866"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.97165991902834"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.1538461538462"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="6.69230769230769"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.3603238866397"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.582995951417"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="38" width="9.18218623481781"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.64705882352941"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.00392156862745"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.2039215686275"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="6.71764705882353"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.4117647058824"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.6509803921569"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="38" width="9.22352941176471"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="13.4" outlineLevel="0" r="1">
@@ -27371,31 +27241,30 @@
       <selection activeCell="A2" activeCellId="0" pane="topLeft" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.8744939271255"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.50607287449393"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="8.06882591093117"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.4251012145749"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="12.2753036437247"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.8097165991903"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.5546558704453"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="9.81376518218623"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.59919028340081"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="11.5546558704453"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="10.3400809716599"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="7.79757085020243"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="8.59919028340081"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="7.38461538461539"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="10.3400809716599"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="10.4817813765182"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="8.53441295546559"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="8.7246963562753"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="7.51417004048583"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="10.4817813765182"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="11.1457489878543"/>
-    <col collapsed="false" hidden="false" max="1025" min="25" style="0" width="7.51417004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.9411764705882"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.54117647058824"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="8.10196078431373"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.4980392156863"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="12.3254901960784"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.8901960784314"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.6039215686275"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.03529411764706"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="9.85098039215686"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.63529411764706"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="11.6039215686275"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="10.3843137254902"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="7.83137254901961"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="8.63529411764706"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="7.4156862745098"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="10.3843137254902"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="10.5254901960784"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="8.56862745098039"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="8.76470588235294"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="7.54509803921569"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="10.5254901960784"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="11.1921568627451"/>
+    <col collapsed="false" hidden="false" max="1025" min="25" style="0" width="7.54509803921569"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="true" ht="12.2" outlineLevel="0" r="1" s="39">
@@ -27828,22 +27697,21 @@
       <selection activeCell="C24" activeCellId="0" pane="topLeft" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.1052631578947"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.8502024291498"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.66396761133603"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.51821862348178"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="10.1821862348178"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.412955465587"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.4210526315789"/>
-    <col collapsed="false" hidden="false" max="12" min="9" style="0" width="8.46963562753036"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="16.4453441295547"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="12.2753036437247"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="22.2793522267206"/>
-    <col collapsed="false" hidden="false" max="26" min="16" style="0" width="7.54655870445344"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="8.93522267206478"/>
-    <col collapsed="false" hidden="false" max="1025" min="28" style="0" width="5.85425101214575"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.1490196078431"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.87843137254902"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.69803921568627"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.55686274509804"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="10.2274509803922"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.4588235294118"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.4627450980392"/>
+    <col collapsed="false" hidden="false" max="12" min="9" style="0" width="8.50588235294118"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="16.5137254901961"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="12.3254901960784"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="22.3725490196078"/>
+    <col collapsed="false" hidden="false" max="26" min="16" style="0" width="7.58039215686275"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="8.97254901960784"/>
+    <col collapsed="false" hidden="false" max="1025" min="28" style="0" width="5.87843137254902"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="true" ht="12.2" outlineLevel="0" r="1" s="14">
@@ -28485,11 +28353,10 @@
       <selection activeCell="A4" activeCellId="0" pane="topLeft" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.1012145748988"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.9514170040486"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="5.85425101214575"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.1764705882353"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.0313725490196"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="5.87843137254902"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="19.8" outlineLevel="0" r="1" s="5">

</xml_diff>

<commit_message>
the test setupdata now disables the ShowNewPricingInfo field
</commit_message>
<xml_diff>
--- a/bika/lims/setupdata/test/test.xlsx
+++ b/bika/lims/setupdata/test/test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="44" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="901" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="57" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="593" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" state="visible" r:id="rId2"/>
@@ -96,15 +96,15 @@
             <anchor moveWithCells="false" sizeWithCells="false">
               <xdr:from>
                 <xdr:col>6</xdr:col>
-                <xdr:colOff>70</xdr:colOff>
-                <xdr:row>1</xdr:row>
+                <xdr:colOff>3</xdr:colOff>
+                <xdr:row>-1</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </xdr:from>
               <xdr:to>
                 <xdr:col>12</xdr:col>
-                <xdr:colOff>61</xdr:colOff>
+                <xdr:colOff>3</xdr:colOff>
                 <xdr:row>2</xdr:row>
-                <xdr:rowOff>5</xdr:rowOff>
+                <xdr:rowOff>2</xdr:rowOff>
               </xdr:to>
             </anchor>
           </commentPr>
@@ -142,13 +142,13 @@
             <anchor moveWithCells="false" sizeWithCells="false">
               <xdr:from>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>198</xdr:colOff>
+                <xdr:colOff>197</xdr:colOff>
                 <xdr:row>-1</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </xdr:from>
               <xdr:to>
                 <xdr:col>6</xdr:col>
-                <xdr:colOff>29</xdr:colOff>
+                <xdr:colOff>26</xdr:colOff>
                 <xdr:row>5</xdr:row>
                 <xdr:rowOff>17</xdr:rowOff>
               </xdr:to>
@@ -188,13 +188,13 @@
             <anchor moveWithCells="false" sizeWithCells="false">
               <xdr:from>
                 <xdr:col>2</xdr:col>
-                <xdr:colOff>72</xdr:colOff>
+                <xdr:colOff>71</xdr:colOff>
                 <xdr:row>-1</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </xdr:from>
               <xdr:to>
                 <xdr:col>6</xdr:col>
-                <xdr:colOff>41</xdr:colOff>
+                <xdr:colOff>39</xdr:colOff>
                 <xdr:row>11</xdr:row>
                 <xdr:rowOff>12</xdr:rowOff>
               </xdr:to>
@@ -234,14 +234,14 @@
               <xdr:from>
                 <xdr:col>7</xdr:col>
                 <xdr:colOff>3</xdr:colOff>
-                <xdr:row>14</xdr:row>
-                <xdr:rowOff>13</xdr:rowOff>
+                <xdr:row>13</xdr:row>
+                <xdr:rowOff>14</xdr:rowOff>
               </xdr:from>
               <xdr:to>
                 <xdr:col>9</xdr:col>
                 <xdr:colOff>3</xdr:colOff>
-                <xdr:row>26</xdr:row>
-                <xdr:rowOff>3</xdr:rowOff>
+                <xdr:row>25</xdr:row>
+                <xdr:rowOff>4</xdr:rowOff>
               </xdr:to>
             </anchor>
           </commentPr>
@@ -269,14 +269,14 @@
               <xdr:from>
                 <xdr:col>17</xdr:col>
                 <xdr:colOff>3</xdr:colOff>
-                <xdr:row>6</xdr:row>
+                <xdr:row>5</xdr:row>
                 <xdr:rowOff>17</xdr:rowOff>
               </xdr:from>
               <xdr:to>
                 <xdr:col>24</xdr:col>
                 <xdr:colOff>3</xdr:colOff>
-                <xdr:row>12</xdr:row>
-                <xdr:rowOff>14</xdr:rowOff>
+                <xdr:row>11</xdr:row>
+                <xdr:rowOff>15</xdr:rowOff>
               </xdr:to>
             </anchor>
           </commentPr>
@@ -289,7 +289,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3662" uniqueCount="1449">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3663" uniqueCount="1450">
   <si>
     <t>Instructions</t>
   </si>
@@ -3934,6 +3934,9 @@
   </si>
   <si>
     <t>Id server url</t>
+  </si>
+  <si>
+    <t>ShowNewReleasesInfo</t>
   </si>
   <si>
     <t>AR Import options</t>
@@ -4919,7 +4922,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="146">
+  <cellXfs count="147">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
@@ -5302,6 +5305,7 @@
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
     </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="9" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
     </xf>
@@ -5410,9 +5414,9 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="96.4117647058824"/>
-    <col collapsed="false" hidden="false" max="1023" min="2" style="0" width="8.7921568627451"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="8.82745098039216"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="96.8156862745098"/>
+    <col collapsed="false" hidden="false" max="1023" min="2" style="0" width="8.82745098039216"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="8.86274509803922"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="32.05" outlineLevel="0" r="1" s="3">
@@ -5480,9 +5484,9 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.4941176470588"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.3450980392157"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.54117647058824"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.5725490196078"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.4274509803922"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57647058823529"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="19.8" outlineLevel="0" r="1" s="5">
@@ -5530,9 +5534,9 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.4941176470588"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.3450980392157"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.54117647058824"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.5725490196078"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.4274509803922"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57647058823529"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="12.2" outlineLevel="0" r="1" s="5">
@@ -5631,10 +5635,10 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.2039215686275"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.8352941176471"/>
-    <col collapsed="false" hidden="false" max="5" min="3" style="0" width="14.1254901960784"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.54117647058824"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.2823529411765"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.8941176470588"/>
+    <col collapsed="false" hidden="false" max="5" min="3" style="0" width="14.1843137254902"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57647058823529"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="19.8" outlineLevel="0" r="1" s="5">
@@ -5967,18 +5971,18 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.25882352941177"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.62745098039216"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.83529411764706"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.2823529411765"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.57647058823529"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.57254901960784"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.2823529411765"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.47450980392157"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="7.04313725490196"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="7.57254901960784"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="24.2392156862745"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="9.34509803921569"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.30196078431373"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.65490196078431"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.86274509803922"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.3764705882353"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.61176470588235"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.6078431372549"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.3372549019608"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.51764705882353"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="7.07058823529412"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="7.6"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="24.3372549019608"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="9.38039215686275"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="12.2" outlineLevel="0" r="1" s="5">
@@ -6154,11 +6158,11 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.2823529411765"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="39" width="10.3843137254902"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="39" width="11.9450980392157"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="39" width="12.1607843137255"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57647058823529"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.3333333333333"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="39" width="10.4274509803922"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="39" width="11.9882352941176"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="39" width="12.2117647058824"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.61176470588235"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="12.2" outlineLevel="0" r="1" s="5">
@@ -6332,13 +6336,13 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.2666666666667"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.9098039215686"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.71764705882353"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.3843137254902"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.4"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.2039215686275"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.54117647058824"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.3490196078431"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.0039215686274"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.74901960784314"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.4509803921569"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.4627450980392"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.2666666666667"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57647058823529"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="12.2" outlineLevel="0" r="1" s="5">
@@ -6557,9 +6561,9 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.2392156862745"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.5843137254902"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.54117647058824"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.2901960784314"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.6627450980392"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57647058823529"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="12.2" outlineLevel="0" r="1" s="5">
@@ -6666,16 +6670,16 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3372549019608"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.9725490196078"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.71764705882353"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="4.65490196078431"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.68235294117647"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.81176470588235"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.50980392156863"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.2352941176471"/>
-    <col collapsed="false" hidden="false" max="1023" min="9" style="0" width="6.81176470588235"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="5.8078431372549"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3882352941176"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.0823529411765"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.74901960784314"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="4.67450980392157"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.72156862745098"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.83921568627451"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.54509803921569"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.2901960784314"/>
+    <col collapsed="false" hidden="false" max="1023" min="9" style="0" width="6.83921568627451"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="5.83529411764706"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="13.2" outlineLevel="0" r="1" s="15">
@@ -7102,14 +7106,14 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="12.921568627451"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.9843137254902"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.6352941176471"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="17.6470588235294"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.63529411764706"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.1843137254902"/>
-    <col collapsed="false" hidden="false" max="1018" min="9" style="0" width="8.54117647058824"/>
-    <col collapsed="false" hidden="false" max="1025" min="1019" style="0" width="5.68627450980392"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="12.9803921568627"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.0901960784314"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.7098039215686"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="17.7176470588235"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.66666666666667"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.2274509803922"/>
+    <col collapsed="false" hidden="false" max="1018" min="9" style="0" width="8.57647058823529"/>
+    <col collapsed="false" hidden="false" max="1025" min="1019" style="0" width="5.71372549019608"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="12.2" outlineLevel="0" r="1" s="5">
@@ -7378,11 +7382,11 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.8862745098039"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.6549019607843"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.0196078431373"/>
-    <col collapsed="false" hidden="false" max="1018" min="4" style="0" width="8.54117647058824"/>
-    <col collapsed="false" hidden="false" max="1025" min="1019" style="0" width="5.12156862745098"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.9686274509804"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.7490196078431"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.0823529411765"/>
+    <col collapsed="false" hidden="false" max="1018" min="4" style="0" width="8.57647058823529"/>
+    <col collapsed="false" hidden="false" max="1025" min="1019" style="0" width="5.14117647058824"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="12.2" outlineLevel="0" r="1" s="15">
@@ -7451,10 +7455,10 @@
   </sheetViews>
   <cols>
     <col collapsed="false" hidden="true" max="1" min="1" style="0" width="0"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.7764705882353"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.36078431372549"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="4.75294117647059"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="6.7843137254902"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.8392156862745"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.38823529411765"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="4.77647058823529"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="6.81176470588235"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="12.2" outlineLevel="0" r="1" s="5">
@@ -7648,10 +7652,10 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.5686274509804"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="56.3843137254902"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.9843137254902"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.54117647058824"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.6313725490196"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="56.6196078431373"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.0901960784314"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57647058823529"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="12.2" outlineLevel="0" r="1" s="15">
@@ -7840,9 +7844,9 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.9490196078431"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.9019607843137"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.54117647058824"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.0470588235294"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.9725490196078"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57647058823529"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="12.2" outlineLevel="0" r="1" s="5">
@@ -7980,11 +7984,11 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.7882352941176"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="9.68235294117647"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.4549019607843"/>
-    <col collapsed="false" hidden="false" max="21" min="6" style="0" width="9.68235294117647"/>
-    <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="16.7882352941176"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.8588235294118"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="9.72549019607843"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.5176470588235"/>
+    <col collapsed="false" hidden="false" max="21" min="6" style="0" width="9.72549019607843"/>
+    <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="16.8588235294118"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="12.2" outlineLevel="0" r="1" s="5">
@@ -8210,9 +8214,9 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.0039215686274"/>
-    <col collapsed="false" hidden="false" max="21" min="2" style="0" width="8.10196078431373"/>
-    <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="8.54117647058824"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.0980392156863"/>
+    <col collapsed="false" hidden="false" max="21" min="2" style="0" width="8.13333333333333"/>
+    <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="8.57647058823529"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="12.2" outlineLevel="0" r="1" s="5">
@@ -8488,10 +8492,10 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.7843137254902"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.6549019607843"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="7.70196078431373"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="7.66666666666667"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.878431372549"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.7764705882353"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="7.72941176470588"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="7.70196078431373"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="13.4" outlineLevel="0" r="1">
@@ -8608,18 +8612,18 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.2666666666667"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.8862745098039"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.4039215686275"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.2588235294118"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.7647058823529"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.1529411764706"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.1882352941176"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.4823529411765"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.5058823529412"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="7.70196078431373"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="11.4078431372549"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.54117647058824"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.3490196078431"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.9882352941176"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.4745098039216"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.3333333333333"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.8196078431373"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.2470588235294"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.2313725490196"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.5294117647059"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.556862745098"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="7.72941176470588"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="11.4588235294118"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.57647058823529"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="13.4" outlineLevel="0" r="1" s="86">
@@ -9728,15 +9732,15 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.443137254902"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.6509803921569"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.7843137254902"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.55686274509804"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.5607843137255"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.4549019607843"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.9019607843137"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="29.0274509803922"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="7.70196078431373"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.5058823529412"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.721568627451"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.8274509803922"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.6"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.6156862745098"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.5254901960784"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.9725490196078"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="29.1490196078431"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="7.72941176470588"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="15.1" outlineLevel="0" r="1" s="86">
@@ -9870,15 +9874,15 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.443137254902"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.7254901960784"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.7843137254902"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.55686274509804"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.5607843137255"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.4549019607843"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.9019607843137"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="29.0274509803922"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="7.70196078431373"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.5058823529412"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.7764705882353"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.8274509803922"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.6"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.6156862745098"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.5254901960784"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.9725490196078"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="29.1490196078431"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="7.72941176470588"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="15.1" outlineLevel="0" r="1" s="86">
@@ -10009,14 +10013,14 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.121568627451"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.0156862745098"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.70196078431373"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.3607843137255"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.443137254902"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.6470588235294"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.9725490196078"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="7.70196078431373"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1803921568627"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.0980392156863"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.72941176470588"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.4117647058824"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.4862745098039"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.7098039215686"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.0823529411765"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="7.72941176470588"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="14.9" outlineLevel="0" r="1">
@@ -10995,17 +10999,17 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.2196078431373"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.2392156862745"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.3372549019608"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.2274509803922"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.3372549019608"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="7.70196078431373"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.3411764705882"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.4"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.4901960784314"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="5.32941176470588"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="7.70196078431373"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.278431372549"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.3372549019608"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.4156862745098"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.2705882352941"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.3803921568627"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="7.72941176470588"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.4"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.4627450980392"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.5529411764706"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="5.34901960784314"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="7.72941176470588"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="14.9" outlineLevel="0" r="1" s="86">
@@ -11222,9 +11226,9 @@
   </sheetViews>
   <cols>
     <col collapsed="false" hidden="true" max="1" min="1" style="0" width="0"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.121568627451"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.6039215686275"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="6.81176470588235"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.2588235294118"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.6745098039216"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="6.83921568627451"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="12.2" outlineLevel="0" r="1" s="5">
@@ -11623,17 +11627,17 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.5686274509804"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.8549019607843"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.8901960784314"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.2274509803922"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.3372549019608"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.9960784313725"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.4"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.5529411764706"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="27.9019607843137"/>
-    <col collapsed="false" hidden="false" max="1023" min="10" style="0" width="7.70196078431373"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="7.66666666666667"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.6392156862745"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.9411764705882"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.9725490196078"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.2705882352941"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.3803921568627"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.0588235294118"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.4627450980392"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.6039215686275"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="28.0156862745098"/>
+    <col collapsed="false" hidden="false" max="1023" min="10" style="0" width="7.72941176470588"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="7.70196078431373"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="14.9" outlineLevel="0" r="1" s="86">
@@ -11725,10 +11729,10 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.1058823529412"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.7333333333333"/>
-    <col collapsed="false" hidden="false" max="5" min="3" style="0" width="21.1450980392157"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.54117647058824"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.2274509803922"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.8705882352941"/>
+    <col collapsed="false" hidden="false" max="5" min="3" style="0" width="21.2313725490196"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57647058823529"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="12.2" outlineLevel="0" r="1" s="5">
@@ -11827,10 +11831,10 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.3529411764706"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="46.9607843137255"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="47.5490196078431"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="6.38039215686275"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.4235294117647"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="47.156862745098"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="47.7490196078431"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="6.40392156862745"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="14.15" outlineLevel="0" r="1" s="105">
@@ -11964,10 +11968,10 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="25.0352941176471"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="7.2078431372549"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="3.33333333333333"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.54117647058824"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="25.1411764705882"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="7.23529411764706"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="3.34901960784314"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57647058823529"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="12.2" outlineLevel="0" r="1" s="5">
@@ -12571,28 +12575,28 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.9529411764706"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="29.2862745098039"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.32549019607843"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="5.27058823529412"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.6470588235294"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.3098039215686"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.1411764705882"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="7.3843137254902"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="6.10980392156863"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="7.66666666666667"/>
-    <col collapsed="false" hidden="false" max="14" min="12" style="0" width="3.66274509803922"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="3.94509803921569"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="6.43137254901961"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="3.33333333333333"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="13.5333333333333"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="9.70980392156863"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="13.4313725490196"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="11.4588235294118"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="9.22352941176471"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="8.36078431372549"/>
-    <col collapsed="false" hidden="false" max="25" min="24" style="0" width="10.7294117647059"/>
-    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="7.66666666666667"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.0392156862745"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="29.4078431372549"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.36078431372549"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="5.29019607843137"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.7176470588235"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.3529411764706"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.1843137254902"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="7.4156862745098"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="6.12941176470588"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="7.70196078431373"/>
+    <col collapsed="false" hidden="false" max="14" min="12" style="0" width="3.67843137254902"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="3.95686274509804"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="6.46274509803922"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="3.34901960784314"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="13.5882352941176"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="9.74509803921569"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="13.4901960784314"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="11.5019607843137"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="9.25882352941177"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="8.39607843137255"/>
+    <col collapsed="false" hidden="false" max="25" min="24" style="0" width="10.7725490196078"/>
+    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="7.70196078431373"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="24.1" outlineLevel="0" r="1" s="15">
@@ -14493,12 +14497,12 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.2156862745098"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.86274509803922"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.64705882352941"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.3411764705882"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="3.33333333333333"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.54117647058824"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.3333333333333"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.89803921568628"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.68235294117647"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.4"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="3.34901960784314"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57647058823529"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="12.2" outlineLevel="0" r="1" s="5">
@@ -14564,12 +14568,12 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.5686274509804"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.6509803921569"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.54117647058824"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.3411764705882"/>
-    <col collapsed="false" hidden="false" max="973" min="5" style="0" width="8.54117647058824"/>
-    <col collapsed="false" hidden="false" max="1025" min="974" style="0" width="5.12156862745098"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.6117647058824"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.7019607843137"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.57647058823529"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.4"/>
+    <col collapsed="false" hidden="false" max="973" min="5" style="0" width="8.57647058823529"/>
+    <col collapsed="false" hidden="false" max="1025" min="974" style="0" width="5.14117647058824"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="24.5" outlineLevel="0" r="1" s="15">
@@ -14772,11 +14776,11 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.1764705882353"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="9.46666666666667"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.76862745098039"/>
-    <col collapsed="false" hidden="false" max="997" min="5" style="0" width="8.54117647058824"/>
-    <col collapsed="false" hidden="false" max="1025" min="998" style="0" width="5.12156862745098"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.3294117647059"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="9.50196078431373"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.8078431372549"/>
+    <col collapsed="false" hidden="false" max="997" min="5" style="0" width="8.57647058823529"/>
+    <col collapsed="false" hidden="false" max="1025" min="998" style="0" width="5.14117647058824"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="24.5" outlineLevel="0" r="1" s="15">
@@ -16248,13 +16252,13 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0235294117647"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.678431372549"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.2352941176471"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.9882352941176"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.6627450980392"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="5.49411764705882"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.54117647058824"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0941176470588"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.7450980392157"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.3490196078431"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.0392156862745"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.7058823529412"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="5.51372549019608"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57647058823529"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="12.2" outlineLevel="0" r="1" s="41">
@@ -16400,10 +16404,10 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.4"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.7725490196078"/>
-    <col collapsed="false" hidden="false" max="6" min="3" style="0" width="29.3921568627451"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.54117647058824"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.4941176470588"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.8862745098039"/>
+    <col collapsed="false" hidden="false" max="6" min="3" style="0" width="29.5137254901961"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57647058823529"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.2" outlineLevel="0" r="1" s="41">
@@ -16612,20 +16616,20 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.50980392156863"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.16470588235294"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.1843137254902"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.2901960784314"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.7921568627451"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.8078431372549"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.8196078431373"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.8705882352941"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.5254901960784"/>
-    <col collapsed="false" hidden="false" max="12" min="10" style="0" width="8.7921568627451"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="12.0392156862745"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="10.4392156862745"/>
-    <col collapsed="false" hidden="false" max="16" min="15" style="0" width="30.1803921568627"/>
-    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="8.7921568627451"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.53333333333333"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.1921568627451"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.2274509803922"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.3607843137255"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.82745098039216"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.85098039215686"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.8705882352941"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.9137254901961"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.5686274509804"/>
+    <col collapsed="false" hidden="false" max="12" min="10" style="0" width="8.82745098039216"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="12.0901960784314"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="10.4823529411765"/>
+    <col collapsed="false" hidden="false" max="16" min="15" style="0" width="30.3058823529412"/>
+    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="8.82745098039216"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.2" outlineLevel="0" r="1" s="15">
@@ -17685,13 +17689,13 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.4"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.63921568627451"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.7647058823529"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.1137254901961"/>
-    <col collapsed="false" hidden="false" max="7" min="5" style="0" width="10.1333333333333"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.5803921568627"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.54117647058824"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.4627450980392"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.68235294117647"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.8196078431373"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.2"/>
+    <col collapsed="false" hidden="false" max="7" min="5" style="0" width="10.1764705882353"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.6235294117647"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.57647058823529"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="15.05" outlineLevel="0" r="1" s="5">
@@ -23176,14 +23180,14 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.3333333333333"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.8705882352941"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.4627450980392"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="10.2549019607843"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.7764705882353"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.521568627451"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.321568627451"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.54117647058824"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.4352941176471"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.9137254901961"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.5137254901961"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="10.2980392156863"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.8392156862745"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.5843137254902"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.3725490196078"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.57647058823529"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.2" outlineLevel="0" r="1" s="5">
@@ -23338,10 +23342,10 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.956862745098"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.6588235294118"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.8745098039216"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.54117647058824"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.0196078431373"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.7176470588235"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.9411764705882"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.57647058823529"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="12.2" outlineLevel="0" r="1" s="5">
@@ -23515,12 +23519,12 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.9294117647059"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.443137254902"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.3411764705882"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.9607843137255"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.5725490196078"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.54117647058824"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.9960784313725"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.4901960784314"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.3921568627451"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.0196078431373"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.6509803921569"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57647058823529"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="12.2" outlineLevel="0" r="1" s="5">
@@ -23583,11 +23587,11 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.7882352941176"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.6196078431373"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="10.3764705882353"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="11.4078431372549"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.54117647058824"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.8666666666667"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.7137254901961"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="10.4196078431373"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="11.4588235294118"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57647058823529"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="12.2" outlineLevel="0" r="1" s="5">
@@ -23731,18 +23735,18 @@
   </sheetPr>
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A2" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
-      <selection activeCell="A28" activeCellId="0" pane="topLeft" sqref="A28"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A2" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
+      <selection activeCell="B26" activeCellId="0" pane="topLeft" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.4313725490196"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.156862745098"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.54117647058824"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="8.61176470588235"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.54117647058824"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.8509803921569"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.54117647058824"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.5058823529412"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.2862745098039"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.57647058823529"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="8.64705882352941"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.57647058823529"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.9294117647059"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.57647058823529"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="12.2" outlineLevel="0" r="1" s="5">
@@ -24168,21 +24172,20 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.2666666666667"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.93333333333333"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.0470588235294"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.8470588235294"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.8392156862745"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="5.45098039215686"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.7921568627451"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.8352941176471"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.8078431372549"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="11.1490196078431"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="11.4078431372549"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="10.4823529411765"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="10.2196078431373"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="11.7019607843137"/>
-    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="9.54509803921569"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.3490196078431"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.1254901960784"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.9294117647059"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.9333333333333"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="5.47058823529412"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.82745098039216"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.8941176470588"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.85098039215686"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="11.1921568627451"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="11.4588235294118"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="10.5254901960784"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="10.2627450980392"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="11.7450980392157"/>
+    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="9.58823529411765"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="18.85" outlineLevel="0" r="1" s="5">
@@ -24314,12 +24317,12 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.7411764705882"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.7450980392157"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.26666666666667"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.44705882352941"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.72156862745098"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.54509803921569"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.8901960784314"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.8039215686275"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.29411764705882"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.48235294117647"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.75686274509804"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.58823529411765"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="22.6" outlineLevel="0" r="1" s="5">
@@ -24423,20 +24426,20 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.6235294117647"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.81960784313726"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.0117647058824"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.356862745098"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.44705882352941"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.7921568627451"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.48627450980392"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.6117647058824"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.71372549019608"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.1490196078431"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.57647058823529"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="29.643137254902"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="95.7725490196078"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="9.54509803921569"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.7019607843137"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.85490196078431"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.0705882352941"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.4274509803922"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.48235294117647"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.82745098039216"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.51372549019608"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.6549019607843"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.74901960784314"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.1921568627451"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.61176470588235"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="29.7647058823529"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="96.1686274509804"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="9.58823529411765"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="25.45" outlineLevel="0" r="1">
@@ -24574,12 +24577,12 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.2156862745098"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.86274509803922"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.64705882352941"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.3411764705882"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="3.33333333333333"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.54117647058824"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.3333333333333"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.89803921568628"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.68235294117647"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.4"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="3.34901960784314"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57647058823529"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="12.2" outlineLevel="0" r="1" s="5">
@@ -24651,11 +24654,11 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.2352941176471"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.0117647058824"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.0588235294118"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.8980392156863"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.54117647058824"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.2823529411765"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.1058823529412"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.121568627451"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.9450980392157"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57647058823529"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="12.2" outlineLevel="0" r="1" s="5">
@@ -24843,9 +24846,9 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.7960784313725"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="39.4627450980392"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.54117647058824"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.8823529411765"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="39.6274509803922"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57647058823529"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="12.2" outlineLevel="0" r="1" s="5">
@@ -24925,20 +24928,20 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.878431372549"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.57647058823529"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.4666666666667"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.9882352941176"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.5529411764706"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.8235294117647"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.6117647058824"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.1098039215686"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="6.56078431372549"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.66666666666667"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="11.0156862745098"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="11.1490196078431"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="15.5019607843137"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="9.54509803921569"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.921568627451"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.61176470588235"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.5254901960784"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.0392156862745"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.6039215686275"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.8666666666667"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.6549019607843"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.1607843137255"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="6.58823529411765"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.70980392156863"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="11.0627450980392"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="11.1921568627451"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="15.5686274509804"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="9.58823529411765"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="1">
@@ -25060,17 +25063,17 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.678431372549"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.8078431372549"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.57647058823529"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.5098039215686"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.8509803921569"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.84705882352941"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.156862745098"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.2392156862745"/>
-    <col collapsed="false" hidden="false" max="11" min="9" style="0" width="9.54509803921569"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="11.8235294117647"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="9.54509803921569"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.7450980392157"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.85098039215686"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.61176470588235"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.5843137254902"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.921568627451"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.88627450980392"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.2196078431373"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.2901960784314"/>
+    <col collapsed="false" hidden="false" max="11" min="9" style="0" width="9.58823529411765"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="11.8666666666667"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="9.58823529411765"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="17.9" outlineLevel="0" r="1">
@@ -25190,18 +25193,18 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.6235294117647"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.81960784313726"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.356862745098"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="8.44705882352941"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="8.7921568627451"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="7.48627450980392"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.6117647058824"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.71372549019608"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="11.1490196078431"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.57647058823529"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="29.643137254902"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="9.54509803921569"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.7019607843137"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.85490196078431"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.4274509803922"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="8.48235294117647"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="8.82745098039216"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="7.51372549019608"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.6549019607843"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.74901960784314"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="11.1921568627451"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.61176470588235"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="29.7647058823529"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="9.58823529411765"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="21.65" outlineLevel="0" r="1">
@@ -25409,12 +25412,12 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.2156862745098"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.86274509803922"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.64705882352941"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.3411764705882"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="3.33333333333333"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.54117647058824"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.3333333333333"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.89803921568628"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.68235294117647"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.4"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="3.34901960784314"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57647058823529"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="26.4" outlineLevel="0" r="1" s="5">
@@ -25486,10 +25489,10 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.6352941176471"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.9019607843137"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.078431372549"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.54117647058824"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.7098039215686"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.9882352941176"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.1372549019608"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.57647058823529"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="12.2" outlineLevel="0" r="1" s="5">
@@ -25563,9 +25566,9 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.156862745098"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.4549019607843"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.54117647058824"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.2352941176471"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.5254901960784"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57647058823529"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="12.2" outlineLevel="0" r="1" s="5">
@@ -25642,12 +25645,12 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.9098039215686"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.8039215686275"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.9490196078431"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="10.7725490196078"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.2549019607843"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.54117647058824"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.0039215686274"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.8705882352941"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.9921568627451"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="10.8196078431373"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.2980392156863"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57647058823529"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.2" outlineLevel="0" r="1" s="5">
@@ -26031,20 +26034,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
-      <selection activeCell="B30" activeCellId="0" pane="topLeft" sqref="B30"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
+      <selection activeCell="C32" activeCellId="0" pane="topLeft" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <cols>
     <col collapsed="false" hidden="true" max="1" min="1" style="0" width="0"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.2352941176471"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.82745098039216"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.3803921568627"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.8666666666667"/>
-    <col collapsed="false" hidden="false" max="1023" min="6" style="0" width="8.54117647058824"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="5.12156862745098"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.3490196078431"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.85490196078431"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.4823529411765"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.9529411764706"/>
+    <col collapsed="false" hidden="false" max="1023" min="6" style="0" width="8.57647058823529"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="5.14117647058824"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="12.2" outlineLevel="0" r="1" s="5">
@@ -26370,6 +26373,14 @@
         <v>1214</v>
       </c>
       <c r="C30" s="132"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.4" outlineLevel="0" r="31">
+      <c r="B31" s="0" t="s">
+        <v>1215</v>
+      </c>
+      <c r="C31" s="138" t="n">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="24">
@@ -26495,47 +26506,47 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.2549019607843"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.94901960784314"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="10.2549019607843"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="7.21960784313726"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.68235294117647"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="8.71372549019608"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="6.82745098039216"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="10.2549019607843"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.37647058823529"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.2980392156863"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.9843137254902"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="10.2980392156863"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="7.25098039215686"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.72156862745098"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="8.74901960784314"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="6.85490196078431"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="10.2980392156863"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.41176470588235"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="44.75" outlineLevel="0" r="1" s="77">
-      <c r="A1" s="138" t="s">
+      <c r="A1" s="139" t="s">
         <v>123</v>
       </c>
-      <c r="B1" s="138" t="s">
+      <c r="B1" s="139" t="s">
         <v>122</v>
       </c>
       <c r="C1" s="78" t="s">
-        <v>1215</v>
+        <v>1216</v>
       </c>
       <c r="D1" s="78" t="s">
-        <v>1216</v>
+        <v>1217</v>
       </c>
       <c r="E1" s="78" t="s">
-        <v>1217</v>
+        <v>1218</v>
       </c>
       <c r="F1" s="77" t="s">
-        <v>1218</v>
-      </c>
-      <c r="G1" s="139" t="s">
         <v>1219</v>
       </c>
+      <c r="G1" s="140" t="s">
+        <v>1220</v>
+      </c>
       <c r="H1" s="78" t="s">
-        <v>1220</v>
+        <v>1221</v>
       </c>
       <c r="I1" s="78" t="s">
-        <v>1221</v>
+        <v>1222</v>
       </c>
       <c r="J1" s="78" t="s">
-        <v>1222</v>
+        <v>1223</v>
       </c>
       <c r="K1" s="78" t="s">
         <v>868</v>
@@ -26553,25 +26564,25 @@
         <v>1187</v>
       </c>
       <c r="D2" s="110" t="s">
-        <v>1223</v>
-      </c>
-      <c r="E2" s="140" t="s">
         <v>1224</v>
       </c>
+      <c r="E2" s="141" t="s">
+        <v>1225</v>
+      </c>
       <c r="F2" s="110" t="s">
-        <v>1225</v>
+        <v>1226</v>
       </c>
       <c r="G2" s="110" t="n">
         <v>0</v>
       </c>
       <c r="H2" s="110" t="s">
-        <v>1226</v>
+        <v>1227</v>
       </c>
       <c r="I2" s="110" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
       <c r="J2" s="110" t="s">
-        <v>1228</v>
+        <v>1229</v>
       </c>
       <c r="K2" s="110" t="s">
         <v>885</v>
@@ -26579,34 +26590,34 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="3">
       <c r="A3" s="31" t="s">
-        <v>1229</v>
+        <v>1230</v>
       </c>
       <c r="B3" s="31" t="s">
         <v>170</v>
       </c>
       <c r="C3" s="110" t="s">
-        <v>1230</v>
+        <v>1231</v>
       </c>
       <c r="D3" s="110" t="s">
         <v>319</v>
       </c>
-      <c r="E3" s="140" t="s">
+      <c r="E3" s="141" t="s">
         <v>1203</v>
       </c>
       <c r="F3" s="110" t="s">
-        <v>1231</v>
+        <v>1232</v>
       </c>
       <c r="G3" s="110" t="n">
         <v>1</v>
       </c>
       <c r="H3" s="110" t="s">
-        <v>1232</v>
+        <v>1233</v>
       </c>
       <c r="I3" s="110" t="s">
         <v>21</v>
       </c>
       <c r="J3" s="110" t="s">
-        <v>1233</v>
+        <v>1234</v>
       </c>
       <c r="K3" s="110" t="s">
         <v>893</v>
@@ -26614,21 +26625,21 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="24.5" outlineLevel="0" r="4">
       <c r="A4" s="31" t="s">
-        <v>1234</v>
+        <v>1235</v>
       </c>
       <c r="B4" s="31" t="s">
         <v>151</v>
       </c>
       <c r="C4" s="110" t="s">
-        <v>1235</v>
+        <v>1236</v>
       </c>
       <c r="D4" s="110" t="s">
-        <v>1236</v>
+        <v>1237</v>
       </c>
       <c r="F4" s="110" t="s">
         <v>1200</v>
       </c>
-      <c r="G4" s="140"/>
+      <c r="G4" s="141"/>
       <c r="H4" s="110" t="s">
         <v>317</v>
       </c>
@@ -26640,16 +26651,16 @@
       <c r="B5" s="110" t="s">
         <v>203</v>
       </c>
-      <c r="G5" s="140"/>
+      <c r="G5" s="141"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="6">
       <c r="A6" s="31" t="s">
-        <v>1237</v>
+        <v>1238</v>
       </c>
       <c r="B6" s="31" t="s">
-        <v>1238</v>
-      </c>
-      <c r="G6" s="140"/>
+        <v>1239</v>
+      </c>
+      <c r="G6" s="141"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="7">
       <c r="A7" s="110" t="s">
@@ -26658,99 +26669,99 @@
       <c r="B7" s="110" t="s">
         <v>198</v>
       </c>
-      <c r="G7" s="140"/>
+      <c r="G7" s="141"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="8">
       <c r="A8" s="31" t="s">
-        <v>1239</v>
+        <v>1240</v>
       </c>
       <c r="B8" s="31" t="s">
-        <v>1240</v>
-      </c>
-      <c r="G8" s="140"/>
+        <v>1241</v>
+      </c>
+      <c r="G8" s="141"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="9">
-      <c r="G9" s="140"/>
+      <c r="G9" s="141"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="10">
-      <c r="G10" s="140"/>
+      <c r="G10" s="141"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="11">
-      <c r="G11" s="140"/>
+      <c r="G11" s="141"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="12">
-      <c r="G12" s="140"/>
+      <c r="G12" s="141"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="13">
-      <c r="G13" s="140"/>
+      <c r="G13" s="141"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="14">
-      <c r="G14" s="140"/>
+      <c r="G14" s="141"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="15">
-      <c r="G15" s="140"/>
+      <c r="G15" s="141"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="16">
-      <c r="G16" s="140"/>
+      <c r="G16" s="141"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="17">
-      <c r="G17" s="140"/>
+      <c r="G17" s="141"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="18">
-      <c r="G18" s="140"/>
+      <c r="G18" s="141"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="19">
-      <c r="G19" s="140"/>
+      <c r="G19" s="141"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="20">
-      <c r="A20" s="141"/>
-      <c r="B20" s="141"/>
-      <c r="C20" s="141"/>
-      <c r="D20" s="141"/>
-      <c r="E20" s="142"/>
-      <c r="F20" s="141"/>
-      <c r="G20" s="142"/>
-      <c r="H20" s="141"/>
-      <c r="I20" s="141"/>
-      <c r="J20" s="141"/>
-      <c r="K20" s="141"/>
-      <c r="L20" s="141"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="69.8" outlineLevel="0" r="21" s="144">
+      <c r="A20" s="142"/>
+      <c r="B20" s="142"/>
+      <c r="C20" s="142"/>
+      <c r="D20" s="142"/>
+      <c r="E20" s="143"/>
+      <c r="F20" s="142"/>
+      <c r="G20" s="143"/>
+      <c r="H20" s="142"/>
+      <c r="I20" s="142"/>
+      <c r="J20" s="142"/>
+      <c r="K20" s="142"/>
+      <c r="L20" s="142"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="69.8" outlineLevel="0" r="21" s="145">
       <c r="A21" s="77" t="s">
-        <v>1241</v>
+        <v>1242</v>
       </c>
       <c r="B21" s="78" t="s">
         <v>1162</v>
       </c>
       <c r="C21" s="77" t="s">
-        <v>1242</v>
+        <v>1243</v>
       </c>
       <c r="D21" s="77" t="s">
-        <v>1243</v>
-      </c>
-      <c r="E21" s="143" t="s">
         <v>1244</v>
       </c>
+      <c r="E21" s="144" t="s">
+        <v>1245</v>
+      </c>
       <c r="F21" s="77" t="s">
-        <v>1245</v>
+        <v>1246</v>
       </c>
       <c r="G21" s="77" t="s">
-        <v>1246</v>
+        <v>1247</v>
       </c>
       <c r="H21" s="77" t="s">
-        <v>1247</v>
+        <v>1248</v>
       </c>
       <c r="I21" s="77" t="s">
-        <v>1248</v>
+        <v>1249</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="22">
-      <c r="A22" s="145" t="s">
-        <v>1249</v>
+      <c r="A22" s="146" t="s">
+        <v>1250</v>
       </c>
       <c r="B22" s="110" t="s">
-        <v>1250</v>
+        <v>1251</v>
       </c>
       <c r="C22" s="110" t="s">
         <v>1025</v>
@@ -26758,11 +26769,11 @@
       <c r="D22" s="110" t="s">
         <v>1032</v>
       </c>
-      <c r="E22" s="140" t="s">
-        <v>1251</v>
+      <c r="E22" s="141" t="s">
+        <v>1252</v>
       </c>
       <c r="F22" s="110" t="s">
-        <v>1252</v>
+        <v>1253</v>
       </c>
       <c r="G22" s="110" t="s">
         <v>781</v>
@@ -26776,19 +26787,19 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="24.5" outlineLevel="0" r="23">
       <c r="B23" s="110" t="s">
-        <v>1253</v>
+        <v>1254</v>
       </c>
       <c r="C23" s="110" t="s">
-        <v>1254</v>
+        <v>1255</v>
       </c>
       <c r="D23" s="110" t="s">
         <v>1155</v>
       </c>
-      <c r="E23" s="140" t="s">
-        <v>1255</v>
+      <c r="E23" s="141" t="s">
+        <v>1256</v>
       </c>
       <c r="F23" s="110" t="s">
-        <v>1256</v>
+        <v>1257</v>
       </c>
       <c r="G23" s="110" t="s">
         <v>787</v>
@@ -26797,21 +26808,21 @@
         <v>787</v>
       </c>
       <c r="I23" s="110" t="s">
-        <v>1257</v>
+        <v>1258</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="24.5" outlineLevel="0" r="24">
       <c r="B24" s="110" t="s">
-        <v>1258</v>
+        <v>1259</v>
       </c>
       <c r="C24" s="110" t="s">
-        <v>1259</v>
+        <v>1260</v>
       </c>
       <c r="D24" s="110" t="s">
         <v>1138</v>
       </c>
       <c r="F24" s="110" t="s">
-        <v>1260</v>
+        <v>1261</v>
       </c>
       <c r="G24" s="110" t="s">
         <v>784</v>
@@ -26820,911 +26831,911 @@
         <v>784</v>
       </c>
       <c r="I24" s="110" t="s">
-        <v>1261</v>
+        <v>1262</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="25">
       <c r="B25" s="110" t="s">
-        <v>1262</v>
+        <v>1263</v>
       </c>
       <c r="C25" s="110" t="s">
-        <v>1263</v>
+        <v>1264</v>
       </c>
       <c r="D25" s="110" t="s">
         <v>1156</v>
       </c>
       <c r="H25" s="110" t="s">
-        <v>1264</v>
+        <v>1265</v>
       </c>
       <c r="I25" s="110" t="s">
-        <v>1265</v>
+        <v>1266</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="26">
       <c r="B26" s="110" t="s">
-        <v>1266</v>
+        <v>1267</v>
       </c>
       <c r="C26" s="110" t="s">
-        <v>1267</v>
+        <v>1268</v>
       </c>
       <c r="H26" s="110" t="s">
-        <v>1268</v>
+        <v>1269</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="27">
       <c r="B27" s="110" t="s">
-        <v>1269</v>
+        <v>1270</v>
       </c>
       <c r="C27" s="110" t="s">
-        <v>1270</v>
+        <v>1271</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="28">
       <c r="B28" s="110" t="s">
-        <v>1271</v>
+        <v>1272</v>
       </c>
       <c r="C28" s="110" t="s">
-        <v>1272</v>
+        <v>1273</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="29">
       <c r="B29" s="110" t="s">
-        <v>1273</v>
+        <v>1274</v>
       </c>
       <c r="C29" s="110" t="s">
-        <v>1274</v>
+        <v>1275</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="30">
       <c r="B30" s="110" t="s">
-        <v>1275</v>
+        <v>1276</v>
       </c>
       <c r="C30" s="110" t="s">
-        <v>1276</v>
+        <v>1277</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="31">
       <c r="B31" s="110" t="s">
-        <v>1277</v>
+        <v>1278</v>
       </c>
       <c r="C31" s="110" t="s">
-        <v>1278</v>
+        <v>1279</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="32">
       <c r="B32" s="110" t="s">
-        <v>1279</v>
+        <v>1280</v>
       </c>
       <c r="C32" s="110" t="s">
-        <v>1280</v>
+        <v>1281</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="33">
       <c r="B33" s="110" t="s">
-        <v>1281</v>
+        <v>1282</v>
       </c>
       <c r="C33" s="110" t="s">
-        <v>1282</v>
+        <v>1283</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="34">
       <c r="B34" s="110" t="s">
-        <v>1283</v>
+        <v>1284</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="35">
       <c r="B35" s="110" t="s">
-        <v>1284</v>
+        <v>1285</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="36">
       <c r="B36" s="110" t="s">
-        <v>1285</v>
+        <v>1286</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="37">
       <c r="B37" s="110" t="s">
-        <v>1286</v>
+        <v>1287</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="38">
       <c r="B38" s="110" t="s">
-        <v>1287</v>
+        <v>1288</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="39">
       <c r="B39" s="110" t="s">
-        <v>1288</v>
+        <v>1289</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="40">
       <c r="B40" s="110" t="s">
-        <v>1289</v>
+        <v>1290</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="41">
       <c r="B41" s="110" t="s">
-        <v>1290</v>
+        <v>1291</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="42">
       <c r="B42" s="110" t="s">
-        <v>1291</v>
+        <v>1292</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="43">
       <c r="B43" s="110" t="s">
-        <v>1292</v>
+        <v>1293</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="44">
       <c r="B44" s="110" t="s">
-        <v>1293</v>
+        <v>1294</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="45">
       <c r="B45" s="110" t="s">
-        <v>1294</v>
+        <v>1295</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="46">
       <c r="B46" s="110" t="s">
-        <v>1295</v>
+        <v>1296</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="47">
       <c r="B47" s="110" t="s">
-        <v>1296</v>
+        <v>1297</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="48">
       <c r="B48" s="110" t="s">
-        <v>1297</v>
+        <v>1298</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="49">
       <c r="B49" s="110" t="s">
-        <v>1298</v>
+        <v>1299</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="50">
       <c r="B50" s="110" t="s">
-        <v>1299</v>
+        <v>1300</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="51">
       <c r="B51" s="110" t="s">
-        <v>1300</v>
+        <v>1301</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="52">
       <c r="B52" s="110" t="s">
-        <v>1301</v>
+        <v>1302</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="53">
       <c r="B53" s="110" t="s">
-        <v>1302</v>
+        <v>1303</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="54">
       <c r="B54" s="110" t="s">
-        <v>1303</v>
+        <v>1304</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="55">
       <c r="B55" s="110" t="s">
-        <v>1304</v>
+        <v>1305</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="56">
       <c r="B56" s="110" t="s">
-        <v>1305</v>
+        <v>1306</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="57">
       <c r="B57" s="110" t="s">
-        <v>1306</v>
+        <v>1307</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="58">
       <c r="B58" s="110" t="s">
-        <v>1307</v>
+        <v>1308</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="59">
       <c r="B59" s="110" t="s">
-        <v>1308</v>
+        <v>1309</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="60">
       <c r="B60" s="110" t="s">
-        <v>1309</v>
+        <v>1310</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="61">
       <c r="B61" s="110" t="s">
-        <v>1310</v>
+        <v>1311</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="62">
       <c r="B62" s="110" t="s">
-        <v>1311</v>
+        <v>1312</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="63">
       <c r="B63" s="110" t="s">
-        <v>1312</v>
+        <v>1313</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="64">
       <c r="B64" s="110" t="s">
-        <v>1313</v>
+        <v>1314</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="65">
       <c r="B65" s="110" t="s">
-        <v>1314</v>
+        <v>1315</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="66">
       <c r="B66" s="110" t="s">
-        <v>1315</v>
+        <v>1316</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="67">
       <c r="B67" s="110" t="s">
-        <v>1316</v>
+        <v>1317</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="68">
       <c r="B68" s="110" t="s">
-        <v>1317</v>
+        <v>1318</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="69">
       <c r="B69" s="110" t="s">
-        <v>1318</v>
+        <v>1319</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="70">
       <c r="B70" s="110" t="s">
-        <v>1319</v>
+        <v>1320</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="71">
       <c r="B71" s="110" t="s">
-        <v>1320</v>
+        <v>1321</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="72">
       <c r="B72" s="110" t="s">
-        <v>1321</v>
+        <v>1322</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="73">
       <c r="B73" s="110" t="s">
-        <v>1322</v>
+        <v>1323</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="74">
       <c r="B74" s="110" t="s">
-        <v>1323</v>
+        <v>1324</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="75">
       <c r="B75" s="110" t="s">
-        <v>1324</v>
+        <v>1325</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="76">
       <c r="B76" s="110" t="s">
-        <v>1325</v>
+        <v>1326</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="77">
       <c r="B77" s="110" t="s">
-        <v>1326</v>
+        <v>1327</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="78">
       <c r="B78" s="110" t="s">
-        <v>1327</v>
+        <v>1328</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="79">
       <c r="B79" s="110" t="s">
-        <v>1328</v>
+        <v>1329</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="80">
       <c r="B80" s="110" t="s">
-        <v>1329</v>
+        <v>1330</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="81">
       <c r="B81" s="110" t="s">
-        <v>1330</v>
+        <v>1331</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="82">
       <c r="B82" s="110" t="s">
-        <v>1331</v>
+        <v>1332</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="83">
       <c r="B83" s="110" t="s">
-        <v>1332</v>
+        <v>1333</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="84">
       <c r="B84" s="110" t="s">
-        <v>1333</v>
+        <v>1334</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="85">
       <c r="B85" s="110" t="s">
-        <v>1334</v>
+        <v>1335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="86">
       <c r="B86" s="110" t="s">
-        <v>1335</v>
+        <v>1336</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="87">
       <c r="B87" s="110" t="s">
-        <v>1336</v>
+        <v>1337</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="88">
       <c r="B88" s="110" t="s">
-        <v>1337</v>
+        <v>1338</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="89">
       <c r="B89" s="110" t="s">
-        <v>1338</v>
+        <v>1339</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="90">
       <c r="B90" s="110" t="s">
-        <v>1339</v>
+        <v>1340</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="91">
       <c r="B91" s="110" t="s">
-        <v>1340</v>
+        <v>1341</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="92">
       <c r="B92" s="110" t="s">
-        <v>1341</v>
+        <v>1342</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="93">
       <c r="B93" s="110" t="s">
-        <v>1342</v>
+        <v>1343</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="94">
       <c r="B94" s="110" t="s">
-        <v>1343</v>
+        <v>1344</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="95">
       <c r="B95" s="110" t="s">
-        <v>1344</v>
+        <v>1345</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="96">
       <c r="B96" s="110" t="s">
-        <v>1345</v>
+        <v>1346</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="97">
       <c r="B97" s="110" t="s">
-        <v>1346</v>
+        <v>1347</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="98">
       <c r="B98" s="110" t="s">
-        <v>1347</v>
+        <v>1348</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="99">
       <c r="B99" s="110" t="s">
-        <v>1348</v>
+        <v>1349</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="100">
       <c r="B100" s="110" t="s">
-        <v>1349</v>
+        <v>1350</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="101">
       <c r="B101" s="110" t="s">
-        <v>1350</v>
+        <v>1351</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="102">
       <c r="B102" s="110" t="s">
-        <v>1351</v>
+        <v>1352</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="103">
       <c r="B103" s="110" t="s">
-        <v>1352</v>
+        <v>1353</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="104">
       <c r="B104" s="110" t="s">
-        <v>1353</v>
+        <v>1354</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="105">
       <c r="B105" s="110" t="s">
-        <v>1354</v>
+        <v>1355</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="106">
       <c r="B106" s="110" t="s">
-        <v>1355</v>
+        <v>1356</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="107">
       <c r="B107" s="110" t="s">
-        <v>1356</v>
+        <v>1357</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="108">
       <c r="B108" s="110" t="s">
-        <v>1357</v>
+        <v>1358</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="109">
       <c r="B109" s="110" t="s">
-        <v>1358</v>
+        <v>1359</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="110">
       <c r="B110" s="110" t="s">
-        <v>1359</v>
+        <v>1360</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="111">
       <c r="B111" s="110" t="s">
-        <v>1360</v>
+        <v>1361</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="112">
       <c r="B112" s="110" t="s">
-        <v>1361</v>
+        <v>1362</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="113">
       <c r="B113" s="110" t="s">
-        <v>1362</v>
+        <v>1363</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="114">
       <c r="B114" s="110" t="s">
-        <v>1363</v>
+        <v>1364</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="115">
       <c r="B115" s="110" t="s">
-        <v>1364</v>
+        <v>1365</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="116">
       <c r="B116" s="110" t="s">
-        <v>1365</v>
+        <v>1366</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="117">
       <c r="B117" s="110" t="s">
-        <v>1366</v>
+        <v>1367</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="118">
       <c r="B118" s="110" t="s">
-        <v>1367</v>
+        <v>1368</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="119">
       <c r="B119" s="110" t="s">
-        <v>1368</v>
+        <v>1369</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="120">
       <c r="B120" s="110" t="s">
-        <v>1369</v>
+        <v>1370</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="121">
       <c r="B121" s="110" t="s">
-        <v>1370</v>
+        <v>1371</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="122">
       <c r="B122" s="110" t="s">
-        <v>1371</v>
+        <v>1372</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="123">
       <c r="B123" s="110" t="s">
-        <v>1372</v>
+        <v>1373</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="124">
       <c r="B124" s="110" t="s">
-        <v>1373</v>
+        <v>1374</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="125">
       <c r="B125" s="110" t="s">
-        <v>1374</v>
+        <v>1375</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="126">
       <c r="B126" s="110" t="s">
-        <v>1375</v>
+        <v>1376</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="127">
       <c r="B127" s="110" t="s">
-        <v>1376</v>
+        <v>1377</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="128">
       <c r="B128" s="110" t="s">
-        <v>1377</v>
+        <v>1378</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="129">
       <c r="B129" s="110" t="s">
-        <v>1378</v>
+        <v>1379</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="130">
       <c r="B130" s="110" t="s">
-        <v>1379</v>
+        <v>1380</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="131">
       <c r="B131" s="110" t="s">
-        <v>1380</v>
+        <v>1381</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="132">
       <c r="B132" s="110" t="s">
-        <v>1381</v>
+        <v>1382</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="133">
       <c r="B133" s="110" t="s">
-        <v>1382</v>
+        <v>1383</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="134">
       <c r="B134" s="110" t="s">
-        <v>1383</v>
+        <v>1384</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="135">
       <c r="B135" s="110" t="s">
-        <v>1384</v>
+        <v>1385</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="136">
       <c r="B136" s="110" t="s">
-        <v>1385</v>
+        <v>1386</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="137">
       <c r="B137" s="110" t="s">
-        <v>1386</v>
+        <v>1387</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="138">
       <c r="B138" s="110" t="s">
-        <v>1387</v>
+        <v>1388</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="139">
       <c r="B139" s="110" t="s">
-        <v>1388</v>
+        <v>1389</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="140">
       <c r="B140" s="110" t="s">
-        <v>1389</v>
+        <v>1390</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="141">
       <c r="B141" s="110" t="s">
-        <v>1390</v>
+        <v>1391</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="142">
       <c r="B142" s="110" t="s">
-        <v>1391</v>
+        <v>1392</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="143">
       <c r="B143" s="110" t="s">
-        <v>1392</v>
+        <v>1393</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="144">
       <c r="B144" s="110" t="s">
-        <v>1393</v>
+        <v>1394</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="145">
       <c r="B145" s="110" t="s">
-        <v>1394</v>
+        <v>1395</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="146">
       <c r="B146" s="110" t="s">
-        <v>1395</v>
+        <v>1396</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="147">
       <c r="B147" s="110" t="s">
-        <v>1396</v>
+        <v>1397</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="148">
       <c r="B148" s="110" t="s">
-        <v>1397</v>
+        <v>1398</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="149">
       <c r="B149" s="110" t="s">
-        <v>1398</v>
+        <v>1399</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="150">
       <c r="B150" s="110" t="s">
-        <v>1399</v>
+        <v>1400</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="151">
       <c r="B151" s="110" t="s">
-        <v>1400</v>
+        <v>1401</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="152">
       <c r="B152" s="110" t="s">
-        <v>1401</v>
+        <v>1402</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="153">
       <c r="B153" s="110" t="s">
-        <v>1402</v>
+        <v>1403</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="154">
       <c r="B154" s="110" t="s">
-        <v>1403</v>
+        <v>1404</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="155">
       <c r="B155" s="110" t="s">
-        <v>1404</v>
+        <v>1405</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="156">
       <c r="B156" s="110" t="s">
-        <v>1405</v>
+        <v>1406</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="157">
       <c r="B157" s="110" t="s">
-        <v>1406</v>
+        <v>1407</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="158">
       <c r="B158" s="110" t="s">
-        <v>1407</v>
+        <v>1408</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="159">
       <c r="B159" s="110" t="s">
-        <v>1408</v>
+        <v>1409</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="160">
       <c r="B160" s="110" t="s">
-        <v>1409</v>
+        <v>1410</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="161">
       <c r="B161" s="110" t="s">
-        <v>1410</v>
+        <v>1411</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="162">
       <c r="B162" s="110" t="s">
-        <v>1411</v>
+        <v>1412</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="163">
       <c r="B163" s="110" t="s">
-        <v>1412</v>
+        <v>1413</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="164">
       <c r="B164" s="110" t="s">
-        <v>1413</v>
+        <v>1414</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="165">
       <c r="B165" s="110" t="s">
-        <v>1414</v>
+        <v>1415</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="166">
       <c r="B166" s="110" t="s">
-        <v>1415</v>
+        <v>1416</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="167">
       <c r="B167" s="110" t="s">
-        <v>1416</v>
+        <v>1417</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="168">
       <c r="B168" s="110" t="s">
-        <v>1417</v>
+        <v>1418</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="169">
       <c r="B169" s="110" t="s">
-        <v>1418</v>
+        <v>1419</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="170">
       <c r="B170" s="110" t="s">
-        <v>1419</v>
+        <v>1420</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="171">
       <c r="B171" s="110" t="s">
-        <v>1420</v>
+        <v>1421</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="172">
       <c r="B172" s="110" t="s">
-        <v>1421</v>
+        <v>1422</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="173">
       <c r="B173" s="110" t="s">
-        <v>1422</v>
+        <v>1423</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="174">
       <c r="B174" s="110" t="s">
-        <v>1423</v>
+        <v>1424</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="175">
       <c r="B175" s="110" t="s">
-        <v>1424</v>
+        <v>1425</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="176">
       <c r="B176" s="110" t="s">
-        <v>1425</v>
+        <v>1426</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="177">
       <c r="B177" s="110" t="s">
-        <v>1426</v>
+        <v>1427</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="178">
       <c r="B178" s="110" t="s">
-        <v>1427</v>
+        <v>1428</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="179">
       <c r="B179" s="110" t="s">
-        <v>1428</v>
+        <v>1429</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="180">
       <c r="B180" s="110" t="s">
-        <v>1429</v>
+        <v>1430</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="181">
       <c r="B181" s="110" t="s">
-        <v>1430</v>
+        <v>1431</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="182">
       <c r="B182" s="110" t="s">
-        <v>1431</v>
+        <v>1432</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="183">
       <c r="B183" s="110" t="s">
-        <v>1432</v>
+        <v>1433</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="184">
       <c r="B184" s="110" t="s">
-        <v>1433</v>
+        <v>1434</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="185">
       <c r="B185" s="110" t="s">
-        <v>1434</v>
+        <v>1435</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="186">
       <c r="B186" s="110" t="s">
-        <v>1435</v>
+        <v>1436</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="187">
       <c r="B187" s="110" t="s">
-        <v>1436</v>
+        <v>1437</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="188">
       <c r="B188" s="110" t="s">
-        <v>1437</v>
+        <v>1438</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="189">
       <c r="B189" s="110" t="s">
-        <v>1438</v>
+        <v>1439</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="190">
       <c r="B190" s="110" t="s">
-        <v>1439</v>
+        <v>1440</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="191">
       <c r="B191" s="110" t="s">
-        <v>1440</v>
+        <v>1441</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="192">
       <c r="B192" s="110" t="s">
-        <v>1441</v>
+        <v>1442</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="193">
       <c r="B193" s="110" t="s">
-        <v>1442</v>
+        <v>1443</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="194">
       <c r="B194" s="110" t="s">
-        <v>1443</v>
+        <v>1444</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="195">
       <c r="B195" s="110" t="s">
-        <v>1444</v>
+        <v>1445</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="196">
       <c r="B196" s="110" t="s">
-        <v>1445</v>
+        <v>1446</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="197">
       <c r="B197" s="110" t="s">
-        <v>1446</v>
+        <v>1447</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="198">
@@ -27734,12 +27745,12 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="199">
       <c r="B199" s="110" t="s">
-        <v>1447</v>
+        <v>1448</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="200">
       <c r="B200" s="110" t="s">
-        <v>1448</v>
+        <v>1449</v>
       </c>
     </row>
   </sheetData>
@@ -27765,13 +27776,13 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.2823529411765"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.1058823529412"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="39" width="8.21960784313725"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="39" width="11.9450980392157"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="39" width="6.0078431372549"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="39" width="8.10196078431373"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57647058823529"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.3333333333333"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.1960784313725"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="39" width="8.25490196078431"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="39" width="11.9882352941176"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="39" width="6.03137254901961"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="39" width="8.13333333333333"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.61176470588235"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="12.2" outlineLevel="0" r="1" s="5">
@@ -27926,13 +27937,13 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.7921568627451"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.13333333333333"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.4039215686275"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="6.83529411764706"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.6117647058824"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.9294117647059"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="40" width="9.38039215686275"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.82745098039216"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.16862745098039"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.4549019607843"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="6.86274509803922"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.6627450980392"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.0039215686275"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="40" width="9.42352941176471"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="13.4" outlineLevel="0" r="1">
@@ -28101,28 +28112,29 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.2"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.68235294117647"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="8.23921568627451"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.7843137254902"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="12.5294117647059"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.2235294117647"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.7960784313726"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.18039215686274"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.0196078431373"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.7764705882353"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="11.7960784313726"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="10.556862745098"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="8.7764705882353"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="7.54509803921569"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="10.556862745098"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="10.6980392156863"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="8.71372549019608"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="8.91372549019608"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="7.66666666666667"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="10.6980392156863"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="11.3647058823529"/>
-    <col collapsed="false" hidden="false" max="1025" min="25" style="0" width="7.66666666666667"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.2627450980392"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.72156862745098"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="8.27450980392157"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.8627450980392"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="12.5843137254902"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.3098039215686"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.8470588235294"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.22352941176471"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.0588235294118"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.81176470588235"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="11.8470588235294"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="10.6039215686275"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="8.54117647058824"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="8.81176470588235"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="7.58039215686275"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="10.6039215686275"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="10.7411764705882"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="8.74901960784314"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="8.94901960784314"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="7.70196078431373"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="10.7411764705882"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="11.4078431372549"/>
+    <col collapsed="false" hidden="false" max="1025" min="25" style="0" width="7.70196078431373"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="12.2" outlineLevel="0" r="1" s="41">
@@ -28556,20 +28568,20 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.321568627451"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.9921568627451"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.84313725490196"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.72549019607843"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="10.3960784313725"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.6509803921569"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.6352941176471"/>
-    <col collapsed="false" hidden="false" max="12" min="9" style="0" width="8.64705882352941"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="16.7882352941176"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="12.5294117647059"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="22.7450980392157"/>
-    <col collapsed="false" hidden="false" max="26" min="16" style="0" width="7.70196078431373"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="9.12156862745098"/>
-    <col collapsed="false" hidden="false" max="1025" min="28" style="0" width="8.54117647058824"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3647058823529"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.01960784313726"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.87843137254902"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.76862745098039"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="10.4392156862745"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.7019607843137"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.678431372549"/>
+    <col collapsed="false" hidden="false" max="12" min="9" style="0" width="8.68235294117647"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="16.8588235294118"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="12.5843137254902"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="22.8392156862745"/>
+    <col collapsed="false" hidden="false" max="26" min="16" style="0" width="7.72941176470588"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="9.15686274509804"/>
+    <col collapsed="false" hidden="false" max="1025" min="28" style="0" width="8.57647058823529"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="12.2" outlineLevel="0" r="1" s="15">

</xml_diff>

<commit_message>
Reorganise tests and js
Some things fixed, also.
</commit_message>
<xml_diff>
--- a/bika/lims/setupdata/test/test.xlsx
+++ b/bika/lims/setupdata/test/test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="46" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="929" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="33" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="593" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" state="visible" r:id="rId2"/>
@@ -98,15 +98,15 @@
             <anchor moveWithCells="false" sizeWithCells="false">
               <xdr:from>
                 <xdr:col>6</xdr:col>
-                <xdr:colOff>23</xdr:colOff>
+                <xdr:colOff>3</xdr:colOff>
                 <xdr:row>-1</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </xdr:from>
               <xdr:to>
                 <xdr:col>7</xdr:col>
-                <xdr:colOff>62</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>28</xdr:rowOff>
+                <xdr:colOff>3</xdr:colOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>9</xdr:rowOff>
               </xdr:to>
             </anchor>
           </commentPr>
@@ -144,15 +144,15 @@
             <anchor moveWithCells="false" sizeWithCells="false">
               <xdr:from>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>23</xdr:colOff>
+                <xdr:colOff>21</xdr:colOff>
                 <xdr:row>-1</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </xdr:from>
               <xdr:to>
                 <xdr:col>2</xdr:col>
-                <xdr:colOff>-69</xdr:colOff>
-                <xdr:row>9</xdr:row>
-                <xdr:rowOff>5</xdr:rowOff>
+                <xdr:colOff>-72</xdr:colOff>
+                <xdr:row>17</xdr:row>
+                <xdr:rowOff>7</xdr:rowOff>
               </xdr:to>
             </anchor>
           </commentPr>
@@ -190,15 +190,15 @@
             <anchor moveWithCells="false" sizeWithCells="false">
               <xdr:from>
                 <xdr:col>2</xdr:col>
-                <xdr:colOff>23</xdr:colOff>
+                <xdr:colOff>21</xdr:colOff>
                 <xdr:row>-1</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </xdr:from>
               <xdr:to>
                 <xdr:col>3</xdr:col>
-                <xdr:colOff>52</xdr:colOff>
-                <xdr:row>17</xdr:row>
-                <xdr:rowOff>16</xdr:rowOff>
+                <xdr:colOff>50</xdr:colOff>
+                <xdr:row>34</xdr:row>
+                <xdr:rowOff>11</xdr:rowOff>
               </xdr:to>
             </anchor>
           </commentPr>
@@ -235,15 +235,15 @@
             <anchor moveWithCells="false" sizeWithCells="false">
               <xdr:from>
                 <xdr:col>5</xdr:col>
-                <xdr:colOff>23</xdr:colOff>
+                <xdr:colOff>19</xdr:colOff>
                 <xdr:row>-1</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </xdr:from>
               <xdr:to>
                 <xdr:col>6</xdr:col>
-                <xdr:colOff>35</xdr:colOff>
-                <xdr:row>6</xdr:row>
-                <xdr:rowOff>9</xdr:rowOff>
+                <xdr:colOff>31</xdr:colOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>14</xdr:rowOff>
               </xdr:to>
             </anchor>
           </commentPr>
@@ -270,15 +270,15 @@
             <anchor moveWithCells="false" sizeWithCells="false">
               <xdr:from>
                 <xdr:col>14</xdr:col>
-                <xdr:colOff>23</xdr:colOff>
+                <xdr:colOff>12</xdr:colOff>
                 <xdr:row>-1</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </xdr:from>
               <xdr:to>
                 <xdr:col>15</xdr:col>
-                <xdr:colOff>-79</xdr:colOff>
-                <xdr:row>11</xdr:row>
-                <xdr:rowOff>14</xdr:rowOff>
+                <xdr:colOff>-92</xdr:colOff>
+                <xdr:row>21</xdr:row>
+                <xdr:rowOff>6</xdr:rowOff>
               </xdr:to>
             </anchor>
           </commentPr>
@@ -1097,10 +1097,14 @@
     <t>Client ID</t>
   </si>
   <si>
-    <t>Member discount applies?</t>
-  </si>
-  <si>
-    <t>Bulk discount applies?</t>
+    <t>Member
+discount
+applies?</t>
+  </si>
+  <si>
+    <t>Bulk
+discount
+applies?</t>
   </si>
   <si>
     <t>Account number</t>
@@ -5131,10 +5135,10 @@
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="18" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="18" numFmtId="167" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="18" numFmtId="164" xfId="0">
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
@@ -5408,7 +5412,7 @@
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00E6E6FF"/>
       <rgbColor rgb="00FF0000"/>
       <rgbColor rgb="0000FF00"/>
       <rgbColor rgb="000000FF"/>
@@ -5426,7 +5430,7 @@
       <rgbColor rgb="009999FF"/>
       <rgbColor rgb="00993366"/>
       <rgbColor rgb="00E6E6E6"/>
-      <rgbColor rgb="00E6E6FF"/>
+      <rgbColor rgb="00CCFFFF"/>
       <rgbColor rgb="00660066"/>
       <rgbColor rgb="00FF8080"/>
       <rgbColor rgb="000066CC"/>
@@ -5480,9 +5484,9 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="96.8156862745098"/>
-    <col collapsed="false" hidden="false" max="1023" min="2" style="0" width="8.82745098039216"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="8.86274509803922"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="97.6156862745098"/>
+    <col collapsed="false" hidden="false" max="1023" min="2" style="0" width="8.89803921568628"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="8.93333333333333"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="32.05" outlineLevel="0" r="1" s="3">
@@ -5550,9 +5554,9 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.5725490196078"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.4274509803922"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57647058823529"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.7294117647059"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.5960784313726"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.64705882352941"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="19.8" outlineLevel="0" r="1" s="5">
@@ -5600,9 +5604,9 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.5725490196078"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.4274509803922"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57647058823529"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.7294117647059"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.5960784313726"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.64705882352941"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="12.2" outlineLevel="0" r="1" s="5">
@@ -5701,10 +5705,10 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.2823529411765"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.8941176470588"/>
-    <col collapsed="false" hidden="false" max="5" min="3" style="0" width="14.1843137254902"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57647058823529"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.4392156862745"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.0156862745098"/>
+    <col collapsed="false" hidden="false" max="5" min="3" style="0" width="14.3058823529412"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.64705882352941"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="19.8" outlineLevel="0" r="1" s="5">
@@ -6037,18 +6041,18 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.30196078431373"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.65490196078431"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.86274509803922"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.3764705882353"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.61176470588235"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.6078431372549"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.3372549019608"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.51764705882353"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="7.07058823529412"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="7.6"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="24.3372549019608"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="9.38039215686275"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.38039215686275"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.71372549019608"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.92156862745098"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.5647058823529"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.68235294117647"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.68235294117647"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.4470588235294"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.6"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="7.12941176470588"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="7.66666666666667"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="24.5372549019608"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="9.46666666666667"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="12.2" outlineLevel="0" r="1" s="5">
@@ -6224,11 +6228,11 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.3333333333333"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="39" width="10.4274509803922"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="39" width="11.9882352941176"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="39" width="12.2117647058824"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.61176470588235"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.4352941176471"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="39" width="10.5137254901961"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="39" width="12.0901960784314"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="39" width="12.3137254901961"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.68235294117647"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="12.2" outlineLevel="0" r="1" s="5">
@@ -6402,13 +6406,13 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.3490196078431"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.0039215686274"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.74901960784314"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.4509803921569"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.4627450980392"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.2666666666667"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57647058823529"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.5176470588235"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.1921568627451"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.80392156862745"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.5843137254902"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.5843137254902"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.3882352941176"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.64705882352941"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="12.2" outlineLevel="0" r="1" s="5">
@@ -6627,9 +6631,9 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.2901960784314"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.6627450980392"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57647058823529"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.3921568627451"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.8274509803922"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.64705882352941"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="12.2" outlineLevel="0" r="1" s="5">
@@ -6736,16 +6740,16 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3882352941176"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.0823529411765"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.74901960784314"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="4.67450980392157"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.72156862745098"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.83921568627451"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.54509803921569"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.2901960784314"/>
-    <col collapsed="false" hidden="false" max="1023" min="9" style="0" width="6.83921568627451"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="5.83529411764706"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.5019607843137"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.2941176470588"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.80392156862745"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="4.71764705882353"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.7921568627451"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.89803921568628"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.6078431372549"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.4078431372549"/>
+    <col collapsed="false" hidden="false" max="1023" min="9" style="0" width="6.89803921568628"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="5.87843137254902"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="13.2" outlineLevel="0" r="1" s="15">
@@ -7172,14 +7176,14 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="12.9803921568627"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.0901960784314"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.7098039215686"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="17.7176470588235"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.66666666666667"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.2274509803922"/>
-    <col collapsed="false" hidden="false" max="1018" min="9" style="0" width="8.57647058823529"/>
-    <col collapsed="false" hidden="false" max="1025" min="1019" style="0" width="5.71372549019608"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="13.0941176470588"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.2901960784314"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.8509803921569"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="17.8705882352941"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.72941176470588"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.3098039215686"/>
+    <col collapsed="false" hidden="false" max="1018" min="9" style="0" width="8.64705882352941"/>
+    <col collapsed="false" hidden="false" max="1025" min="1019" style="0" width="5.75686274509804"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="12.2" outlineLevel="0" r="1" s="5">
@@ -7448,11 +7452,11 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.9686274509804"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.7490196078431"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.0823529411765"/>
-    <col collapsed="false" hidden="false" max="1018" min="4" style="0" width="8.57647058823529"/>
-    <col collapsed="false" hidden="false" max="1025" min="1019" style="0" width="5.14117647058824"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.1254901960784"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.9372549019608"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.2117647058824"/>
+    <col collapsed="false" hidden="false" max="1018" min="4" style="0" width="8.64705882352941"/>
+    <col collapsed="false" hidden="false" max="1025" min="1019" style="0" width="5.1843137254902"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="12.2" outlineLevel="0" r="1" s="15">
@@ -7521,10 +7525,10 @@
   </sheetViews>
   <cols>
     <col collapsed="false" hidden="true" max="1" min="1" style="0" width="0"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.8392156862745"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.38823529411765"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="4.77647058823529"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="6.81176470588235"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.9686274509804"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.44705882352941"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="4.81960784313725"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="6.87058823529412"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="12.2" outlineLevel="0" r="1" s="5">
@@ -7718,10 +7722,10 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.6313725490196"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="56.6196078431373"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.0901960784314"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57647058823529"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.7607843137255"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="57.0941176470588"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.2901960784314"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.64705882352941"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="12.2" outlineLevel="0" r="1" s="15">
@@ -7910,9 +7914,9 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.0470588235294"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.9725490196078"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57647058823529"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.2627450980392"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.1176470588235"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.64705882352941"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="12.2" outlineLevel="0" r="1" s="5">
@@ -8050,11 +8054,9 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.8588235294118"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="9.72549019607843"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.5176470588235"/>
-    <col collapsed="false" hidden="false" max="21" min="6" style="0" width="9.72549019607843"/>
-    <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="16.8588235294118"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="9.8078431372549"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.6470588235294"/>
+    <col collapsed="false" hidden="false" max="21" min="6" style="0" width="9.8078431372549"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="12.2" outlineLevel="0" r="1" s="5">
@@ -8280,9 +8282,9 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.0980392156863"/>
-    <col collapsed="false" hidden="false" max="21" min="2" style="0" width="8.13333333333333"/>
-    <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="8.57647058823529"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.2823529411765"/>
+    <col collapsed="false" hidden="false" max="21" min="2" style="0" width="8.20392156862745"/>
+    <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="8.64705882352941"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="12.2" outlineLevel="0" r="1" s="5">
@@ -8558,10 +8560,10 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.878431372549"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.7764705882353"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="7.72941176470588"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="7.70196078431373"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.0666666666667"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.0196078431373"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="7.79607843137255"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="7.76078431372549"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="13.4" outlineLevel="0" r="1">
@@ -8678,18 +8680,18 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.3490196078431"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.9882352941176"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.4745098039216"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.3333333333333"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.8196078431373"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.2470588235294"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.2313725490196"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.5294117647059"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.556862745098"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="7.72941176470588"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="11.4588235294118"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.57647058823529"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.5176470588235"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.1882352941176"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.6274509803922"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.4745098039216"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.921568627451"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.4352941176471"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.321568627451"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.6235294117647"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.6627450980392"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="7.79607843137255"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="11.5529411764706"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.64705882352941"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="13.4" outlineLevel="0" r="1" s="86">
@@ -9798,15 +9800,15 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.5058823529412"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.721568627451"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.8274509803922"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.6"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.6156862745098"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.5254901960784"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.9725490196078"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="29.1490196078431"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="7.72941176470588"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.6352941176471"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.8588235294118"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.9137254901961"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.68235294117647"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.7333333333333"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.6705882352941"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.1176470588235"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="29.3921568627451"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="7.79607843137255"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="15.1" outlineLevel="0" r="1" s="86">
@@ -9940,15 +9942,15 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.5058823529412"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.7764705882353"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.8274509803922"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.6"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.6156862745098"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.5254901960784"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.9725490196078"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="29.1490196078431"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="7.72941176470588"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.6352941176471"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.8666666666667"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.9137254901961"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.68235294117647"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.7333333333333"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.6705882352941"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.1176470588235"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="29.3921568627451"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="7.79607843137255"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="15.1" outlineLevel="0" r="1" s="86">
@@ -10079,14 +10081,14 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1803921568627"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.0980392156863"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.72941176470588"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.4117647058824"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.4862745098039"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.7098039215686"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.0823529411765"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="7.72941176470588"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.3098039215686"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.2666666666667"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.79607843137255"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.5137254901961"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.5803921568627"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.8392156862745"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.2941176470588"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="7.79607843137255"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="14.9" outlineLevel="0" r="1">
@@ -11065,17 +11067,17 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.278431372549"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.3372549019608"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.4156862745098"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.2705882352941"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.3803921568627"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="7.72941176470588"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.4"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.4627450980392"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.5529411764706"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="5.34901960784314"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="7.72941176470588"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.4"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.5372549019608"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.5725490196078"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.3529411764706"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.4823529411765"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="7.79607843137255"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.521568627451"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.5843137254902"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.6823529411765"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="5.3921568627451"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="7.79607843137255"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="14.9" outlineLevel="0" r="1" s="86">
@@ -11292,9 +11294,9 @@
   </sheetViews>
   <cols>
     <col collapsed="false" hidden="true" max="1" min="1" style="0" width="0"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.2588235294118"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.6745098039216"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="6.83921568627451"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.5372549019608"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.8196078431373"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="6.89803921568628"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="12.2" outlineLevel="0" r="1" s="5">
@@ -11693,17 +11695,17 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.6392156862745"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.9411764705882"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.9725490196078"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.2705882352941"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.3803921568627"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.0588235294118"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.4627450980392"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.6039215686275"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="28.0156862745098"/>
-    <col collapsed="false" hidden="false" max="1023" min="10" style="0" width="7.72941176470588"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="7.70196078431373"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.7843137254902"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.121568627451"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.1411764705882"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.3529411764706"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.4823529411765"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.1803921568627"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.5843137254902"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.7019607843137"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="28.2470588235294"/>
+    <col collapsed="false" hidden="false" max="1023" min="10" style="0" width="7.79607843137255"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="7.76078431372549"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="14.9" outlineLevel="0" r="1" s="86">
@@ -11795,10 +11797,10 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.2274509803922"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.8705882352941"/>
-    <col collapsed="false" hidden="false" max="5" min="3" style="0" width="21.2313725490196"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57647058823529"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.4705882352941"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.1450980392157"/>
+    <col collapsed="false" hidden="false" max="5" min="3" style="0" width="21.4039215686274"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.64705882352941"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="12.2" outlineLevel="0" r="1" s="5">
@@ -11897,10 +11899,10 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.4235294117647"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="47.156862745098"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="47.7490196078431"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="6.40392156862745"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.5686274509804"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="47.5490196078431"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="48.1450980392157"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="6.46274509803922"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="14.15" outlineLevel="0" r="1" s="105">
@@ -12034,10 +12036,10 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="25.1411764705882"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="7.23529411764706"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="3.34901960784314"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57647058823529"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="25.3490196078431"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="7.29411764705882"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="3.37647058823529"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.64705882352941"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="12.2" outlineLevel="0" r="1" s="5">
@@ -12636,33 +12638,33 @@
   </sheetPr>
   <dimension ref="1:28"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
-      <selection activeCell="B31" activeCellId="0" pane="topLeft" sqref="B31"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="C1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
+      <selection activeCell="C35" activeCellId="0" pane="topLeft" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.0392156862745"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="29.4078431372549"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.36078431372549"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="5.29019607843137"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.7176470588235"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.3529411764706"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.1843137254902"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="7.4156862745098"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="6.12941176470588"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="7.70196078431373"/>
-    <col collapsed="false" hidden="false" max="14" min="12" style="0" width="3.67843137254902"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="3.95686274509804"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="6.46274509803922"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="3.34901960784314"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="13.5882352941176"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="9.74509803921569"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="13.4901960784314"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="11.5019607843137"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="9.25882352941177"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="8.39607843137255"/>
-    <col collapsed="false" hidden="false" max="25" min="24" style="0" width="10.7725490196078"/>
-    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="7.70196078431373"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.2117647058824"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="29.6509803921569"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.43137254901961"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="5.33333333333333"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.8705882352941"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.4392156862745"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.2705882352941"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="7.47843137254902"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="6.18039215686275"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="7.76078431372549"/>
+    <col collapsed="false" hidden="false" max="14" min="12" style="0" width="3.70588235294118"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="3.98823529411765"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="6.51764705882353"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="3.37647058823529"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="13.7019607843137"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="9.83137254901961"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="13.6039215686275"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="11.6039215686275"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="9.34509803921569"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="8.47058823529412"/>
+    <col collapsed="false" hidden="false" max="25" min="24" style="0" width="10.8627450980392"/>
+    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="7.76078431372549"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="24.1" outlineLevel="0" r="1" s="15">
@@ -13022,7 +13024,7 @@
         <v>7.5</v>
       </c>
       <c r="Q6" s="33" t="n">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="R6" s="118"/>
       <c r="S6" s="121"/>
@@ -14563,12 +14565,11 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.3333333333333"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.89803921568628"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.68235294117647"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.4"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="3.34901960784314"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57647058823529"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.5607843137255"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.75686274509804"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.521568627451"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="3.37647058823529"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.64705882352941"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="12.2" outlineLevel="0" r="1" s="5">
@@ -14634,12 +14635,12 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.6117647058824"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.7019607843137"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.57647058823529"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.4"/>
-    <col collapsed="false" hidden="false" max="973" min="5" style="0" width="8.57647058823529"/>
-    <col collapsed="false" hidden="false" max="1025" min="974" style="0" width="5.14117647058824"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.6980392156863"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.7960784313726"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.64705882352941"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.521568627451"/>
+    <col collapsed="false" hidden="false" max="973" min="5" style="0" width="8.64705882352941"/>
+    <col collapsed="false" hidden="false" max="1025" min="974" style="0" width="5.1843137254902"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="24.5" outlineLevel="0" r="1" s="15">
@@ -14842,11 +14843,11 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.3294117647059"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="9.50196078431373"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.8078431372549"/>
-    <col collapsed="false" hidden="false" max="997" min="5" style="0" width="8.57647058823529"/>
-    <col collapsed="false" hidden="false" max="1025" min="998" style="0" width="5.14117647058824"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.6274509803922"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="9.58823529411765"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.89019607843137"/>
+    <col collapsed="false" hidden="false" max="997" min="5" style="0" width="8.64705882352941"/>
+    <col collapsed="false" hidden="false" max="1025" min="998" style="0" width="5.1843137254902"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="24.5" outlineLevel="0" r="1" s="15">
@@ -16318,13 +16319,13 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0941176470588"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.7450980392157"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.3490196078431"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.0392156862745"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.7058823529412"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="5.51372549019608"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57647058823529"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.2392156862745"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.8705882352941"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.5725490196078"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.1411764705882"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.7921568627451"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="5.56470588235294"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.64705882352941"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="12.2" outlineLevel="0" r="1" s="41">
@@ -16470,10 +16471,10 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.4941176470588"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.8862745098039"/>
-    <col collapsed="false" hidden="false" max="6" min="3" style="0" width="29.5137254901961"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57647058823529"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.6823529411765"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.1176470588235"/>
+    <col collapsed="false" hidden="false" max="6" min="3" style="0" width="29.7607843137255"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.64705882352941"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.2" outlineLevel="0" r="1" s="41">
@@ -16690,20 +16691,20 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.53333333333333"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.1921568627451"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.2274509803922"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.3607843137255"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.82745098039216"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.85098039215686"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.8705882352941"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.9137254901961"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.5686274509804"/>
-    <col collapsed="false" hidden="false" max="12" min="10" style="0" width="8.82745098039216"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="12.0901960784314"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="10.4823529411765"/>
-    <col collapsed="false" hidden="false" max="16" min="15" style="0" width="30.3058823529412"/>
-    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="8.82745098039216"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.57647058823529"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.25098039215686"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.3098039215686"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.5058823529412"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.89803921568628"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.93333333333333"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.9803921568627"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.6549019607843"/>
+    <col collapsed="false" hidden="false" max="12" min="10" style="0" width="8.89803921568628"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="12.1921568627451"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="10.5686274509804"/>
+    <col collapsed="false" hidden="false" max="16" min="15" style="0" width="30.5607843137255"/>
+    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="8.89803921568628"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.2" outlineLevel="0" r="1" s="15">
@@ -17763,13 +17764,13 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.4627450980392"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.68235294117647"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.8196078431373"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.2"/>
-    <col collapsed="false" hidden="false" max="7" min="5" style="0" width="10.1764705882353"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.6235294117647"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.57647058823529"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.5843137254902"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.76862745098039"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.921568627451"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.3647058823529"/>
+    <col collapsed="false" hidden="false" max="7" min="5" style="0" width="10.2627450980392"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.7254901960784"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.64705882352941"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="15.05" outlineLevel="0" r="1" s="5">
@@ -23254,14 +23255,14 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.4352941176471"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.9137254901961"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.5137254901961"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="10.2980392156863"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.8392156862745"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.5843137254902"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.3725490196078"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.57647058823529"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.6509803921569"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.6117647058824"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="10.3843137254902"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.9686274509804"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.7058823529412"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.4901960784314"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.64705882352941"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.2" outlineLevel="0" r="1" s="5">
@@ -23416,10 +23417,10 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.0196078431373"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.7176470588235"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.9411764705882"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.57647058823529"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.1490196078431"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.8313725490196"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.0705882352941"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.64705882352941"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="12.2" outlineLevel="0" r="1" s="5">
@@ -23593,12 +23594,12 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.9960784313725"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.4901960784314"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.3921568627451"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.0196078431373"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.6509803921569"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57647058823529"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.121568627451"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.5921568627451"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.4901960784314"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.1333333333333"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.8078431372549"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.64705882352941"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="12.2" outlineLevel="0" r="1" s="5">
@@ -23661,14 +23662,14 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.7058823529412"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.85098039215686"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.0862745098039"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.9372549019608"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.5176470588235"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="39" width="12.1098039215686"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="39" width="14.956862745098"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.72156862745098"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.8274509803922"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.93333333333333"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.2862745098039"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.1529411764706"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.6470588235294"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="39" width="12.2117647058824"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="39" width="15.078431372549"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.7921568627451"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="15.05" outlineLevel="0" r="1" s="5">
@@ -23831,14 +23832,14 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.478431372549"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.0705882352941"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.0862745098039"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.9372549019608"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.5176470588235"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="39" width="12.1098039215686"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="39" width="14.956862745098"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.72156862745098"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.721568627451"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.278431372549"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.2862745098039"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.1529411764706"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.6470588235294"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="39" width="12.2117647058824"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="39" width="15.078431372549"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.7921568627451"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="15.05" outlineLevel="0" r="1" s="5">
@@ -23933,11 +23934,11 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.8666666666667"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.7137254901961"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="10.4196078431373"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="11.4588235294118"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57647058823529"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.0235294117647"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.9137254901961"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="10.5058823529412"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="11.5529411764706"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.64705882352941"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="12.2" outlineLevel="0" r="1" s="5">
@@ -24081,18 +24082,18 @@
   </sheetPr>
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A2" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A2" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
       <selection activeCell="D25" activeCellId="0" pane="topLeft" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.5058823529412"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.2862745098039"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.57647058823529"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="8.64705882352941"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.57647058823529"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.9294117647059"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.57647058823529"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.6470588235294"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.5450980392157"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.64705882352941"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="8.72156862745098"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.64705882352941"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.0901960784314"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.64705882352941"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="12.2" outlineLevel="0" r="1" s="5">
@@ -24518,21 +24519,21 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.3490196078431"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.71372549019608"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.1254901960784"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.9294117647059"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.9333333333333"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="5.47058823529412"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.82745098039216"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.8941176470588"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.85098039215686"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="11.1921568627451"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="11.4588235294118"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="10.5254901960784"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="10.2627450980392"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="11.7450980392157"/>
-    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="9.58823529411765"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.5176470588235"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.7843137254902"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.2823529411765"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.0980392156863"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.1254901960784"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="5.51372549019608"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.89803921568628"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.0156862745098"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.93333333333333"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="11.278431372549"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="11.5529411764706"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="10.6117647058824"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="10.3490196078431"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="11.8470588235294"/>
+    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="9.66666666666667"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="18.85" outlineLevel="0" r="1" s="5">
@@ -24664,12 +24665,12 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.8901960784314"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.8039215686275"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.29411764705882"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.48235294117647"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.75686274509804"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.58823529411765"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.1921568627451"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.9176470588235"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.35294117647059"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.55294117647059"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.82745098039216"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.66666666666667"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="22.6" outlineLevel="0" r="1" s="5">
@@ -24773,11 +24774,11 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.2823529411765"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.1058823529412"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.121568627451"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.9450980392157"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57647058823529"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.3843137254902"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.2901960784314"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.2470588235294"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.0392156862745"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.64705882352941"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="12.2" outlineLevel="0" r="1" s="5">
@@ -24965,20 +24966,20 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.7019607843137"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.85490196078431"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.0705882352941"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.4274509803922"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.48235294117647"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.82745098039216"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.51372549019608"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.6549019607843"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.74901960784314"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.1921568627451"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.61176470588235"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="29.7647058823529"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="96.1686274509804"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="9.58823529411765"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.8588235294118"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.92941176470588"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.1843137254902"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.5882352941176"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.55294117647059"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.89803921568628"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.58039215686275"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.7411764705882"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.81960784313726"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.278431372549"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.68235294117647"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="30.0117647058823"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="96.964705882353"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="9.66666666666667"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="25.45" outlineLevel="0" r="1">
@@ -25116,12 +25117,11 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.3333333333333"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.89803921568628"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.68235294117647"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.4"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="3.34901960784314"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57647058823529"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.5607843137255"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.75686274509804"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.521568627451"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="3.37647058823529"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.64705882352941"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="12.2" outlineLevel="0" r="1" s="5">
@@ -25193,9 +25193,9 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.8823529411765"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="39.6274509803922"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57647058823529"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.0549019607843"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="39.956862745098"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.64705882352941"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="12.2" outlineLevel="0" r="1" s="5">
@@ -25275,20 +25275,20 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.921568627451"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.61176470588235"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.5254901960784"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.0392156862745"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.6039215686275"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.8666666666667"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.6549019607843"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.1607843137255"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="6.58823529411765"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.70980392156863"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="11.0627450980392"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="11.1921568627451"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="15.5686274509804"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="9.58823529411765"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.0156862745098"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.68235294117647"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.6313725490196"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.1411764705882"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.7019607843137"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.9686274509804"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.7411764705882"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.2627450980392"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="6.63921568627451"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.78823529411765"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="11.1490196078431"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="11.278431372549"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="15.6980392156863"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="9.66666666666667"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.4" outlineLevel="0" r="1">
@@ -25410,17 +25410,17 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.7450980392157"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.85098039215686"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.61176470588235"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.5843137254902"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.921568627451"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.88627450980392"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.2196078431373"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.2901960784314"/>
-    <col collapsed="false" hidden="false" max="11" min="9" style="0" width="9.58823529411765"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="11.8666666666667"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="9.58823529411765"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.8705882352941"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.93333333333333"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.68235294117647"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.7254901960784"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.0666666666667"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.96470588235294"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.3411764705882"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.3921568627451"/>
+    <col collapsed="false" hidden="false" max="11" min="9" style="0" width="9.66666666666667"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="11.9686274509804"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="9.66666666666667"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="17.9" outlineLevel="0" r="1">
@@ -25540,18 +25540,18 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.7019607843137"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.85490196078431"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.4274509803922"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="8.48235294117647"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="8.82745098039216"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="7.51372549019608"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.6549019607843"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.74901960784314"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="11.1921568627451"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.61176470588235"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="29.7647058823529"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="9.58823529411765"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.8588235294118"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.92941176470588"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.5882352941176"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="8.55294117647059"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="8.89803921568628"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="7.58039215686275"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.7411764705882"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.81960784313726"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="11.278431372549"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.68235294117647"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="30.0117647058823"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="9.66666666666667"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="21.65" outlineLevel="0" r="1">
@@ -25759,12 +25759,11 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.3333333333333"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.89803921568628"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.68235294117647"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.4"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="3.34901960784314"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57647058823529"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.5607843137255"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.75686274509804"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.521568627451"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="3.37647058823529"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.64705882352941"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="26.4" outlineLevel="0" r="1" s="5">
@@ -25836,10 +25835,10 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.7098039215686"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.9882352941176"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.1372549019608"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.57647058823529"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.8509803921569"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.1607843137255"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.2666666666667"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.64705882352941"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="12.2" outlineLevel="0" r="1" s="5">
@@ -25913,9 +25912,9 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.2352941176471"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.5254901960784"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57647058823529"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.3843137254902"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.6705882352941"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.64705882352941"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="12.2" outlineLevel="0" r="1" s="5">
@@ -25992,12 +25991,12 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.0039215686274"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.8705882352941"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.9921568627451"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="10.8196078431373"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.2980392156863"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57647058823529"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.1921568627451"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.078431372549"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="10.9058823529412"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.3843137254902"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.64705882352941"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.2" outlineLevel="0" r="1" s="5">
@@ -26388,13 +26387,13 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.3333333333333"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.1960784313725"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="39" width="8.25490196078431"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="39" width="11.9882352941176"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="39" width="6.03137254901961"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="39" width="8.13333333333333"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.61176470588235"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.4352941176471"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.3921568627451"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="39" width="8.32549019607843"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="39" width="12.0901960784314"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="39" width="6.08627450980392"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="39" width="8.20392156862745"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.68235294117647"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="12.2" outlineLevel="0" r="1" s="5">
@@ -26550,12 +26549,12 @@
   </sheetViews>
   <cols>
     <col collapsed="false" hidden="true" max="1" min="1" style="0" width="0"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.3490196078431"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.85490196078431"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.4823529411765"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.9529411764706"/>
-    <col collapsed="false" hidden="false" max="1023" min="6" style="0" width="8.57647058823529"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="5.14117647058824"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.5725490196078"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="6.91372549019608"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.6823529411765"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.1254901960784"/>
+    <col collapsed="false" hidden="false" max="1023" min="6" style="0" width="8.64705882352941"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="5.1843137254902"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="12.2" outlineLevel="0" r="1" s="5">
@@ -27006,15 +27005,15 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.2980392156863"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.9843137254902"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="10.2980392156863"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="7.25098039215686"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.72156862745098"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="8.74901960784314"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="6.85490196078431"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="10.2980392156863"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.41176470588235"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.3843137254902"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.05490196078431"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="10.3843137254902"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="7.30588235294118"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.7921568627451"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="8.81960784313726"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="6.91372549019608"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="10.3843137254902"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.48235294117647"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="44.75" outlineLevel="0" r="1" s="77">
@@ -28276,13 +28275,13 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.82745098039216"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.16862745098039"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.4549019607843"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="6.86274509803922"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.6627450980392"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.0039215686275"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="40" width="9.42352941176471"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.89803921568628"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.23921568627451"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.556862745098"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="6.92156862745098"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.7647058823529"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.1450980392157"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="40" width="9.50196078431373"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="13.4" outlineLevel="0" r="1">
@@ -28447,33 +28446,33 @@
   <dimension ref="1:8"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
-      <selection activeCell="H9" activeCellId="0" pane="topLeft" sqref="H9"/>
+      <selection activeCell="A2" activeCellId="0" pane="topLeft" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.2627450980392"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.72156862745098"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="8.27450980392157"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.8627450980392"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="12.5843137254902"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.3098039215686"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.8470588235294"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.22352941176471"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.0588235294118"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.81176470588235"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="11.8470588235294"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="10.6039215686275"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="8.54117647058824"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="8.81176470588235"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="7.58039215686275"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="10.6039215686275"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="10.7411764705882"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="8.74901960784314"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="8.94901960784314"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="7.70196078431373"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="10.7411764705882"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="11.4078431372549"/>
-    <col collapsed="false" hidden="false" max="1025" min="25" style="0" width="7.70196078431373"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.3921568627451"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.7921568627451"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="12.1098039215686"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.0078431372549"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="12.6862745098039"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.478431372549"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.9450980392157"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.30196078431373"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.1411764705882"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.88627450980392"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="11.9450980392157"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="10.6901960784314"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="8.61176470588235"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="8.88627450980392"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="7.63529411764706"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="10.6901960784314"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="10.8274509803922"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="8.81960784313726"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="9.01960784313726"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="7.76078431372549"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="10.8274509803922"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="11.5019607843137"/>
+    <col collapsed="false" hidden="false" max="1025" min="25" style="0" width="7.76078431372549"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="12.2" outlineLevel="0" r="1" s="41">
@@ -28581,7 +28580,7 @@
       <c r="X2" s="48"/>
       <c r="AMJ2" s="49"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.2" outlineLevel="0" r="3" s="50">
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="38.75" outlineLevel="0" r="3" s="50">
       <c r="A3" s="50" t="s">
         <v>42</v>
       </c>
@@ -28706,7 +28705,7 @@
         <v>277</v>
       </c>
       <c r="C5" s="56" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5" s="56" t="n">
         <v>1</v>
@@ -28748,10 +28747,10 @@
         <v>283</v>
       </c>
       <c r="C6" s="56" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6" s="56" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6" s="55" t="s">
         <v>284</v>
@@ -28907,20 +28906,20 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3647058823529"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.01960784313726"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.87843137254902"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.76862745098039"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="10.4392156862745"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.7019607843137"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.678431372549"/>
-    <col collapsed="false" hidden="false" max="12" min="9" style="0" width="8.68235294117647"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="16.8588235294118"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="12.5843137254902"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="22.8392156862745"/>
-    <col collapsed="false" hidden="false" max="26" min="16" style="0" width="7.72941176470588"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="9.15686274509804"/>
-    <col collapsed="false" hidden="false" max="1025" min="28" style="0" width="8.57647058823529"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.4588235294118"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.07843137254902"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.94901960784314"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.85098039215686"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="10.5254901960784"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.7960784313726"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.7725490196078"/>
+    <col collapsed="false" hidden="false" max="12" min="9" style="0" width="8.75686274509804"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="17.0039215686275"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="12.6862745098039"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="23.0313725490196"/>
+    <col collapsed="false" hidden="false" max="26" min="16" style="0" width="7.79607843137255"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="9.22745098039216"/>
+    <col collapsed="false" hidden="false" max="1025" min="28" style="0" width="8.64705882352941"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="12.2" outlineLevel="0" r="1" s="15">

</xml_diff>

<commit_message>
Added DefaultCountry and ScheduleSamplingEnabled in Setup tab
</commit_message>
<xml_diff>
--- a/bika/lims/setupdata/test/test.xlsx
+++ b/bika/lims/setupdata/test/test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="943" firstSheet="0" activeTab="34"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="415" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" state="visible" r:id="rId2"/>
@@ -99,13 +99,13 @@
             <anchor moveWithCells="false" sizeWithCells="false">
               <xdr:from>
                 <xdr:col>7</xdr:col>
-                <xdr:colOff>47</xdr:colOff>
+                <xdr:colOff>54</xdr:colOff>
                 <xdr:row>1</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </xdr:from>
               <xdr:to>
                 <xdr:col>13</xdr:col>
-                <xdr:colOff>43</xdr:colOff>
+                <xdr:colOff>49</xdr:colOff>
                 <xdr:row>2</xdr:row>
                 <xdr:rowOff>5</xdr:rowOff>
               </xdr:to>
@@ -236,13 +236,13 @@
             <anchor moveWithCells="false" sizeWithCells="false">
               <xdr:from>
                 <xdr:col>7</xdr:col>
-                <xdr:colOff>34</xdr:colOff>
+                <xdr:colOff>39</xdr:colOff>
                 <xdr:row>14</xdr:row>
-                <xdr:rowOff>5</xdr:rowOff>
+                <xdr:rowOff>4</xdr:rowOff>
               </xdr:from>
               <xdr:to>
                 <xdr:col>9</xdr:col>
-                <xdr:colOff>34</xdr:colOff>
+                <xdr:colOff>39</xdr:colOff>
                 <xdr:row>25</xdr:row>
                 <xdr:rowOff>12</xdr:rowOff>
               </xdr:to>
@@ -271,13 +271,13 @@
             <anchor moveWithCells="false" sizeWithCells="false">
               <xdr:from>
                 <xdr:col>17</xdr:col>
-                <xdr:colOff>34</xdr:colOff>
+                <xdr:colOff>39</xdr:colOff>
                 <xdr:row>6</xdr:row>
                 <xdr:rowOff>9</xdr:rowOff>
               </xdr:from>
               <xdr:to>
                 <xdr:col>24</xdr:col>
-                <xdr:colOff>34</xdr:colOff>
+                <xdr:colOff>39</xdr:colOff>
                 <xdr:row>12</xdr:row>
                 <xdr:rowOff>6</xdr:rowOff>
               </xdr:to>
@@ -292,7 +292,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3912" uniqueCount="1578">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3917" uniqueCount="1583">
   <si>
     <t>Instructions</t>
   </si>
@@ -4224,6 +4224,12 @@
     <t>Sampling workflow enabled?</t>
   </si>
   <si>
+    <t>ScheduleSamplingEnabled</t>
+  </si>
+  <si>
+    <t>Schedule Sampling workflow enabled</t>
+  </si>
+  <si>
     <t>CategoriseAnalysisServices</t>
   </si>
   <si>
@@ -4324,6 +4330,15 @@
   </si>
   <si>
     <t>Id server url</t>
+  </si>
+  <si>
+    <t>DefaultCountry</t>
+  </si>
+  <si>
+    <t>Default Country</t>
+  </si>
+  <si>
+    <t>ZA</t>
   </si>
   <si>
     <t>AR Import options</t>
@@ -5340,7 +5355,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="177">
+  <cellXfs count="178">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -6017,6 +6032,10 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -6128,8 +6147,8 @@
   </sheetPr>
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -13600,7 +13619,7 @@
   </sheetPr>
   <dimension ref="A1:AE28"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="L33" activeCellId="0" sqref="L33"/>
     </sheetView>
   </sheetViews>
@@ -27790,10 +27809,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B30" activeCellId="0" sqref="B30"/>
+      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -27973,41 +27992,40 @@
         <v>1311</v>
       </c>
       <c r="C16" s="164" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="24.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="s">
         <v>1312</v>
       </c>
       <c r="B17" s="142" t="s">
         <v>1313</v>
       </c>
-      <c r="C17" s="165" t="s">
-        <v>935</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C17" s="164" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="24.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="5" t="s">
         <v>1314</v>
       </c>
       <c r="B18" s="142" t="s">
         <v>1315</v>
       </c>
-      <c r="C18" s="166" t="s">
-        <v>1316</v>
-      </c>
-      <c r="D18" s="167"/>
+      <c r="C18" s="165" t="s">
+        <v>935</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="5" t="s">
+        <v>1316</v>
+      </c>
+      <c r="B19" s="142" t="s">
         <v>1317</v>
       </c>
-      <c r="B19" s="142" t="s">
+      <c r="C19" s="166" t="s">
         <v>1318</v>
-      </c>
-      <c r="C19" s="165" t="s">
-        <v>322</v>
       </c>
       <c r="D19" s="167"/>
     </row>
@@ -28021,6 +28039,7 @@
       <c r="C20" s="165" t="s">
         <v>322</v>
       </c>
+      <c r="D20" s="167"/>
     </row>
     <row r="21" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="5" t="s">
@@ -28029,8 +28048,8 @@
       <c r="B21" s="142" t="s">
         <v>1322</v>
       </c>
-      <c r="C21" s="166" t="n">
-        <v>30</v>
+      <c r="C21" s="165" t="s">
+        <v>322</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -28041,7 +28060,7 @@
         <v>1324</v>
       </c>
       <c r="C22" s="166" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -28062,53 +28081,53 @@
       <c r="B24" s="142" t="s">
         <v>1328</v>
       </c>
-      <c r="C24" s="165" t="s">
-        <v>1329</v>
-      </c>
-      <c r="D24" s="168"/>
+      <c r="C24" s="166" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="5" t="s">
+        <v>1329</v>
+      </c>
+      <c r="B25" s="142" t="s">
         <v>1330</v>
       </c>
-      <c r="B25" s="142" t="s">
+      <c r="C25" s="165" t="s">
         <v>1331</v>
       </c>
-      <c r="C25" s="165" t="s">
+      <c r="D25" s="168"/>
+    </row>
+    <row r="26" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="5" t="s">
         <v>1332</v>
       </c>
-    </row>
-    <row r="26" customFormat="false" ht="24.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="5" t="s">
+      <c r="B26" s="142" t="s">
         <v>1333</v>
       </c>
-      <c r="B26" s="142" t="s">
+      <c r="C26" s="165" t="s">
         <v>1334</v>
       </c>
-      <c r="C26" s="164" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="27" customFormat="false" ht="24.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="5" t="s">
         <v>1335</v>
       </c>
       <c r="B27" s="142" t="s">
         <v>1336</v>
       </c>
-      <c r="C27" s="163" t="s">
-        <v>1337</v>
+      <c r="C27" s="164" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="5" t="s">
+        <v>1337</v>
+      </c>
+      <c r="B28" s="142" t="s">
         <v>1338</v>
       </c>
-      <c r="B28" s="142" t="s">
+      <c r="C28" s="163" t="s">
         <v>1339</v>
-      </c>
-      <c r="C28" s="163" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -28118,8 +28137,8 @@
       <c r="B29" s="142" t="s">
         <v>1341</v>
       </c>
-      <c r="C29" s="164" t="n">
-        <v>0</v>
+      <c r="C29" s="163" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -28129,23 +28148,45 @@
       <c r="B30" s="142" t="s">
         <v>1343</v>
       </c>
-      <c r="C30" s="163"/>
+      <c r="C30" s="164" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A31" s="5" t="s">
+        <v>1344</v>
+      </c>
+      <c r="B31" s="142" t="s">
+        <v>1345</v>
+      </c>
+      <c r="C31" s="163"/>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="5" t="s">
+        <v>1346</v>
+      </c>
+      <c r="B32" s="142" t="s">
+        <v>1347</v>
+      </c>
+      <c r="C32" s="169" t="s">
+        <v>1348</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="24">
-    <dataValidation allowBlank="true" error="Please enter a whole number bigger than 0" errorTitle="Invalid entry" operator="greaterThan" prompt="Please enter a whole number bigger than 0" promptTitle="Integer" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C21" type="whole">
+    <dataValidation allowBlank="true" error="Please enter a whole number bigger than 0" errorTitle="Invalid entry" operator="greaterThan" prompt="Please enter a whole number bigger than 0" promptTitle="Integer" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C22" type="whole">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" error="Select 0 or 1  from the drop-down menu" errorTitle="Invalid entry" operator="equal" prompt="Select 1 (True) or 0 (False) from the drop-down menu" promptTitle="Boolean" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C7:C8 C15:C16 C26 C29" type="list">
+    <dataValidation allowBlank="false" error="Select 0 or 1  from the drop-down menu" errorTitle="Invalid entry" operator="equal" prompt="Select 1 (True) or 0 (False) from the drop-down menu" promptTitle="Boolean" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C7:C8 C15:C17 C27 C30" type="list">
       <formula1>Constants!$G$2:$G$3</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" error="Please enter a whole number between 0 and 23" errorTitle="Invalid data" operator="between" prompt="Please enter a whole number between 0 and 23" promptTitle="Valid entries" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C22" type="whole">
+    <dataValidation allowBlank="true" error="Please enter a whole number between 0 and 23" errorTitle="Invalid data" operator="between" prompt="Please enter a whole number between 0 and 23" promptTitle="Valid entries" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C23" type="whole">
       <formula1>0</formula1>
       <formula2>23</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" error="Please enter a whole number between 0 and 59" errorTitle="Invalid data" operator="between" prompt="Please enter a whole number between 0 and 59" promptTitle="Valid entries" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C23" type="whole">
+    <dataValidation allowBlank="true" error="Please enter a whole number between 0 and 59" errorTitle="Invalid data" operator="between" prompt="Please enter a whole number between 0 and 59" promptTitle="Valid entries" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C24" type="whole">
       <formula1>0</formula1>
       <formula2>59</formula2>
     </dataValidation>
@@ -28185,47 +28226,47 @@
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" error="Please select a valid entry from the drop-down menu" errorTitle="Invalid entry" operator="equal" prompt="The analysis to be used for determining dry matter. Please select a valid entry from the drop-down menu" promptTitle="Dry Matter Analysis" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C17" type="list">
+    <dataValidation allowBlank="true" error="Please select a valid entry from the drop-down menu" errorTitle="Invalid entry" operator="equal" prompt="The analysis to be used for determining dry matter. Please select a valid entry from the drop-down menu" promptTitle="Dry Matter Analysis" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C18" type="list">
       <formula1>'Analysis Services'!$A$4:$A$141</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" error="Please selct a valid option from the drop-down menu" errorTitle="Invalid entry" operator="equal" prompt="The list is mainatined on the &quot;Constants&quot; sheet" promptTitle="Select an import format from the list" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C18" type="list">
+    <dataValidation allowBlank="false" error="Please selct a valid option from the drop-down menu" errorTitle="Invalid entry" operator="equal" prompt="The list is mainatined on the &quot;Constants&quot; sheet" promptTitle="Select an import format from the list" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C19" type="list">
       <formula1>Constants!$C$2:$C$4</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" error="Please select a valid entry from the drop-down menu" errorTitle="Invalid entry" operator="equal" prompt="The analysis to be used for determining moisture. Please select a valid entry from the drop-down menu" promptTitle="Analysis keyword" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D18" type="list">
+    <dataValidation allowBlank="false" error="Please select a valid entry from the drop-down menu" errorTitle="Invalid entry" operator="equal" prompt="The analysis to be used for determining moisture. Please select a valid entry from the drop-down menu" promptTitle="Analysis keyword" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D19" type="list">
       <formula1>'analysis services'</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" error="Please select a valid entry from the drop-down menu" errorTitle="Invalid entry" operator="equal" prompt="Please select a valid option from the list" promptTitle="File attachments Required, Permitted or Not?" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C19:C20" type="list">
+    <dataValidation allowBlank="false" error="Please select a valid entry from the drop-down menu" errorTitle="Invalid entry" operator="equal" prompt="Please select a valid option from the list" promptTitle="File attachments Required, Permitted or Not?" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C20:C21" type="list">
       <formula1>Constants!$D$2:$D$4</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" error="Please select a valid entry from the drop-down menu" errorTitle="Invalid entry" operator="equal" prompt="'Classic' indicates importing analysis requests per sample and analysis service selection. With 'Profiles', analysis profile keywords are used to select multiple analysis services together" promptTitle="AR Import options" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D19" type="list">
+    <dataValidation allowBlank="false" error="Please select a valid entry from the drop-down menu" errorTitle="Invalid entry" operator="equal" prompt="'Classic' indicates importing analysis requests per sample and analysis service selection. With 'Profiles', analysis profile keywords are used to select multiple analysis services together" promptTitle="AR Import options" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D20" type="list">
       <formula1>Constants!$B$2:$B$25</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" error="Please select a valid entry from the drop-down menu" errorTitle="Invalid entry" operator="equal" prompt="Select 'Register' if you want labels to be automatically printed when new ARs or sample records are created. Select 'Receive' to print labels when ARs or Samples are received. Select 'None' to disable automatic printing" promptTitle="Select a valid option" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C24" type="list">
+    <dataValidation allowBlank="false" error="Please select a valid entry from the drop-down menu" errorTitle="Invalid entry" operator="equal" prompt="Select 'Register' if you want labels to be automatically printed when new ARs or sample records are created. Select 'Receive' to print labels when ARs or Samples are received. Select 'None' to disable automatic printing" promptTitle="Select a valid option" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C25" type="list">
       <formula1>Constants!$F$2:$F$4</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" error="Not sure why, must be whole number greater than 0" errorTitle="Invalid entry" operator="greaterThan" prompt="The number of days before a sample expires and cannot be analysed any more. This setting can be overwritten per individual sample type  in the sample types setup" promptTitle="Default sample retention period" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D24" type="whole">
+    <dataValidation allowBlank="true" error="Not sure why, must be whole number greater than 0" errorTitle="Invalid entry" operator="greaterThan" prompt="The number of days before a sample expires and cannot be analysed any more. This setting can be overwritten per individual sample type  in the sample types setup" promptTitle="Default sample retention period" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D25" type="whole">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" error="Please select a valid entry from the drop-down menu" errorTitle="Invalid entry" operator="equal" prompt="Select the which label to print when automatic label printing is enabled" promptTitle="Sample label size" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C25" type="list">
+    <dataValidation allowBlank="false" error="Please select a valid entry from the drop-down menu" errorTitle="Invalid entry" operator="equal" prompt="Select the which label to print when automatic label printing is enabled" promptTitle="Sample label size" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C26" type="list">
       <formula1>Constants!$E$2:$E$3</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" error="Must be whole number greater than 0" errorTitle="Invalid entry" operator="greaterThan" prompt="The length of the zero-padding for Sample IDs. E.g, a water sample will be given an ID of W-0001 if the sample padding was set to 4, and water samples are prefixed with W" promptTitle="Sample ID Padding" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C27" type="whole">
+    <dataValidation allowBlank="false" error="Must be whole number greater than 0" errorTitle="Invalid entry" operator="greaterThan" prompt="The length of the zero-padding for Sample IDs. E.g, a water sample will be given an ID of W-0001 if the sample padding was set to 4, and water samples are prefixed with W" promptTitle="Sample ID Padding" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C28" type="whole">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" error="Must be whole number greater than 0" errorTitle="Invalid entry" operator="greaterThan" prompt="The length of the zero-padding for AR IDs. E.g, a the first AR on a water sample with ID of W-0001 will be given an ID of W-0001-01 if the AR padding was set to 2" promptTitle="Analysis request (AR) ID Padding" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C28" type="whole">
+    <dataValidation allowBlank="false" error="Must be whole number greater than 0" errorTitle="Invalid entry" operator="greaterThan" prompt="The length of the zero-padding for AR IDs. E.g, a the first AR on a water sample with ID of W-0001 will be given an ID of W-0001-01 if the AR padding was set to 2" promptTitle="Analysis request (AR) ID Padding" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C29" type="whole">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" error="Not sure why, must be whole number greater than 0" errorTitle="Invalid entry" operator="greaterThan" prompt="The full URL: http://URL/path:port" promptTitle="ID Server URL if an external ID server is used" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C30" type="whole">
+    <dataValidation allowBlank="true" error="Not sure why, must be whole number greater than 0" errorTitle="Invalid entry" operator="greaterThan" prompt="The full URL: http://URL/path:port" promptTitle="ID Server URL if an external ID server is used" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C31" type="whole">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -28268,35 +28309,35 @@
   </cols>
   <sheetData>
     <row r="1" s="77" customFormat="true" ht="44.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="169" t="s">
+      <c r="A1" s="170" t="s">
         <v>126</v>
       </c>
-      <c r="B1" s="169" t="s">
+      <c r="B1" s="170" t="s">
         <v>125</v>
       </c>
       <c r="C1" s="78" t="s">
-        <v>1344</v>
+        <v>1349</v>
       </c>
       <c r="D1" s="78" t="s">
-        <v>1345</v>
+        <v>1350</v>
       </c>
       <c r="E1" s="78" t="s">
-        <v>1346</v>
+        <v>1351</v>
       </c>
       <c r="F1" s="77" t="s">
-        <v>1347</v>
-      </c>
-      <c r="G1" s="170" t="s">
-        <v>1348</v>
+        <v>1352</v>
+      </c>
+      <c r="G1" s="171" t="s">
+        <v>1353</v>
       </c>
       <c r="H1" s="78" t="s">
-        <v>1349</v>
+        <v>1354</v>
       </c>
       <c r="I1" s="78" t="s">
-        <v>1350</v>
+        <v>1355</v>
       </c>
       <c r="J1" s="78" t="s">
-        <v>1351</v>
+        <v>1356</v>
       </c>
       <c r="K1" s="78" t="s">
         <v>987</v>
@@ -28311,28 +28352,28 @@
         <v>184</v>
       </c>
       <c r="C2" s="142" t="s">
-        <v>1316</v>
+        <v>1318</v>
       </c>
       <c r="D2" s="142" t="s">
-        <v>1352</v>
-      </c>
-      <c r="E2" s="171" t="s">
-        <v>1353</v>
+        <v>1357</v>
+      </c>
+      <c r="E2" s="172" t="s">
+        <v>1358</v>
       </c>
       <c r="F2" s="142" t="s">
-        <v>1354</v>
+        <v>1359</v>
       </c>
       <c r="G2" s="142" t="n">
         <v>0</v>
       </c>
       <c r="H2" s="142" t="s">
-        <v>1355</v>
+        <v>1360</v>
       </c>
       <c r="I2" s="142" t="s">
-        <v>1356</v>
+        <v>1361</v>
       </c>
       <c r="J2" s="142" t="s">
-        <v>1357</v>
+        <v>1362</v>
       </c>
       <c r="K2" s="142" t="s">
         <v>1009</v>
@@ -28340,34 +28381,34 @@
     </row>
     <row r="3" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="32" t="s">
-        <v>1358</v>
+        <v>1363</v>
       </c>
       <c r="B3" s="32" t="s">
         <v>173</v>
       </c>
       <c r="C3" s="142" t="s">
-        <v>1359</v>
+        <v>1364</v>
       </c>
       <c r="D3" s="142" t="s">
         <v>322</v>
       </c>
-      <c r="E3" s="171" t="s">
-        <v>1332</v>
+      <c r="E3" s="172" t="s">
+        <v>1334</v>
       </c>
       <c r="F3" s="142" t="s">
-        <v>1360</v>
+        <v>1365</v>
       </c>
       <c r="G3" s="142" t="n">
         <v>1</v>
       </c>
       <c r="H3" s="142" t="s">
-        <v>1361</v>
+        <v>1366</v>
       </c>
       <c r="I3" s="142" t="s">
         <v>24</v>
       </c>
       <c r="J3" s="142" t="s">
-        <v>1362</v>
+        <v>1367</v>
       </c>
       <c r="K3" s="142" t="s">
         <v>1017</v>
@@ -28375,21 +28416,21 @@
     </row>
     <row r="4" customFormat="false" ht="24.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="32" t="s">
-        <v>1363</v>
+        <v>1368</v>
       </c>
       <c r="B4" s="32" t="s">
         <v>154</v>
       </c>
       <c r="C4" s="142" t="s">
-        <v>1364</v>
+        <v>1369</v>
       </c>
       <c r="D4" s="142" t="s">
-        <v>1365</v>
+        <v>1370</v>
       </c>
       <c r="F4" s="142" t="s">
-        <v>1329</v>
-      </c>
-      <c r="G4" s="171"/>
+        <v>1331</v>
+      </c>
+      <c r="G4" s="172"/>
       <c r="H4" s="142" t="s">
         <v>320</v>
       </c>
@@ -28401,16 +28442,16 @@
       <c r="B5" s="142" t="s">
         <v>206</v>
       </c>
-      <c r="G5" s="171"/>
+      <c r="G5" s="172"/>
     </row>
     <row r="6" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="32" t="s">
-        <v>1366</v>
+        <v>1371</v>
       </c>
       <c r="B6" s="32" t="s">
-        <v>1367</v>
-      </c>
-      <c r="G6" s="171"/>
+        <v>1372</v>
+      </c>
+      <c r="G6" s="172"/>
     </row>
     <row r="7" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="142" t="s">
@@ -28419,99 +28460,99 @@
       <c r="B7" s="142" t="s">
         <v>201</v>
       </c>
-      <c r="G7" s="171"/>
+      <c r="G7" s="172"/>
     </row>
     <row r="8" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="32" t="s">
-        <v>1368</v>
+        <v>1373</v>
       </c>
       <c r="B8" s="32" t="s">
-        <v>1369</v>
-      </c>
-      <c r="G8" s="171"/>
+        <v>1374</v>
+      </c>
+      <c r="G8" s="172"/>
     </row>
     <row r="9" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G9" s="171"/>
+      <c r="G9" s="172"/>
     </row>
     <row r="10" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G10" s="171"/>
+      <c r="G10" s="172"/>
     </row>
     <row r="11" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G11" s="171"/>
+      <c r="G11" s="172"/>
     </row>
     <row r="12" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G12" s="171"/>
+      <c r="G12" s="172"/>
     </row>
     <row r="13" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G13" s="171"/>
+      <c r="G13" s="172"/>
     </row>
     <row r="14" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G14" s="171"/>
+      <c r="G14" s="172"/>
     </row>
     <row r="15" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G15" s="171"/>
+      <c r="G15" s="172"/>
     </row>
     <row r="16" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G16" s="171"/>
+      <c r="G16" s="172"/>
     </row>
     <row r="17" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G17" s="171"/>
+      <c r="G17" s="172"/>
     </row>
     <row r="18" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G18" s="171"/>
+      <c r="G18" s="172"/>
     </row>
     <row r="19" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G19" s="171"/>
+      <c r="G19" s="172"/>
     </row>
     <row r="20" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="172"/>
-      <c r="B20" s="172"/>
-      <c r="C20" s="172"/>
-      <c r="D20" s="172"/>
-      <c r="E20" s="173"/>
-      <c r="F20" s="172"/>
-      <c r="G20" s="173"/>
-      <c r="H20" s="172"/>
-      <c r="I20" s="172"/>
-      <c r="J20" s="172"/>
-      <c r="K20" s="172"/>
-      <c r="L20" s="172"/>
-    </row>
-    <row r="21" s="175" customFormat="true" ht="69.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="173"/>
+      <c r="B20" s="173"/>
+      <c r="C20" s="173"/>
+      <c r="D20" s="173"/>
+      <c r="E20" s="174"/>
+      <c r="F20" s="173"/>
+      <c r="G20" s="174"/>
+      <c r="H20" s="173"/>
+      <c r="I20" s="173"/>
+      <c r="J20" s="173"/>
+      <c r="K20" s="173"/>
+      <c r="L20" s="173"/>
+    </row>
+    <row r="21" s="176" customFormat="true" ht="69.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="77" t="s">
-        <v>1370</v>
+        <v>1375</v>
       </c>
       <c r="B21" s="78" t="s">
         <v>1291</v>
       </c>
       <c r="C21" s="77" t="s">
-        <v>1371</v>
+        <v>1376</v>
       </c>
       <c r="D21" s="77" t="s">
-        <v>1372</v>
-      </c>
-      <c r="E21" s="174" t="s">
-        <v>1373</v>
+        <v>1377</v>
+      </c>
+      <c r="E21" s="175" t="s">
+        <v>1378</v>
       </c>
       <c r="F21" s="77" t="s">
-        <v>1374</v>
+        <v>1379</v>
       </c>
       <c r="G21" s="77" t="s">
-        <v>1375</v>
+        <v>1380</v>
       </c>
       <c r="H21" s="77" t="s">
-        <v>1376</v>
+        <v>1381</v>
       </c>
       <c r="I21" s="77" t="s">
-        <v>1377</v>
+        <v>1382</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="176" t="s">
-        <v>1378</v>
+      <c r="A22" s="177" t="s">
+        <v>1383</v>
       </c>
       <c r="B22" s="142" t="s">
-        <v>1379</v>
+        <v>1384</v>
       </c>
       <c r="C22" s="142" t="s">
         <v>1154</v>
@@ -28519,11 +28560,11 @@
       <c r="D22" s="142" t="s">
         <v>1161</v>
       </c>
-      <c r="E22" s="171" t="s">
-        <v>1380</v>
+      <c r="E22" s="172" t="s">
+        <v>1385</v>
       </c>
       <c r="F22" s="142" t="s">
-        <v>1381</v>
+        <v>1386</v>
       </c>
       <c r="G22" s="142" t="s">
         <v>896</v>
@@ -28537,19 +28578,19 @@
     </row>
     <row r="23" customFormat="false" ht="24.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B23" s="142" t="s">
-        <v>1382</v>
+        <v>1387</v>
       </c>
       <c r="C23" s="142" t="s">
-        <v>1383</v>
+        <v>1388</v>
       </c>
       <c r="D23" s="142" t="s">
         <v>1284</v>
       </c>
-      <c r="E23" s="171" t="s">
-        <v>1384</v>
+      <c r="E23" s="172" t="s">
+        <v>1389</v>
       </c>
       <c r="F23" s="142" t="s">
-        <v>1385</v>
+        <v>1390</v>
       </c>
       <c r="G23" s="142" t="s">
         <v>903</v>
@@ -28558,21 +28599,21 @@
         <v>903</v>
       </c>
       <c r="I23" s="142" t="s">
-        <v>1386</v>
+        <v>1391</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="24.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B24" s="142" t="s">
-        <v>1387</v>
+        <v>1392</v>
       </c>
       <c r="C24" s="142" t="s">
-        <v>1388</v>
+        <v>1393</v>
       </c>
       <c r="D24" s="142" t="s">
         <v>1267</v>
       </c>
       <c r="F24" s="142" t="s">
-        <v>1389</v>
+        <v>1394</v>
       </c>
       <c r="G24" s="142" t="s">
         <v>900</v>
@@ -28581,911 +28622,911 @@
         <v>900</v>
       </c>
       <c r="I24" s="142" t="s">
-        <v>1390</v>
+        <v>1395</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B25" s="142" t="s">
-        <v>1391</v>
+        <v>1396</v>
       </c>
       <c r="C25" s="142" t="s">
-        <v>1392</v>
+        <v>1397</v>
       </c>
       <c r="D25" s="142" t="s">
         <v>1285</v>
       </c>
       <c r="H25" s="142" t="s">
-        <v>1393</v>
+        <v>1398</v>
       </c>
       <c r="I25" s="142" t="s">
-        <v>1394</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B26" s="142" t="s">
-        <v>1395</v>
+        <v>1400</v>
       </c>
       <c r="C26" s="142" t="s">
-        <v>1396</v>
+        <v>1401</v>
       </c>
       <c r="H26" s="142" t="s">
-        <v>1397</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B27" s="142" t="s">
-        <v>1398</v>
+        <v>1403</v>
       </c>
       <c r="C27" s="142" t="s">
-        <v>1399</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B28" s="142" t="s">
-        <v>1400</v>
+        <v>1405</v>
       </c>
       <c r="C28" s="142" t="s">
-        <v>1401</v>
+        <v>1406</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B29" s="142" t="s">
-        <v>1402</v>
+        <v>1407</v>
       </c>
       <c r="C29" s="142" t="s">
-        <v>1403</v>
+        <v>1408</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B30" s="142" t="s">
-        <v>1404</v>
+        <v>1409</v>
       </c>
       <c r="C30" s="142" t="s">
-        <v>1405</v>
+        <v>1410</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B31" s="142" t="s">
-        <v>1406</v>
+        <v>1411</v>
       </c>
       <c r="C31" s="142" t="s">
-        <v>1407</v>
+        <v>1412</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B32" s="142" t="s">
-        <v>1408</v>
+        <v>1413</v>
       </c>
       <c r="C32" s="142" t="s">
-        <v>1409</v>
+        <v>1414</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B33" s="142" t="s">
-        <v>1410</v>
+        <v>1415</v>
       </c>
       <c r="C33" s="142" t="s">
-        <v>1411</v>
+        <v>1416</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B34" s="142" t="s">
-        <v>1412</v>
+        <v>1417</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B35" s="142" t="s">
-        <v>1413</v>
+        <v>1418</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B36" s="142" t="s">
-        <v>1414</v>
+        <v>1419</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B37" s="142" t="s">
-        <v>1415</v>
+        <v>1420</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B38" s="142" t="s">
-        <v>1416</v>
+        <v>1421</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B39" s="142" t="s">
-        <v>1417</v>
+        <v>1422</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B40" s="142" t="s">
-        <v>1418</v>
+        <v>1423</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B41" s="142" t="s">
-        <v>1419</v>
+        <v>1424</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B42" s="142" t="s">
-        <v>1420</v>
+        <v>1425</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B43" s="142" t="s">
-        <v>1421</v>
+        <v>1426</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B44" s="142" t="s">
-        <v>1422</v>
+        <v>1427</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B45" s="142" t="s">
-        <v>1423</v>
+        <v>1428</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B46" s="142" t="s">
-        <v>1424</v>
+        <v>1429</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B47" s="142" t="s">
-        <v>1425</v>
+        <v>1430</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B48" s="142" t="s">
-        <v>1426</v>
+        <v>1431</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B49" s="142" t="s">
-        <v>1427</v>
+        <v>1432</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B50" s="142" t="s">
-        <v>1428</v>
+        <v>1433</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B51" s="142" t="s">
-        <v>1429</v>
+        <v>1434</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B52" s="142" t="s">
-        <v>1430</v>
+        <v>1435</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B53" s="142" t="s">
-        <v>1431</v>
+        <v>1436</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B54" s="142" t="s">
-        <v>1432</v>
+        <v>1437</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B55" s="142" t="s">
-        <v>1433</v>
+        <v>1438</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B56" s="142" t="s">
-        <v>1434</v>
+        <v>1439</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B57" s="142" t="s">
-        <v>1435</v>
+        <v>1440</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B58" s="142" t="s">
-        <v>1436</v>
+        <v>1441</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B59" s="142" t="s">
-        <v>1437</v>
+        <v>1442</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B60" s="142" t="s">
-        <v>1438</v>
+        <v>1443</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B61" s="142" t="s">
-        <v>1439</v>
+        <v>1444</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B62" s="142" t="s">
-        <v>1440</v>
+        <v>1445</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B63" s="142" t="s">
-        <v>1441</v>
+        <v>1446</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B64" s="142" t="s">
-        <v>1442</v>
+        <v>1447</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B65" s="142" t="s">
-        <v>1443</v>
+        <v>1448</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B66" s="142" t="s">
-        <v>1444</v>
+        <v>1449</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B67" s="142" t="s">
-        <v>1445</v>
+        <v>1450</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B68" s="142" t="s">
-        <v>1446</v>
+        <v>1451</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B69" s="142" t="s">
-        <v>1447</v>
+        <v>1452</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B70" s="142" t="s">
-        <v>1448</v>
+        <v>1453</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B71" s="142" t="s">
-        <v>1449</v>
+        <v>1454</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B72" s="142" t="s">
-        <v>1450</v>
+        <v>1455</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B73" s="142" t="s">
-        <v>1451</v>
+        <v>1456</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B74" s="142" t="s">
-        <v>1452</v>
+        <v>1457</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B75" s="142" t="s">
-        <v>1453</v>
+        <v>1458</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B76" s="142" t="s">
-        <v>1454</v>
+        <v>1459</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B77" s="142" t="s">
-        <v>1455</v>
+        <v>1460</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B78" s="142" t="s">
-        <v>1456</v>
+        <v>1461</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B79" s="142" t="s">
-        <v>1457</v>
+        <v>1462</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B80" s="142" t="s">
-        <v>1458</v>
+        <v>1463</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B81" s="142" t="s">
-        <v>1459</v>
+        <v>1464</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B82" s="142" t="s">
-        <v>1460</v>
+        <v>1465</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B83" s="142" t="s">
-        <v>1461</v>
+        <v>1466</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B84" s="142" t="s">
-        <v>1462</v>
+        <v>1467</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B85" s="142" t="s">
-        <v>1463</v>
+        <v>1468</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B86" s="142" t="s">
-        <v>1464</v>
+        <v>1469</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B87" s="142" t="s">
-        <v>1465</v>
+        <v>1470</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B88" s="142" t="s">
-        <v>1466</v>
+        <v>1471</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B89" s="142" t="s">
-        <v>1467</v>
+        <v>1472</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B90" s="142" t="s">
-        <v>1468</v>
+        <v>1473</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B91" s="142" t="s">
-        <v>1469</v>
+        <v>1474</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B92" s="142" t="s">
-        <v>1470</v>
+        <v>1475</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B93" s="142" t="s">
-        <v>1471</v>
+        <v>1476</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B94" s="142" t="s">
-        <v>1472</v>
+        <v>1477</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B95" s="142" t="s">
-        <v>1473</v>
+        <v>1478</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B96" s="142" t="s">
-        <v>1474</v>
+        <v>1479</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B97" s="142" t="s">
-        <v>1475</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B98" s="142" t="s">
-        <v>1476</v>
+        <v>1481</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B99" s="142" t="s">
-        <v>1477</v>
+        <v>1482</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B100" s="142" t="s">
-        <v>1478</v>
+        <v>1483</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B101" s="142" t="s">
-        <v>1479</v>
+        <v>1484</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B102" s="142" t="s">
-        <v>1480</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B103" s="142" t="s">
-        <v>1481</v>
+        <v>1486</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B104" s="142" t="s">
-        <v>1482</v>
+        <v>1487</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B105" s="142" t="s">
-        <v>1483</v>
+        <v>1488</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B106" s="142" t="s">
-        <v>1484</v>
+        <v>1489</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B107" s="142" t="s">
-        <v>1485</v>
+        <v>1490</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B108" s="142" t="s">
-        <v>1486</v>
+        <v>1491</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B109" s="142" t="s">
-        <v>1487</v>
+        <v>1492</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B110" s="142" t="s">
-        <v>1488</v>
+        <v>1493</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B111" s="142" t="s">
-        <v>1489</v>
+        <v>1494</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B112" s="142" t="s">
-        <v>1490</v>
+        <v>1495</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B113" s="142" t="s">
-        <v>1491</v>
+        <v>1496</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B114" s="142" t="s">
-        <v>1492</v>
+        <v>1497</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B115" s="142" t="s">
-        <v>1493</v>
+        <v>1498</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B116" s="142" t="s">
-        <v>1494</v>
+        <v>1499</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B117" s="142" t="s">
-        <v>1495</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B118" s="142" t="s">
-        <v>1496</v>
+        <v>1501</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B119" s="142" t="s">
-        <v>1497</v>
+        <v>1502</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B120" s="142" t="s">
-        <v>1498</v>
+        <v>1503</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B121" s="142" t="s">
-        <v>1499</v>
+        <v>1504</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B122" s="142" t="s">
-        <v>1500</v>
+        <v>1505</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B123" s="142" t="s">
-        <v>1501</v>
+        <v>1506</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B124" s="142" t="s">
-        <v>1502</v>
+        <v>1507</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B125" s="142" t="s">
-        <v>1503</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B126" s="142" t="s">
-        <v>1504</v>
+        <v>1509</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B127" s="142" t="s">
-        <v>1505</v>
+        <v>1510</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B128" s="142" t="s">
-        <v>1506</v>
+        <v>1511</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B129" s="142" t="s">
-        <v>1507</v>
+        <v>1512</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B130" s="142" t="s">
-        <v>1508</v>
+        <v>1513</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B131" s="142" t="s">
-        <v>1509</v>
+        <v>1514</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B132" s="142" t="s">
-        <v>1510</v>
+        <v>1515</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B133" s="142" t="s">
-        <v>1511</v>
+        <v>1516</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B134" s="142" t="s">
-        <v>1512</v>
+        <v>1517</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B135" s="142" t="s">
-        <v>1513</v>
+        <v>1518</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B136" s="142" t="s">
-        <v>1514</v>
+        <v>1519</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B137" s="142" t="s">
-        <v>1515</v>
+        <v>1520</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B138" s="142" t="s">
-        <v>1516</v>
+        <v>1521</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B139" s="142" t="s">
-        <v>1517</v>
+        <v>1522</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B140" s="142" t="s">
-        <v>1518</v>
+        <v>1523</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B141" s="142" t="s">
-        <v>1519</v>
+        <v>1524</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B142" s="142" t="s">
-        <v>1520</v>
+        <v>1525</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B143" s="142" t="s">
-        <v>1521</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B144" s="142" t="s">
-        <v>1522</v>
+        <v>1527</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B145" s="142" t="s">
-        <v>1523</v>
+        <v>1528</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B146" s="142" t="s">
-        <v>1524</v>
+        <v>1529</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B147" s="142" t="s">
-        <v>1525</v>
+        <v>1530</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B148" s="142" t="s">
-        <v>1526</v>
+        <v>1531</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B149" s="142" t="s">
-        <v>1527</v>
+        <v>1532</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B150" s="142" t="s">
-        <v>1528</v>
+        <v>1533</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B151" s="142" t="s">
-        <v>1529</v>
+        <v>1534</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B152" s="142" t="s">
-        <v>1530</v>
+        <v>1535</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B153" s="142" t="s">
-        <v>1531</v>
+        <v>1536</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B154" s="142" t="s">
-        <v>1532</v>
+        <v>1537</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B155" s="142" t="s">
-        <v>1533</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B156" s="142" t="s">
-        <v>1534</v>
+        <v>1539</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B157" s="142" t="s">
-        <v>1535</v>
+        <v>1540</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B158" s="142" t="s">
-        <v>1536</v>
+        <v>1541</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B159" s="142" t="s">
-        <v>1537</v>
+        <v>1542</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B160" s="142" t="s">
-        <v>1538</v>
+        <v>1543</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B161" s="142" t="s">
-        <v>1539</v>
+        <v>1544</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B162" s="142" t="s">
-        <v>1540</v>
+        <v>1545</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B163" s="142" t="s">
-        <v>1541</v>
+        <v>1546</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B164" s="142" t="s">
-        <v>1542</v>
+        <v>1547</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B165" s="142" t="s">
-        <v>1543</v>
+        <v>1548</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B166" s="142" t="s">
-        <v>1544</v>
+        <v>1549</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B167" s="142" t="s">
-        <v>1545</v>
+        <v>1550</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B168" s="142" t="s">
-        <v>1546</v>
+        <v>1551</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B169" s="142" t="s">
-        <v>1547</v>
+        <v>1552</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B170" s="142" t="s">
-        <v>1548</v>
+        <v>1553</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B171" s="142" t="s">
-        <v>1549</v>
+        <v>1554</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B172" s="142" t="s">
-        <v>1550</v>
+        <v>1555</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B173" s="142" t="s">
-        <v>1551</v>
+        <v>1556</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B174" s="142" t="s">
-        <v>1552</v>
+        <v>1557</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B175" s="142" t="s">
-        <v>1553</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B176" s="142" t="s">
-        <v>1554</v>
+        <v>1559</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B177" s="142" t="s">
-        <v>1555</v>
+        <v>1560</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B178" s="142" t="s">
-        <v>1556</v>
+        <v>1561</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B179" s="142" t="s">
-        <v>1557</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B180" s="142" t="s">
-        <v>1558</v>
+        <v>1563</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B181" s="142" t="s">
-        <v>1559</v>
+        <v>1564</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B182" s="142" t="s">
-        <v>1560</v>
+        <v>1565</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B183" s="142" t="s">
-        <v>1561</v>
+        <v>1566</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B184" s="142" t="s">
-        <v>1562</v>
+        <v>1567</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B185" s="142" t="s">
-        <v>1563</v>
+        <v>1568</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B186" s="142" t="s">
-        <v>1564</v>
+        <v>1569</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B187" s="142" t="s">
-        <v>1565</v>
+        <v>1570</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B188" s="142" t="s">
-        <v>1566</v>
+        <v>1571</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B189" s="142" t="s">
-        <v>1567</v>
+        <v>1572</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B190" s="142" t="s">
-        <v>1568</v>
+        <v>1573</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B191" s="142" t="s">
-        <v>1569</v>
+        <v>1574</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B192" s="142" t="s">
-        <v>1570</v>
+        <v>1575</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B193" s="142" t="s">
-        <v>1571</v>
+        <v>1576</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B194" s="142" t="s">
-        <v>1572</v>
+        <v>1577</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B195" s="142" t="s">
-        <v>1573</v>
+        <v>1578</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B196" s="142" t="s">
-        <v>1574</v>
+        <v>1579</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B197" s="142" t="s">
-        <v>1575</v>
+        <v>1580</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -29495,12 +29536,12 @@
     </row>
     <row r="199" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B199" s="142" t="s">
-        <v>1576</v>
+        <v>1581</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B200" s="142" t="s">
-        <v>1577</v>
+        <v>1582</v>
       </c>
     </row>
   </sheetData>

</xml_diff>